<commit_message>
Updated Balaji Payment info
</commit_message>
<xml_diff>
--- a/ATT_Bill.xlsx
+++ b/ATT_Bill.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>ATT Family Plan Bill Details</t>
   </si>
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,11 +910,12 @@
         <v>175.34</v>
       </c>
       <c r="N8" s="11">
-        <v>113.35</v>
-      </c>
-      <c r="O8" s="16">
+        <f>113.35+61.99</f>
+        <v>175.34</v>
+      </c>
+      <c r="O8" s="15">
         <f t="shared" si="0"/>
-        <v>61.990000000000009</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="1"/>
     </row>
@@ -955,10 +956,12 @@
         <f>SUM(I3:I15)</f>
         <v>51.99</v>
       </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="16">
+      <c r="N9" s="11">
+        <v>51.99</v>
+      </c>
+      <c r="O9" s="15">
         <f t="shared" si="0"/>
-        <v>51.99</v>
+        <v>0</v>
       </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
@@ -1403,12 +1406,22 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="L24" s="3"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="17"/>
+      <c r="L24" s="3">
+        <v>8</v>
+      </c>
+      <c r="M24" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="N24" s="17">
+        <v>42364</v>
+      </c>
       <c r="O24" s="17"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="3"/>
+      <c r="P24" s="13">
+        <v>113.98</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L25" s="3"/>

</xml_diff>

<commit_message>
Feb 2016 Bill updated
</commit_message>
<xml_diff>
--- a/ATT_Bill.xlsx
+++ b/ATT_Bill.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="6120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="6120" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2015" sheetId="1" r:id="rId1"/>
+    <sheet name="2016" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="33">
   <si>
     <t>ATT Family Plan Bill Details</t>
   </si>
@@ -120,7 +121,14 @@
     <t>Sankari</t>
   </si>
   <si>
-    <t>ATT discount claimed for incorrect billing.</t>
+    <t>Previous Balance</t>
+  </si>
+  <si>
+    <t>Balaji Contract - $25 extra
+Giri India Calling - $15 extra</t>
+  </si>
+  <si>
+    <t>ATT discount claimed for incorrect billing in 2015.</t>
   </si>
 </sst>
 </file>
@@ -133,7 +141,7 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +181,20 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -200,7 +222,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -297,12 +319,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -354,24 +396,33 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -384,9 +435,6 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -394,6 +442,60 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -679,9 +781,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,19 +803,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -783,16 +885,16 @@
       <c r="F3" s="11">
         <v>53.44</v>
       </c>
-      <c r="G3" s="25">
-        <v>0</v>
-      </c>
-      <c r="H3" s="25">
-        <v>0</v>
-      </c>
-      <c r="I3" s="25">
-        <v>0</v>
-      </c>
-      <c r="J3" s="25">
+      <c r="G3" s="28">
+        <v>0</v>
+      </c>
+      <c r="H3" s="28">
+        <v>0</v>
+      </c>
+      <c r="I3" s="28">
+        <v>0</v>
+      </c>
+      <c r="J3" s="28">
         <v>0</v>
       </c>
       <c r="K3" s="2"/>
@@ -830,10 +932,10 @@
       <c r="F4" s="11">
         <v>38.54</v>
       </c>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
       <c r="K4" s="2"/>
       <c r="L4" s="1"/>
       <c r="M4" s="2" t="s">
@@ -841,15 +943,15 @@
       </c>
       <c r="N4" s="11">
         <f>SUM(C3:C15)</f>
-        <v>490.43999999999994</v>
-      </c>
-      <c r="O4" s="25">
+        <v>482.77999999999992</v>
+      </c>
+      <c r="O4" s="28">
         <f>200+490.45</f>
         <v>690.45</v>
       </c>
-      <c r="P4" s="27">
+      <c r="P4" s="30">
         <f>N4+N5-O4</f>
-        <v>-192.35000000000008</v>
+        <v>-207.67000000000013</v>
       </c>
       <c r="R4" s="1"/>
     </row>
@@ -872,10 +974,10 @@
       <c r="F5" s="11">
         <v>38.229999999999997</v>
       </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
       <c r="K5" s="2"/>
       <c r="L5" s="1"/>
       <c r="M5" s="2" t="s">
@@ -883,10 +985,10 @@
       </c>
       <c r="N5" s="11">
         <f>SUM(J3:J15)</f>
-        <v>7.66</v>
-      </c>
-      <c r="O5" s="26"/>
-      <c r="P5" s="28"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="29"/>
+      <c r="P5" s="31"/>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -908,10 +1010,10 @@
       <c r="F6" s="11">
         <v>38.54</v>
       </c>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
       <c r="K6" s="2"/>
       <c r="L6" s="1"/>
       <c r="M6" s="2" t="s">
@@ -919,15 +1021,15 @@
       </c>
       <c r="N6" s="11">
         <f>SUM(D3:D15)</f>
-        <v>486.91999999999996</v>
+        <v>479.25999999999993</v>
       </c>
       <c r="O6" s="11">
         <f>368+80</f>
         <v>448</v>
       </c>
-      <c r="P6" s="29">
-        <f t="shared" ref="P4:P11" si="0">N6-O6</f>
-        <v>38.919999999999959</v>
+      <c r="P6" s="19">
+        <f t="shared" ref="P6:P11" si="0">N6-O6</f>
+        <v>31.259999999999934</v>
       </c>
       <c r="R6" s="1"/>
     </row>
@@ -950,10 +1052,10 @@
       <c r="F7" s="11">
         <v>38.69</v>
       </c>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
       <c r="K7" s="2"/>
       <c r="L7" s="1"/>
       <c r="M7" s="2" t="s">
@@ -961,12 +1063,12 @@
       </c>
       <c r="N7" s="11">
         <f>SUM(F3:F15)</f>
-        <v>498.79999999999995</v>
-      </c>
-      <c r="O7" s="25">
-        <v>1031.94</v>
-      </c>
-      <c r="P7" s="27">
+        <v>491.13999999999993</v>
+      </c>
+      <c r="O7" s="28">
+        <v>1024.28</v>
+      </c>
+      <c r="P7" s="30">
         <f>N7+N8-O7</f>
         <v>0</v>
       </c>
@@ -991,10 +1093,10 @@
       <c r="F8" s="11">
         <v>39.799999999999997</v>
       </c>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
       <c r="K8" s="2"/>
       <c r="L8" s="1"/>
       <c r="M8" s="2" t="s">
@@ -1004,8 +1106,8 @@
         <f>SUM(E3:E14)</f>
         <v>533.14</v>
       </c>
-      <c r="O8" s="26"/>
-      <c r="P8" s="28"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="31"/>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1027,10 +1129,10 @@
       <c r="F9" s="11">
         <v>38.69</v>
       </c>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
       <c r="K9" s="2"/>
       <c r="L9" s="1"/>
       <c r="M9" s="2" t="s">
@@ -1038,15 +1140,15 @@
       </c>
       <c r="N9" s="11">
         <f>SUM(G3:G15)</f>
-        <v>183</v>
-      </c>
-      <c r="O9" s="25">
+        <v>175.34</v>
+      </c>
+      <c r="O9" s="28">
         <f>113.35+61.99+51.99</f>
         <v>227.33</v>
       </c>
-      <c r="P9" s="30">
+      <c r="P9" s="32">
         <f>N9+N10-O9</f>
-        <v>15.319999999999993</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -1070,10 +1172,10 @@
       <c r="F10" s="11">
         <v>39.14</v>
       </c>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
       <c r="K10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1083,10 +1185,10 @@
       </c>
       <c r="N10" s="11">
         <f>SUM(I3:I15)</f>
-        <v>59.650000000000006</v>
-      </c>
-      <c r="O10" s="26"/>
-      <c r="P10" s="31"/>
+        <v>51.99</v>
+      </c>
+      <c r="O10" s="29"/>
+      <c r="P10" s="33"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
@@ -1109,10 +1211,10 @@
       <c r="F11" s="11">
         <v>38.92</v>
       </c>
-      <c r="G11" s="26"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
       <c r="K11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1127,7 +1229,7 @@
       <c r="O11" s="11">
         <v>0</v>
       </c>
-      <c r="P11" s="29">
+      <c r="P11" s="19">
         <f t="shared" si="0"/>
         <v>106.63</v>
       </c>
@@ -1156,9 +1258,9 @@
       <c r="G12" s="11">
         <v>52.78</v>
       </c>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
       <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1192,9 +1294,9 @@
       <c r="G13" s="11">
         <v>60.57</v>
       </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="32"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="34"/>
       <c r="K13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1240,7 +1342,7 @@
         <f>36.99+15</f>
         <v>51.99</v>
       </c>
-      <c r="J14" s="26"/>
+      <c r="J14" s="29"/>
       <c r="K14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1257,50 +1359,48 @@
         <v>42353</v>
       </c>
       <c r="B15" s="4">
-        <v>45.96</v>
+        <v>0</v>
       </c>
       <c r="C15" s="4">
         <f>B15/6</f>
-        <v>7.66</v>
+        <v>0</v>
       </c>
       <c r="D15" s="4">
         <f>B15/6</f>
-        <v>7.66</v>
+        <v>0</v>
       </c>
       <c r="E15" s="4">
         <v>0</v>
       </c>
       <c r="F15" s="4">
         <f>B15/6</f>
-        <v>7.66</v>
+        <v>0</v>
       </c>
       <c r="G15" s="4">
         <f>B15/6</f>
-        <v>7.66</v>
+        <v>0</v>
       </c>
       <c r="H15" s="4">
         <v>0</v>
       </c>
       <c r="I15" s="4">
         <f>B15/6</f>
-        <v>7.66</v>
+        <v>0</v>
       </c>
       <c r="J15" s="4">
         <f>B15/6</f>
-        <v>7.66</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K15" s="2"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="22" t="s">
+      <c r="M15" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="24"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="26"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -1321,10 +1421,10 @@
       <c r="N16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O16" s="21" t="s">
+      <c r="O16" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="P16" s="21"/>
+      <c r="P16" s="27"/>
       <c r="Q16" s="10" t="s">
         <v>23</v>
       </c>
@@ -1351,10 +1451,10 @@
       <c r="N17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O17" s="19">
+      <c r="O17" s="22">
         <v>42053</v>
       </c>
-      <c r="P17" s="19"/>
+      <c r="P17" s="22"/>
       <c r="Q17" s="13">
         <v>108</v>
       </c>
@@ -1380,10 +1480,10 @@
       <c r="N18" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O18" s="19">
+      <c r="O18" s="22">
         <v>42086</v>
       </c>
-      <c r="P18" s="19"/>
+      <c r="P18" s="22"/>
       <c r="Q18" s="13">
         <v>200</v>
       </c>
@@ -1409,10 +1509,10 @@
       <c r="N19" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O19" s="19">
+      <c r="O19" s="22">
         <v>42111</v>
       </c>
-      <c r="P19" s="19"/>
+      <c r="P19" s="22"/>
       <c r="Q19" s="13">
         <v>100</v>
       </c>
@@ -1437,10 +1537,10 @@
       <c r="N20" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O20" s="19">
+      <c r="O20" s="22">
         <v>42214</v>
       </c>
-      <c r="P20" s="19"/>
+      <c r="P20" s="22"/>
       <c r="Q20" s="13">
         <v>160</v>
       </c>
@@ -1459,10 +1559,10 @@
       <c r="N21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O21" s="19">
+      <c r="O21" s="22">
         <v>42325</v>
       </c>
-      <c r="P21" s="19"/>
+      <c r="P21" s="22"/>
       <c r="Q21" s="13">
         <v>113.35</v>
       </c>
@@ -1481,10 +1581,10 @@
       <c r="N22" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O22" s="19">
+      <c r="O22" s="22">
         <v>42325</v>
       </c>
-      <c r="P22" s="19"/>
+      <c r="P22" s="22"/>
       <c r="Q22" s="13">
         <v>80</v>
       </c>
@@ -1502,10 +1602,10 @@
       <c r="N23" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O23" s="19">
+      <c r="O23" s="22">
         <v>42341</v>
       </c>
-      <c r="P23" s="19"/>
+      <c r="P23" s="22"/>
       <c r="Q23" s="13">
         <v>490.45</v>
       </c>
@@ -1521,10 +1621,10 @@
       <c r="N24" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O24" s="19">
+      <c r="O24" s="22">
         <v>42364</v>
       </c>
-      <c r="P24" s="19"/>
+      <c r="P24" s="22"/>
       <c r="Q24" s="13">
         <v>113.98</v>
       </c>
@@ -1536,8 +1636,8 @@
       <c r="G25" s="1"/>
       <c r="M25" s="3"/>
       <c r="N25" s="14"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="22"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="3"/>
     </row>
@@ -1584,4 +1684,686 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="27.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>42384</v>
+      </c>
+      <c r="B3" s="35">
+        <v>45.96</v>
+      </c>
+      <c r="C3" s="4">
+        <f>B3/6</f>
+        <v>7.66</v>
+      </c>
+      <c r="D3" s="4">
+        <f>B3/6</f>
+        <v>7.66</v>
+      </c>
+      <c r="E3" s="4">
+        <f>B3/6</f>
+        <v>7.66</v>
+      </c>
+      <c r="F3" s="4">
+        <f>B3/6</f>
+        <v>7.66</v>
+      </c>
+      <c r="G3" s="4">
+        <f>B3/6</f>
+        <v>7.66</v>
+      </c>
+      <c r="H3" s="4">
+        <f>B3/6</f>
+        <v>7.66</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>42415</v>
+      </c>
+      <c r="B4" s="36">
+        <v>263.16000000000003</v>
+      </c>
+      <c r="C4" s="36">
+        <v>31.88</v>
+      </c>
+      <c r="D4" s="37">
+        <f>31.88</f>
+        <v>31.88</v>
+      </c>
+      <c r="E4" s="36">
+        <v>31.88</v>
+      </c>
+      <c r="F4" s="36">
+        <f>31.88+15</f>
+        <v>46.879999999999995</v>
+      </c>
+      <c r="G4" s="37">
+        <f>31.88+25</f>
+        <v>56.879999999999995</v>
+      </c>
+      <c r="H4" s="37">
+        <f>31.88</f>
+        <v>31.88</v>
+      </c>
+      <c r="I4" s="37">
+        <f>31.88</f>
+        <v>31.88</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="4">
+        <f>SUM(C3:C14)</f>
+        <v>39.54</v>
+      </c>
+      <c r="N4" s="43">
+        <v>207.67</v>
+      </c>
+      <c r="O4" s="44">
+        <f>SUM(M4:M5)-N4+P4</f>
+        <v>-128.58999999999997</v>
+      </c>
+      <c r="P4" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>42444</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="4">
+        <f>SUM(D3:D14)</f>
+        <v>39.54</v>
+      </c>
+      <c r="N5" s="43"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>42475</v>
+      </c>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="4">
+        <f>SUM(E3:E14)</f>
+        <v>39.54</v>
+      </c>
+      <c r="N6" s="4">
+        <v>100</v>
+      </c>
+      <c r="O6" s="47">
+        <f>M6-N6+P6</f>
+        <v>-29.2</v>
+      </c>
+      <c r="P6" s="48">
+        <v>31.26</v>
+      </c>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>42505</v>
+      </c>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" s="4">
+        <f>SUM(F3:F14)</f>
+        <v>54.539999999999992</v>
+      </c>
+      <c r="N7" s="4">
+        <v>54.54</v>
+      </c>
+      <c r="O7" s="47">
+        <f>M7-N7</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="49">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>42536</v>
+      </c>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="4">
+        <f>SUM(G2:G13)</f>
+        <v>64.539999999999992</v>
+      </c>
+      <c r="N8" s="50">
+        <v>0</v>
+      </c>
+      <c r="O8" s="51">
+        <f>M8+M9-N8</f>
+        <v>104.07999999999998</v>
+      </c>
+      <c r="P8" s="41">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>42566</v>
+      </c>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="4">
+        <f>SUM(H2:H13)</f>
+        <v>39.54</v>
+      </c>
+      <c r="N9" s="52"/>
+      <c r="O9" s="53"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>42597</v>
+      </c>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="4">
+        <f>SUM(I2:I13)</f>
+        <v>31.88</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+      <c r="O10" s="54">
+        <f>M10-N10+P10</f>
+        <v>138.51</v>
+      </c>
+      <c r="P10" s="4">
+        <v>106.63</v>
+      </c>
+      <c r="Q10" s="1"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>42628</v>
+      </c>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>42658</v>
+      </c>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>42689</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>42719</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="26"/>
+    </row>
+    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="26"/>
+      <c r="O15" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="P15" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="3">
+        <v>1</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="M16" s="39">
+        <v>42401</v>
+      </c>
+      <c r="N16" s="40"/>
+      <c r="O16" s="38">
+        <v>100</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="3">
+        <v>2</v>
+      </c>
+      <c r="L17" s="14"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="3"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="3">
+        <v>3</v>
+      </c>
+      <c r="L18" s="14"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="3"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="3">
+        <v>4</v>
+      </c>
+      <c r="L19" s="14"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="3"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="E20" s="17"/>
+      <c r="K20" s="3">
+        <v>5</v>
+      </c>
+      <c r="L20" s="14"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="3"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="G21" s="7"/>
+      <c r="K21" s="3">
+        <v>6</v>
+      </c>
+      <c r="L21" s="14"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="3"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="K22" s="3">
+        <v>7</v>
+      </c>
+      <c r="L22" s="14"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="3"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F23" s="1"/>
+      <c r="K23" s="3">
+        <v>8</v>
+      </c>
+      <c r="L23" s="14"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="40"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="3"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F24" s="1"/>
+      <c r="K24" s="3">
+        <v>9</v>
+      </c>
+      <c r="L24" s="14"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="40"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="3"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F29" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="K14:P14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated payments for Feb Billing
</commit_message>
<xml_diff>
--- a/ATT_Bill.xlsx
+++ b/ATT_Bill.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8b893bbfaaa31d3c/ATT_Bill/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giria\OneDrive\ATT_Bill\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -344,7 +344,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -425,78 +425,81 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -514,70 +517,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>16</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>8</xdr:col>
-          <xdr:colOff>857250</xdr:colOff>
-          <xdr:row>26</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
-        </xdr:to>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="3" name="Picture 2"/>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-              <a:extLst>
-                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="$L$3:$P$10" spid="_x0000_s1027"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-            <a:srcRect/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="3009900" y="3619500"/>
-              <a:ext cx="3762375" cy="1914525"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -867,19 +806,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -949,16 +888,16 @@
       <c r="F3" s="11">
         <v>53.44</v>
       </c>
-      <c r="G3" s="30">
-        <v>0</v>
-      </c>
-      <c r="H3" s="30">
-        <v>0</v>
-      </c>
-      <c r="I3" s="30">
-        <v>0</v>
-      </c>
-      <c r="J3" s="30">
+      <c r="G3" s="37">
+        <v>0</v>
+      </c>
+      <c r="H3" s="37">
+        <v>0</v>
+      </c>
+      <c r="I3" s="37">
+        <v>0</v>
+      </c>
+      <c r="J3" s="37">
         <v>0</v>
       </c>
       <c r="K3" s="2"/>
@@ -996,10 +935,10 @@
       <c r="F4" s="11">
         <v>38.54</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
       <c r="K4" s="2"/>
       <c r="L4" s="1"/>
       <c r="M4" s="2" t="s">
@@ -1009,11 +948,11 @@
         <f>SUM(C3:C15)</f>
         <v>482.77999999999992</v>
       </c>
-      <c r="O4" s="30">
+      <c r="O4" s="37">
         <f>200+490.45</f>
         <v>690.45</v>
       </c>
-      <c r="P4" s="33">
+      <c r="P4" s="39">
         <f>N4+N5-O4</f>
         <v>-207.67000000000013</v>
       </c>
@@ -1038,10 +977,10 @@
       <c r="F5" s="11">
         <v>38.229999999999997</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
       <c r="K5" s="2"/>
       <c r="L5" s="1"/>
       <c r="M5" s="2" t="s">
@@ -1051,8 +990,8 @@
         <f>SUM(J3:J15)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="32"/>
-      <c r="P5" s="34"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="40"/>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1074,10 +1013,10 @@
       <c r="F6" s="11">
         <v>38.54</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
       <c r="K6" s="2"/>
       <c r="L6" s="1"/>
       <c r="M6" s="2" t="s">
@@ -1116,10 +1055,10 @@
       <c r="F7" s="11">
         <v>38.69</v>
       </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
       <c r="K7" s="2"/>
       <c r="L7" s="1"/>
       <c r="M7" s="2" t="s">
@@ -1129,10 +1068,10 @@
         <f>SUM(F3:F15)</f>
         <v>491.13999999999993</v>
       </c>
-      <c r="O7" s="30">
+      <c r="O7" s="37">
         <v>1024.28</v>
       </c>
-      <c r="P7" s="33">
+      <c r="P7" s="39">
         <f>N7+N8-O7</f>
         <v>0</v>
       </c>
@@ -1157,10 +1096,10 @@
       <c r="F8" s="11">
         <v>39.799999999999997</v>
       </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
       <c r="K8" s="2"/>
       <c r="L8" s="1"/>
       <c r="M8" s="2" t="s">
@@ -1170,8 +1109,8 @@
         <f>SUM(E3:E14)</f>
         <v>533.14</v>
       </c>
-      <c r="O8" s="32"/>
-      <c r="P8" s="34"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="40"/>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1193,10 +1132,10 @@
       <c r="F9" s="11">
         <v>38.69</v>
       </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
       <c r="K9" s="2"/>
       <c r="L9" s="1"/>
       <c r="M9" s="2" t="s">
@@ -1206,7 +1145,7 @@
         <f>SUM(G3:G15)</f>
         <v>175.34</v>
       </c>
-      <c r="O9" s="30">
+      <c r="O9" s="37">
         <f>113.35+61.99+51.99</f>
         <v>227.33</v>
       </c>
@@ -1236,10 +1175,10 @@
       <c r="F10" s="11">
         <v>39.14</v>
       </c>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
       <c r="K10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1251,7 +1190,7 @@
         <f>SUM(I3:I15)</f>
         <v>51.99</v>
       </c>
-      <c r="O10" s="32"/>
+      <c r="O10" s="38"/>
       <c r="P10" s="42"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
@@ -1275,10 +1214,10 @@
       <c r="F11" s="11">
         <v>38.92</v>
       </c>
-      <c r="G11" s="32"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
       <c r="K11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1322,9 +1261,9 @@
       <c r="G12" s="11">
         <v>52.78</v>
       </c>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
       <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1358,9 +1297,9 @@
       <c r="G13" s="11">
         <v>60.57</v>
       </c>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="31"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="43"/>
       <c r="K13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1406,7 +1345,7 @@
         <f>36.99+15</f>
         <v>51.99</v>
       </c>
-      <c r="J14" s="32"/>
+      <c r="J14" s="38"/>
       <c r="K14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1457,14 +1396,14 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="37" t="s">
+      <c r="M15" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="38"/>
-      <c r="O15" s="38"/>
-      <c r="P15" s="38"/>
-      <c r="Q15" s="38"/>
-      <c r="R15" s="39"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="35"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -1485,10 +1424,10 @@
       <c r="N16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O16" s="40" t="s">
+      <c r="O16" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="P16" s="40"/>
+      <c r="P16" s="36"/>
       <c r="Q16" s="10" t="s">
         <v>23</v>
       </c>
@@ -1515,10 +1454,10 @@
       <c r="N17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O17" s="35">
+      <c r="O17" s="31">
         <v>42053</v>
       </c>
-      <c r="P17" s="35"/>
+      <c r="P17" s="31"/>
       <c r="Q17" s="13">
         <v>108</v>
       </c>
@@ -1544,10 +1483,10 @@
       <c r="N18" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O18" s="35">
+      <c r="O18" s="31">
         <v>42086</v>
       </c>
-      <c r="P18" s="35"/>
+      <c r="P18" s="31"/>
       <c r="Q18" s="13">
         <v>200</v>
       </c>
@@ -1573,10 +1512,10 @@
       <c r="N19" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O19" s="35">
+      <c r="O19" s="31">
         <v>42111</v>
       </c>
-      <c r="P19" s="35"/>
+      <c r="P19" s="31"/>
       <c r="Q19" s="13">
         <v>100</v>
       </c>
@@ -1601,10 +1540,10 @@
       <c r="N20" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O20" s="35">
+      <c r="O20" s="31">
         <v>42214</v>
       </c>
-      <c r="P20" s="35"/>
+      <c r="P20" s="31"/>
       <c r="Q20" s="13">
         <v>160</v>
       </c>
@@ -1623,10 +1562,10 @@
       <c r="N21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O21" s="35">
+      <c r="O21" s="31">
         <v>42325</v>
       </c>
-      <c r="P21" s="35"/>
+      <c r="P21" s="31"/>
       <c r="Q21" s="13">
         <v>113.35</v>
       </c>
@@ -1645,10 +1584,10 @@
       <c r="N22" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O22" s="35">
+      <c r="O22" s="31">
         <v>42325</v>
       </c>
-      <c r="P22" s="35"/>
+      <c r="P22" s="31"/>
       <c r="Q22" s="13">
         <v>80</v>
       </c>
@@ -1666,10 +1605,10 @@
       <c r="N23" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O23" s="35">
+      <c r="O23" s="31">
         <v>42341</v>
       </c>
-      <c r="P23" s="35"/>
+      <c r="P23" s="31"/>
       <c r="Q23" s="13">
         <v>490.45</v>
       </c>
@@ -1685,10 +1624,10 @@
       <c r="N24" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O24" s="35">
+      <c r="O24" s="31">
         <v>42364</v>
       </c>
-      <c r="P24" s="35"/>
+      <c r="P24" s="31"/>
       <c r="Q24" s="13">
         <v>113.98</v>
       </c>
@@ -1700,8 +1639,8 @@
       <c r="G25" s="1"/>
       <c r="M25" s="3"/>
       <c r="N25" s="14"/>
-      <c r="O25" s="35"/>
-      <c r="P25" s="35"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="31"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="3"/>
     </row>
@@ -1722,6 +1661,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="G3:G11"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="J3:J14"/>
+    <mergeCell ref="I3:I13"/>
+    <mergeCell ref="H3:H13"/>
     <mergeCell ref="O25:P25"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M15:R15"/>
@@ -1738,12 +1683,6 @@
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="O9:O10"/>
     <mergeCell ref="P9:P10"/>
-    <mergeCell ref="G3:G11"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="J3:J14"/>
-    <mergeCell ref="I3:I13"/>
-    <mergeCell ref="H3:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1751,11 +1690,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1778,18 +1717,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
+      <c r="A1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1935,14 +1874,14 @@
         <f>SUM(C3:C14)</f>
         <v>39.54</v>
       </c>
-      <c r="N4" s="45">
+      <c r="N4" s="55">
         <v>207.67</v>
       </c>
       <c r="O4" s="46">
         <f>SUM(M4:M5)-N4+P4</f>
         <v>-128.58999999999997</v>
       </c>
-      <c r="P4" s="51">
+      <c r="P4" s="49">
         <v>0</v>
       </c>
       <c r="Q4" s="1"/>
@@ -1968,9 +1907,9 @@
         <f>SUM(D3:D14)</f>
         <v>39.54</v>
       </c>
-      <c r="N5" s="45"/>
+      <c r="N5" s="55"/>
       <c r="O5" s="46"/>
-      <c r="P5" s="52"/>
+      <c r="P5" s="50"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -2061,13 +2000,13 @@
         <v>64.539999999999992</v>
       </c>
       <c r="N8" s="47">
-        <v>0</v>
-      </c>
-      <c r="O8" s="49">
+        <v>104.08</v>
+      </c>
+      <c r="O8" s="56">
         <f>M8+M9-N8</f>
-        <v>104.07999999999998</v>
-      </c>
-      <c r="P8" s="53">
+        <v>0</v>
+      </c>
+      <c r="P8" s="51">
         <v>0</v>
       </c>
       <c r="Q8" s="1"/>
@@ -2094,8 +2033,8 @@
         <v>39.54</v>
       </c>
       <c r="N9" s="48"/>
-      <c r="O9" s="50"/>
-      <c r="P9" s="54"/>
+      <c r="O9" s="57"/>
+      <c r="P9" s="52"/>
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -2120,11 +2059,11 @@
         <v>31.88</v>
       </c>
       <c r="N10" s="4">
-        <v>0</v>
-      </c>
-      <c r="O10" s="29">
+        <v>138.51</v>
+      </c>
+      <c r="O10" s="30">
         <f>M10-N10+P10</f>
-        <v>138.51</v>
+        <v>0</v>
       </c>
       <c r="P10" s="29">
         <v>106.63</v>
@@ -2209,14 +2148,14 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="37" t="s">
+      <c r="K14" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="38"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="39"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="35"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -2235,10 +2174,10 @@
       <c r="L15" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="37" t="s">
+      <c r="M15" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="N15" s="39"/>
+      <c r="N15" s="35"/>
       <c r="O15" s="21" t="s">
         <v>23</v>
       </c>
@@ -2263,10 +2202,10 @@
       <c r="L16" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="M16" s="43">
+      <c r="M16" s="53">
         <v>42401</v>
       </c>
-      <c r="N16" s="44"/>
+      <c r="N16" s="54"/>
       <c r="O16" s="25">
         <v>100</v>
       </c>
@@ -2288,8 +2227,8 @@
         <v>2</v>
       </c>
       <c r="L17" s="14"/>
-      <c r="M17" s="43"/>
-      <c r="N17" s="44"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="54"/>
       <c r="O17" s="13"/>
       <c r="P17" s="3"/>
     </row>
@@ -2307,8 +2246,8 @@
         <v>3</v>
       </c>
       <c r="L18" s="14"/>
-      <c r="M18" s="43"/>
-      <c r="N18" s="44"/>
+      <c r="M18" s="53"/>
+      <c r="N18" s="54"/>
       <c r="O18" s="13"/>
       <c r="P18" s="3"/>
     </row>
@@ -2325,8 +2264,8 @@
         <v>4</v>
       </c>
       <c r="L19" s="14"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="44"/>
+      <c r="M19" s="53"/>
+      <c r="N19" s="54"/>
       <c r="O19" s="13"/>
       <c r="P19" s="3"/>
     </row>
@@ -2338,8 +2277,8 @@
         <v>5</v>
       </c>
       <c r="L20" s="14"/>
-      <c r="M20" s="43"/>
-      <c r="N20" s="44"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="54"/>
       <c r="O20" s="13"/>
       <c r="P20" s="3"/>
     </row>
@@ -2351,8 +2290,8 @@
         <v>6</v>
       </c>
       <c r="L21" s="14"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="44"/>
+      <c r="M21" s="53"/>
+      <c r="N21" s="54"/>
       <c r="O21" s="13"/>
       <c r="P21" s="3"/>
     </row>
@@ -2364,8 +2303,8 @@
         <v>7</v>
       </c>
       <c r="L22" s="14"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="44"/>
+      <c r="M22" s="53"/>
+      <c r="N22" s="54"/>
       <c r="O22" s="13"/>
       <c r="P22" s="3"/>
     </row>
@@ -2375,8 +2314,8 @@
         <v>8</v>
       </c>
       <c r="L23" s="14"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="44"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="54"/>
       <c r="O23" s="13"/>
       <c r="P23" s="3"/>
     </row>
@@ -2386,8 +2325,8 @@
         <v>9</v>
       </c>
       <c r="L24" s="14"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="44"/>
+      <c r="M24" s="53"/>
+      <c r="N24" s="54"/>
       <c r="O24" s="13"/>
       <c r="P24" s="3"/>
     </row>
@@ -2408,16 +2347,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="K14:P14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M22:N22"/>
     <mergeCell ref="M23:N23"/>
     <mergeCell ref="M24:N24"/>
     <mergeCell ref="N4:N5"/>
@@ -2426,10 +2355,18 @@
     <mergeCell ref="M18:N18"/>
     <mergeCell ref="M19:N19"/>
     <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="K14:P14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated March ATT Bill
</commit_message>
<xml_diff>
--- a/ATT_Bill.xlsx
+++ b/ATT_Bill.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giria\OneDrive\ATT_Bill\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mithun\OneDrive\ATT_Bill\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="33">
   <si>
     <t>ATT Family Plan Bill Details</t>
   </si>
@@ -196,7 +196,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +218,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -344,7 +350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -420,14 +426,29 @@
     <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="6" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -446,27 +467,25 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="7" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="3" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="3" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -482,23 +501,13 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -784,9 +793,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P6" sqref="P6"/>
+      <selection pane="bottomLeft" activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,19 +815,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -888,16 +897,16 @@
       <c r="F3" s="11">
         <v>53.44</v>
       </c>
-      <c r="G3" s="37">
+      <c r="G3" s="31">
         <v>0</v>
       </c>
-      <c r="H3" s="37">
+      <c r="H3" s="31">
         <v>0</v>
       </c>
-      <c r="I3" s="37">
+      <c r="I3" s="31">
         <v>0</v>
       </c>
-      <c r="J3" s="37">
+      <c r="J3" s="31">
         <v>0</v>
       </c>
       <c r="K3" s="2"/>
@@ -935,10 +944,10 @@
       <c r="F4" s="11">
         <v>38.54</v>
       </c>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
       <c r="K4" s="2"/>
       <c r="L4" s="1"/>
       <c r="M4" s="2" t="s">
@@ -948,11 +957,11 @@
         <f>SUM(C3:C15)</f>
         <v>482.77999999999992</v>
       </c>
-      <c r="O4" s="37">
+      <c r="O4" s="31">
         <f>200+490.45</f>
         <v>690.45</v>
       </c>
-      <c r="P4" s="39">
+      <c r="P4" s="34">
         <f>N4+N5-O4</f>
         <v>-207.67000000000013</v>
       </c>
@@ -977,10 +986,10 @@
       <c r="F5" s="11">
         <v>38.229999999999997</v>
       </c>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
       <c r="K5" s="2"/>
       <c r="L5" s="1"/>
       <c r="M5" s="2" t="s">
@@ -990,8 +999,8 @@
         <f>SUM(J3:J15)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="38"/>
-      <c r="P5" s="40"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="35"/>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1013,10 +1022,10 @@
       <c r="F6" s="11">
         <v>38.54</v>
       </c>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
       <c r="K6" s="2"/>
       <c r="L6" s="1"/>
       <c r="M6" s="2" t="s">
@@ -1055,10 +1064,10 @@
       <c r="F7" s="11">
         <v>38.69</v>
       </c>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
       <c r="K7" s="2"/>
       <c r="L7" s="1"/>
       <c r="M7" s="2" t="s">
@@ -1068,10 +1077,10 @@
         <f>SUM(F3:F15)</f>
         <v>491.13999999999993</v>
       </c>
-      <c r="O7" s="37">
+      <c r="O7" s="31">
         <v>1024.28</v>
       </c>
-      <c r="P7" s="39">
+      <c r="P7" s="34">
         <f>N7+N8-O7</f>
         <v>0</v>
       </c>
@@ -1096,10 +1105,10 @@
       <c r="F8" s="11">
         <v>39.799999999999997</v>
       </c>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
       <c r="K8" s="2"/>
       <c r="L8" s="1"/>
       <c r="M8" s="2" t="s">
@@ -1109,8 +1118,8 @@
         <f>SUM(E3:E14)</f>
         <v>533.14</v>
       </c>
-      <c r="O8" s="38"/>
-      <c r="P8" s="40"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="35"/>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1132,10 +1141,10 @@
       <c r="F9" s="11">
         <v>38.69</v>
       </c>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
       <c r="K9" s="2"/>
       <c r="L9" s="1"/>
       <c r="M9" s="2" t="s">
@@ -1145,11 +1154,11 @@
         <f>SUM(G3:G15)</f>
         <v>175.34</v>
       </c>
-      <c r="O9" s="37">
+      <c r="O9" s="31">
         <f>113.35+61.99+51.99</f>
         <v>227.33</v>
       </c>
-      <c r="P9" s="41">
+      <c r="P9" s="42">
         <f>N9+N10-O9</f>
         <v>0</v>
       </c>
@@ -1175,10 +1184,10 @@
       <c r="F10" s="11">
         <v>39.14</v>
       </c>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
       <c r="K10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1190,8 +1199,8 @@
         <f>SUM(I3:I15)</f>
         <v>51.99</v>
       </c>
-      <c r="O10" s="38"/>
-      <c r="P10" s="42"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="43"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
@@ -1214,10 +1223,10 @@
       <c r="F11" s="11">
         <v>38.92</v>
       </c>
-      <c r="G11" s="38"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
       <c r="K11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1261,9 +1270,9 @@
       <c r="G12" s="11">
         <v>52.78</v>
       </c>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
       <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1297,9 +1306,9 @@
       <c r="G13" s="11">
         <v>60.57</v>
       </c>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="43"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="32"/>
       <c r="K13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1345,7 +1354,7 @@
         <f>36.99+15</f>
         <v>51.99</v>
       </c>
-      <c r="J14" s="38"/>
+      <c r="J14" s="33"/>
       <c r="K14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1396,14 +1405,14 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="33" t="s">
+      <c r="M15" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
-      <c r="P15" s="34"/>
-      <c r="Q15" s="34"/>
-      <c r="R15" s="35"/>
+      <c r="N15" s="39"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="40"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -1424,10 +1433,10 @@
       <c r="N16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O16" s="36" t="s">
+      <c r="O16" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="P16" s="36"/>
+      <c r="P16" s="41"/>
       <c r="Q16" s="10" t="s">
         <v>23</v>
       </c>
@@ -1454,10 +1463,10 @@
       <c r="N17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O17" s="31">
+      <c r="O17" s="36">
         <v>42053</v>
       </c>
-      <c r="P17" s="31"/>
+      <c r="P17" s="36"/>
       <c r="Q17" s="13">
         <v>108</v>
       </c>
@@ -1483,10 +1492,10 @@
       <c r="N18" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O18" s="31">
+      <c r="O18" s="36">
         <v>42086</v>
       </c>
-      <c r="P18" s="31"/>
+      <c r="P18" s="36"/>
       <c r="Q18" s="13">
         <v>200</v>
       </c>
@@ -1512,10 +1521,10 @@
       <c r="N19" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O19" s="31">
+      <c r="O19" s="36">
         <v>42111</v>
       </c>
-      <c r="P19" s="31"/>
+      <c r="P19" s="36"/>
       <c r="Q19" s="13">
         <v>100</v>
       </c>
@@ -1540,10 +1549,10 @@
       <c r="N20" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O20" s="31">
+      <c r="O20" s="36">
         <v>42214</v>
       </c>
-      <c r="P20" s="31"/>
+      <c r="P20" s="36"/>
       <c r="Q20" s="13">
         <v>160</v>
       </c>
@@ -1562,10 +1571,10 @@
       <c r="N21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O21" s="31">
+      <c r="O21" s="36">
         <v>42325</v>
       </c>
-      <c r="P21" s="31"/>
+      <c r="P21" s="36"/>
       <c r="Q21" s="13">
         <v>113.35</v>
       </c>
@@ -1584,10 +1593,10 @@
       <c r="N22" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O22" s="31">
+      <c r="O22" s="36">
         <v>42325</v>
       </c>
-      <c r="P22" s="31"/>
+      <c r="P22" s="36"/>
       <c r="Q22" s="13">
         <v>80</v>
       </c>
@@ -1605,10 +1614,10 @@
       <c r="N23" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O23" s="31">
+      <c r="O23" s="36">
         <v>42341</v>
       </c>
-      <c r="P23" s="31"/>
+      <c r="P23" s="36"/>
       <c r="Q23" s="13">
         <v>490.45</v>
       </c>
@@ -1624,10 +1633,10 @@
       <c r="N24" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O24" s="31">
+      <c r="O24" s="36">
         <v>42364</v>
       </c>
-      <c r="P24" s="31"/>
+      <c r="P24" s="36"/>
       <c r="Q24" s="13">
         <v>113.98</v>
       </c>
@@ -1639,8 +1648,8 @@
       <c r="G25" s="1"/>
       <c r="M25" s="3"/>
       <c r="N25" s="14"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="31"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="36"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="3"/>
     </row>
@@ -1661,12 +1670,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="G3:G11"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="J3:J14"/>
-    <mergeCell ref="I3:I13"/>
-    <mergeCell ref="H3:H13"/>
     <mergeCell ref="O25:P25"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M15:R15"/>
@@ -1683,6 +1686,12 @@
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="O9:O10"/>
     <mergeCell ref="P9:P10"/>
+    <mergeCell ref="G3:G11"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="J3:J14"/>
+    <mergeCell ref="I3:I13"/>
+    <mergeCell ref="H3:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1693,8 +1702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1717,18 +1726,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1872,33 +1881,53 @@
       </c>
       <c r="M4" s="4">
         <f>SUM(C3:C14)</f>
-        <v>39.54</v>
-      </c>
-      <c r="N4" s="55">
+        <v>73.37</v>
+      </c>
+      <c r="N4" s="46">
         <v>207.67</v>
       </c>
-      <c r="O4" s="46">
+      <c r="O4" s="53">
         <f>SUM(M4:M5)-N4+P4</f>
-        <v>-128.58999999999997</v>
-      </c>
-      <c r="P4" s="49">
+        <v>-94.759999999999991</v>
+      </c>
+      <c r="P4" s="47">
         <v>0</v>
       </c>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>42444</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="2"/>
+      <c r="B5" s="22">
+        <v>242.97</v>
+      </c>
+      <c r="C5" s="22">
+        <v>33.83</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="22">
+        <v>33.83</v>
+      </c>
+      <c r="F5" s="22">
+        <f>33.83+15</f>
+        <v>48.83</v>
+      </c>
+      <c r="G5" s="4">
+        <f>33.83+25</f>
+        <v>58.83</v>
+      </c>
+      <c r="H5" s="4">
+        <v>33.83</v>
+      </c>
+      <c r="I5" s="4">
+        <v>33.83</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="K5" s="1"/>
       <c r="L5" s="2" t="s">
         <v>29</v>
@@ -1907,9 +1936,9 @@
         <f>SUM(D3:D14)</f>
         <v>39.54</v>
       </c>
-      <c r="N5" s="55"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="50"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="48"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -1931,16 +1960,16 @@
       </c>
       <c r="M6" s="4">
         <f>SUM(E3:E14)</f>
-        <v>39.54</v>
+        <v>73.37</v>
       </c>
       <c r="N6" s="4">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="O6" s="26">
         <f>M6-N6+P6</f>
-        <v>-29.2</v>
-      </c>
-      <c r="P6" s="27">
+        <v>-25.369999999999994</v>
+      </c>
+      <c r="P6" s="28">
         <v>31.26</v>
       </c>
       <c r="Q6" s="1"/>
@@ -1964,16 +1993,16 @@
       </c>
       <c r="M7" s="4">
         <f>SUM(F3:F14)</f>
-        <v>54.539999999999992</v>
+        <v>103.36999999999999</v>
       </c>
       <c r="N7" s="4">
-        <v>54.54</v>
+        <v>103.37</v>
       </c>
       <c r="O7" s="26">
         <f>M7-N7</f>
         <v>0</v>
       </c>
-      <c r="P7" s="28">
+      <c r="P7" s="29">
         <v>0</v>
       </c>
       <c r="Q7" s="1"/>
@@ -1997,16 +2026,16 @@
       </c>
       <c r="M8" s="4">
         <f>SUM(G2:G13)</f>
-        <v>64.539999999999992</v>
-      </c>
-      <c r="N8" s="47">
+        <v>123.36999999999999</v>
+      </c>
+      <c r="N8" s="54">
         <v>104.08</v>
       </c>
       <c r="O8" s="56">
         <f>M8+M9-N8</f>
-        <v>0</v>
-      </c>
-      <c r="P8" s="51">
+        <v>92.660000000000011</v>
+      </c>
+      <c r="P8" s="49">
         <v>0</v>
       </c>
       <c r="Q8" s="1"/>
@@ -2030,11 +2059,11 @@
       </c>
       <c r="M9" s="4">
         <f>SUM(H2:H13)</f>
-        <v>39.54</v>
-      </c>
-      <c r="N9" s="48"/>
+        <v>73.37</v>
+      </c>
+      <c r="N9" s="55"/>
       <c r="O9" s="57"/>
-      <c r="P9" s="52"/>
+      <c r="P9" s="50"/>
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -2056,16 +2085,16 @@
       </c>
       <c r="M10" s="4">
         <f>SUM(I2:I13)</f>
-        <v>31.88</v>
+        <v>65.709999999999994</v>
       </c>
       <c r="N10" s="4">
         <v>138.51</v>
       </c>
-      <c r="O10" s="30">
+      <c r="O10" s="27">
         <f>M10-N10+P10</f>
-        <v>0</v>
-      </c>
-      <c r="P10" s="29">
+        <v>33.83</v>
+      </c>
+      <c r="P10" s="30">
         <v>106.63</v>
       </c>
       <c r="Q10" s="1"/>
@@ -2148,14 +2177,14 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="33" t="s">
+      <c r="K14" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="34"/>
-      <c r="P14" s="35"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="40"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -2174,10 +2203,10 @@
       <c r="L15" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="33" t="s">
+      <c r="M15" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="N15" s="35"/>
+      <c r="N15" s="40"/>
       <c r="O15" s="21" t="s">
         <v>23</v>
       </c>
@@ -2202,10 +2231,10 @@
       <c r="L16" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="M16" s="53">
+      <c r="M16" s="44">
         <v>42401</v>
       </c>
-      <c r="N16" s="54"/>
+      <c r="N16" s="45"/>
       <c r="O16" s="25">
         <v>100</v>
       </c>
@@ -2226,18 +2255,26 @@
       <c r="K17" s="3">
         <v>2</v>
       </c>
-      <c r="L17" s="14"/>
-      <c r="M17" s="53"/>
-      <c r="N17" s="54"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="3"/>
+      <c r="L17" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="M17" s="44">
+        <v>42433</v>
+      </c>
+      <c r="N17" s="45"/>
+      <c r="O17" s="25">
+        <v>30</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="E18" s="8"/>
       <c r="F18" s="1"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
@@ -2246,8 +2283,8 @@
         <v>3</v>
       </c>
       <c r="L18" s="14"/>
-      <c r="M18" s="53"/>
-      <c r="N18" s="54"/>
+      <c r="M18" s="44"/>
+      <c r="N18" s="45"/>
       <c r="O18" s="13"/>
       <c r="P18" s="3"/>
     </row>
@@ -2256,7 +2293,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="16"/>
+      <c r="E19" s="58"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="J19" s="1"/>
@@ -2264,8 +2301,8 @@
         <v>4</v>
       </c>
       <c r="L19" s="14"/>
-      <c r="M19" s="53"/>
-      <c r="N19" s="54"/>
+      <c r="M19" s="44"/>
+      <c r="N19" s="45"/>
       <c r="O19" s="13"/>
       <c r="P19" s="3"/>
     </row>
@@ -2277,8 +2314,8 @@
         <v>5</v>
       </c>
       <c r="L20" s="14"/>
-      <c r="M20" s="53"/>
-      <c r="N20" s="54"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="45"/>
       <c r="O20" s="13"/>
       <c r="P20" s="3"/>
     </row>
@@ -2290,8 +2327,8 @@
         <v>6</v>
       </c>
       <c r="L21" s="14"/>
-      <c r="M21" s="53"/>
-      <c r="N21" s="54"/>
+      <c r="M21" s="44"/>
+      <c r="N21" s="45"/>
       <c r="O21" s="13"/>
       <c r="P21" s="3"/>
     </row>
@@ -2303,8 +2340,8 @@
         <v>7</v>
       </c>
       <c r="L22" s="14"/>
-      <c r="M22" s="53"/>
-      <c r="N22" s="54"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="45"/>
       <c r="O22" s="13"/>
       <c r="P22" s="3"/>
     </row>
@@ -2314,8 +2351,8 @@
         <v>8</v>
       </c>
       <c r="L23" s="14"/>
-      <c r="M23" s="53"/>
-      <c r="N23" s="54"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="45"/>
       <c r="O23" s="13"/>
       <c r="P23" s="3"/>
     </row>
@@ -2325,8 +2362,8 @@
         <v>9</v>
       </c>
       <c r="L24" s="14"/>
-      <c r="M24" s="53"/>
-      <c r="N24" s="54"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="45"/>
       <c r="O24" s="13"/>
       <c r="P24" s="3"/>
     </row>
@@ -2347,6 +2384,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="K14:P14"/>
     <mergeCell ref="M23:N23"/>
     <mergeCell ref="M24:N24"/>
     <mergeCell ref="N4:N5"/>
@@ -2356,15 +2402,6 @@
     <mergeCell ref="M19:N19"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="M15:N15"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="K14:P14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated April 2016 Bill
</commit_message>
<xml_diff>
--- a/ATT_Bill.xlsx
+++ b/ATT_Bill.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="33">
   <si>
     <t>ATT Family Plan Bill Details</t>
   </si>
@@ -141,7 +141,7 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,13 +180,6 @@
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -423,15 +416,20 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -482,10 +480,10 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="7" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="3" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="3" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="6" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="6" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="5" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -501,13 +499,10 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -815,19 +810,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
+      <c r="A1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -897,16 +892,16 @@
       <c r="F3" s="11">
         <v>53.44</v>
       </c>
-      <c r="G3" s="31">
-        <v>0</v>
-      </c>
-      <c r="H3" s="31">
-        <v>0</v>
-      </c>
-      <c r="I3" s="31">
-        <v>0</v>
-      </c>
-      <c r="J3" s="31">
+      <c r="G3" s="32">
+        <v>0</v>
+      </c>
+      <c r="H3" s="32">
+        <v>0</v>
+      </c>
+      <c r="I3" s="32">
+        <v>0</v>
+      </c>
+      <c r="J3" s="32">
         <v>0</v>
       </c>
       <c r="K3" s="2"/>
@@ -944,10 +939,10 @@
       <c r="F4" s="11">
         <v>38.54</v>
       </c>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="2"/>
       <c r="L4" s="1"/>
       <c r="M4" s="2" t="s">
@@ -957,11 +952,11 @@
         <f>SUM(C3:C15)</f>
         <v>482.77999999999992</v>
       </c>
-      <c r="O4" s="31">
+      <c r="O4" s="32">
         <f>200+490.45</f>
         <v>690.45</v>
       </c>
-      <c r="P4" s="34">
+      <c r="P4" s="35">
         <f>N4+N5-O4</f>
         <v>-207.67000000000013</v>
       </c>
@@ -986,10 +981,10 @@
       <c r="F5" s="11">
         <v>38.229999999999997</v>
       </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
       <c r="K5" s="2"/>
       <c r="L5" s="1"/>
       <c r="M5" s="2" t="s">
@@ -999,8 +994,8 @@
         <f>SUM(J3:J15)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="33"/>
-      <c r="P5" s="35"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="36"/>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1022,10 +1017,10 @@
       <c r="F6" s="11">
         <v>38.54</v>
       </c>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
       <c r="K6" s="2"/>
       <c r="L6" s="1"/>
       <c r="M6" s="2" t="s">
@@ -1064,10 +1059,10 @@
       <c r="F7" s="11">
         <v>38.69</v>
       </c>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
       <c r="K7" s="2"/>
       <c r="L7" s="1"/>
       <c r="M7" s="2" t="s">
@@ -1077,10 +1072,10 @@
         <f>SUM(F3:F15)</f>
         <v>491.13999999999993</v>
       </c>
-      <c r="O7" s="31">
+      <c r="O7" s="32">
         <v>1024.28</v>
       </c>
-      <c r="P7" s="34">
+      <c r="P7" s="35">
         <f>N7+N8-O7</f>
         <v>0</v>
       </c>
@@ -1105,10 +1100,10 @@
       <c r="F8" s="11">
         <v>39.799999999999997</v>
       </c>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
       <c r="K8" s="2"/>
       <c r="L8" s="1"/>
       <c r="M8" s="2" t="s">
@@ -1118,8 +1113,8 @@
         <f>SUM(E3:E14)</f>
         <v>533.14</v>
       </c>
-      <c r="O8" s="33"/>
-      <c r="P8" s="35"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="36"/>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1141,10 +1136,10 @@
       <c r="F9" s="11">
         <v>38.69</v>
       </c>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
       <c r="K9" s="2"/>
       <c r="L9" s="1"/>
       <c r="M9" s="2" t="s">
@@ -1154,11 +1149,11 @@
         <f>SUM(G3:G15)</f>
         <v>175.34</v>
       </c>
-      <c r="O9" s="31">
+      <c r="O9" s="32">
         <f>113.35+61.99+51.99</f>
         <v>227.33</v>
       </c>
-      <c r="P9" s="42">
+      <c r="P9" s="43">
         <f>N9+N10-O9</f>
         <v>0</v>
       </c>
@@ -1184,10 +1179,10 @@
       <c r="F10" s="11">
         <v>39.14</v>
       </c>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
       <c r="K10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1199,8 +1194,8 @@
         <f>SUM(I3:I15)</f>
         <v>51.99</v>
       </c>
-      <c r="O10" s="33"/>
-      <c r="P10" s="43"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="44"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
@@ -1223,10 +1218,10 @@
       <c r="F11" s="11">
         <v>38.92</v>
       </c>
-      <c r="G11" s="33"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
       <c r="K11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1270,9 +1265,9 @@
       <c r="G12" s="11">
         <v>52.78</v>
       </c>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
       <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1306,9 +1301,9 @@
       <c r="G13" s="11">
         <v>60.57</v>
       </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="32"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="33"/>
       <c r="K13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1354,7 +1349,7 @@
         <f>36.99+15</f>
         <v>51.99</v>
       </c>
-      <c r="J14" s="33"/>
+      <c r="J14" s="34"/>
       <c r="K14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1405,14 +1400,14 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="38" t="s">
+      <c r="M15" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="39"/>
-      <c r="R15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="41"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -1433,10 +1428,10 @@
       <c r="N16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O16" s="41" t="s">
+      <c r="O16" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="P16" s="41"/>
+      <c r="P16" s="42"/>
       <c r="Q16" s="10" t="s">
         <v>23</v>
       </c>
@@ -1463,10 +1458,10 @@
       <c r="N17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O17" s="36">
+      <c r="O17" s="37">
         <v>42053</v>
       </c>
-      <c r="P17" s="36"/>
+      <c r="P17" s="37"/>
       <c r="Q17" s="13">
         <v>108</v>
       </c>
@@ -1492,10 +1487,10 @@
       <c r="N18" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O18" s="36">
+      <c r="O18" s="37">
         <v>42086</v>
       </c>
-      <c r="P18" s="36"/>
+      <c r="P18" s="37"/>
       <c r="Q18" s="13">
         <v>200</v>
       </c>
@@ -1521,10 +1516,10 @@
       <c r="N19" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O19" s="36">
+      <c r="O19" s="37">
         <v>42111</v>
       </c>
-      <c r="P19" s="36"/>
+      <c r="P19" s="37"/>
       <c r="Q19" s="13">
         <v>100</v>
       </c>
@@ -1549,10 +1544,10 @@
       <c r="N20" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O20" s="36">
+      <c r="O20" s="37">
         <v>42214</v>
       </c>
-      <c r="P20" s="36"/>
+      <c r="P20" s="37"/>
       <c r="Q20" s="13">
         <v>160</v>
       </c>
@@ -1571,10 +1566,10 @@
       <c r="N21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O21" s="36">
+      <c r="O21" s="37">
         <v>42325</v>
       </c>
-      <c r="P21" s="36"/>
+      <c r="P21" s="37"/>
       <c r="Q21" s="13">
         <v>113.35</v>
       </c>
@@ -1593,10 +1588,10 @@
       <c r="N22" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O22" s="36">
+      <c r="O22" s="37">
         <v>42325</v>
       </c>
-      <c r="P22" s="36"/>
+      <c r="P22" s="37"/>
       <c r="Q22" s="13">
         <v>80</v>
       </c>
@@ -1614,10 +1609,10 @@
       <c r="N23" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O23" s="36">
+      <c r="O23" s="37">
         <v>42341</v>
       </c>
-      <c r="P23" s="36"/>
+      <c r="P23" s="37"/>
       <c r="Q23" s="13">
         <v>490.45</v>
       </c>
@@ -1633,10 +1628,10 @@
       <c r="N24" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O24" s="36">
+      <c r="O24" s="37">
         <v>42364</v>
       </c>
-      <c r="P24" s="36"/>
+      <c r="P24" s="37"/>
       <c r="Q24" s="13">
         <v>113.98</v>
       </c>
@@ -1648,8 +1643,8 @@
       <c r="G25" s="1"/>
       <c r="M25" s="3"/>
       <c r="N25" s="14"/>
-      <c r="O25" s="36"/>
-      <c r="P25" s="36"/>
+      <c r="O25" s="37"/>
+      <c r="P25" s="37"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="3"/>
     </row>
@@ -1702,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1726,18 +1721,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
+      <c r="A1" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1881,16 +1876,16 @@
       </c>
       <c r="M4" s="4">
         <f>SUM(C3:C14)</f>
-        <v>73.37</v>
-      </c>
-      <c r="N4" s="46">
+        <v>107.2</v>
+      </c>
+      <c r="N4" s="47">
         <v>207.67</v>
       </c>
-      <c r="O4" s="53">
+      <c r="O4" s="54">
         <f>SUM(M4:M5)-N4+P4</f>
-        <v>-94.759999999999991</v>
-      </c>
-      <c r="P4" s="47">
+        <v>-60.929999999999978</v>
+      </c>
+      <c r="P4" s="48">
         <v>0</v>
       </c>
       <c r="Q4" s="1"/>
@@ -1936,40 +1931,60 @@
         <f>SUM(D3:D14)</f>
         <v>39.54</v>
       </c>
-      <c r="N5" s="46"/>
-      <c r="O5" s="53"/>
-      <c r="P5" s="48"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="49"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>42475</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="2"/>
+      <c r="B6" s="22">
+        <v>242.97</v>
+      </c>
+      <c r="C6" s="22">
+        <v>33.83</v>
+      </c>
+      <c r="D6" s="27">
+        <v>0</v>
+      </c>
+      <c r="E6" s="22">
+        <v>33.83</v>
+      </c>
+      <c r="F6" s="22">
+        <f>33.83+15</f>
+        <v>48.83</v>
+      </c>
+      <c r="G6" s="27">
+        <f>33.83+25</f>
+        <v>58.83</v>
+      </c>
+      <c r="H6" s="27">
+        <v>33.83</v>
+      </c>
+      <c r="I6" s="27">
+        <v>33.83</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="M6" s="4">
         <f>SUM(E3:E14)</f>
-        <v>73.37</v>
+        <v>107.2</v>
       </c>
       <c r="N6" s="4">
         <v>120</v>
       </c>
-      <c r="O6" s="26">
+      <c r="O6" s="28">
         <f>M6-N6+P6</f>
-        <v>-15.369999999999994</v>
-      </c>
-      <c r="P6" s="27">
+        <v>18.460000000000004</v>
+      </c>
+      <c r="P6" s="30">
         <v>31.26</v>
       </c>
       <c r="Q6" s="1"/>
@@ -1993,16 +2008,16 @@
       </c>
       <c r="M7" s="4">
         <f>SUM(F3:F14)</f>
-        <v>103.36999999999999</v>
+        <v>152.19999999999999</v>
       </c>
       <c r="N7" s="4">
-        <v>103.37</v>
-      </c>
-      <c r="O7" s="26">
+        <v>152.19999999999999</v>
+      </c>
+      <c r="O7" s="29">
         <f>M7-N7</f>
         <v>0</v>
       </c>
-      <c r="P7" s="28">
+      <c r="P7" s="30">
         <v>0</v>
       </c>
       <c r="Q7" s="1"/>
@@ -2025,18 +2040,18 @@
         <v>7</v>
       </c>
       <c r="M8" s="4">
-        <f>SUM(G2:G13)</f>
-        <v>123.36999999999999</v>
-      </c>
-      <c r="N8" s="54">
+        <f>SUM(G3:G14)</f>
+        <v>182.2</v>
+      </c>
+      <c r="N8" s="55">
         <f>104.08+92.66</f>
         <v>196.74</v>
       </c>
-      <c r="O8" s="56">
+      <c r="O8" s="57">
         <f>M8+M9-N8</f>
-        <v>0</v>
-      </c>
-      <c r="P8" s="49">
+        <v>92.659999999999968</v>
+      </c>
+      <c r="P8" s="50">
         <v>0</v>
       </c>
       <c r="Q8" s="1"/>
@@ -2059,12 +2074,12 @@
         <v>9</v>
       </c>
       <c r="M9" s="4">
-        <f>SUM(H2:H13)</f>
-        <v>73.37</v>
-      </c>
-      <c r="N9" s="55"/>
-      <c r="O9" s="57"/>
-      <c r="P9" s="50"/>
+        <f>SUM(H3:H14)</f>
+        <v>107.2</v>
+      </c>
+      <c r="N9" s="56"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="51"/>
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -2085,17 +2100,17 @@
         <v>8</v>
       </c>
       <c r="M10" s="4">
-        <f>SUM(I2:I13)</f>
-        <v>65.709999999999994</v>
+        <f>SUM(I3:I14)</f>
+        <v>99.539999999999992</v>
       </c>
       <c r="N10" s="4">
         <v>138.51</v>
       </c>
-      <c r="O10" s="58">
+      <c r="O10" s="28">
         <f>M10-N10+P10</f>
-        <v>33.83</v>
-      </c>
-      <c r="P10" s="29">
+        <v>67.66</v>
+      </c>
+      <c r="P10" s="31">
         <v>106.63</v>
       </c>
       <c r="Q10" s="1"/>
@@ -2139,7 +2154,7 @@
         <v>28</v>
       </c>
       <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+      <c r="N12" s="8"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -2178,14 +2193,14 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="38" t="s">
+      <c r="K14" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="39"/>
-      <c r="P14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="41"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -2204,10 +2219,10 @@
       <c r="L15" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="38" t="s">
+      <c r="M15" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="N15" s="40"/>
+      <c r="N15" s="41"/>
       <c r="O15" s="21" t="s">
         <v>23</v>
       </c>
@@ -2232,10 +2247,10 @@
       <c r="L16" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="M16" s="44">
+      <c r="M16" s="45">
         <v>42401</v>
       </c>
-      <c r="N16" s="45"/>
+      <c r="N16" s="46"/>
       <c r="O16" s="25">
         <v>100</v>
       </c>
@@ -2259,10 +2274,10 @@
       <c r="L17" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="44">
+      <c r="M17" s="45">
         <v>42402</v>
       </c>
-      <c r="N17" s="45"/>
+      <c r="N17" s="46"/>
       <c r="O17" s="25">
         <v>104.08</v>
       </c>
@@ -2286,10 +2301,10 @@
       <c r="L18" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="M18" s="44">
+      <c r="M18" s="45">
         <v>42433</v>
       </c>
-      <c r="N18" s="45"/>
+      <c r="N18" s="46"/>
       <c r="O18" s="25">
         <v>20</v>
       </c>
@@ -2302,7 +2317,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="30"/>
+      <c r="E19" s="26"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="J19" s="1"/>
@@ -2312,10 +2327,10 @@
       <c r="L19" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M19" s="44">
+      <c r="M19" s="45">
         <v>42433</v>
       </c>
-      <c r="N19" s="45"/>
+      <c r="N19" s="46"/>
       <c r="O19" s="25">
         <v>92.66</v>
       </c>
@@ -2331,8 +2346,8 @@
         <v>5</v>
       </c>
       <c r="L20" s="14"/>
-      <c r="M20" s="44"/>
-      <c r="N20" s="45"/>
+      <c r="M20" s="45"/>
+      <c r="N20" s="46"/>
       <c r="O20" s="13"/>
       <c r="P20" s="3"/>
     </row>
@@ -2344,8 +2359,8 @@
         <v>6</v>
       </c>
       <c r="L21" s="14"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="45"/>
+      <c r="M21" s="45"/>
+      <c r="N21" s="46"/>
       <c r="O21" s="13"/>
       <c r="P21" s="3"/>
     </row>
@@ -2357,8 +2372,8 @@
         <v>7</v>
       </c>
       <c r="L22" s="14"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="45"/>
+      <c r="M22" s="45"/>
+      <c r="N22" s="46"/>
       <c r="O22" s="13"/>
       <c r="P22" s="3"/>
     </row>
@@ -2368,8 +2383,8 @@
         <v>8</v>
       </c>
       <c r="L23" s="14"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="45"/>
+      <c r="M23" s="45"/>
+      <c r="N23" s="46"/>
       <c r="O23" s="13"/>
       <c r="P23" s="3"/>
     </row>
@@ -2379,8 +2394,8 @@
         <v>9</v>
       </c>
       <c r="L24" s="14"/>
-      <c r="M24" s="44"/>
-      <c r="N24" s="45"/>
+      <c r="M24" s="45"/>
+      <c r="N24" s="46"/>
       <c r="O24" s="13"/>
       <c r="P24" s="3"/>
     </row>

</xml_diff>

<commit_message>
Updated May 2016 Bill
</commit_message>
<xml_diff>
--- a/ATT_Bill.xlsx
+++ b/ATT_Bill.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="34">
   <si>
     <t>ATT Family Plan Bill Details</t>
   </si>
@@ -129,6 +129,11 @@
   </si>
   <si>
     <t>ATT discount claimed for incorrect billing in 2015.</t>
+  </si>
+  <si>
+    <t>Balaji Contract - $25 extra
+Giri India Calling - $15 extra
+Sundar roaming - $15 extra</t>
   </si>
 </sst>
 </file>
@@ -343,7 +348,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -395,9 +400,6 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -417,9 +419,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -432,6 +431,15 @@
     <xf numFmtId="44" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -460,12 +468,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -499,10 +501,10 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -790,8 +792,8 @@
   <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M25" sqref="M25"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,19 +813,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
+      <c r="A1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -893,16 +895,16 @@
       <c r="F3" s="11">
         <v>53.44</v>
       </c>
-      <c r="G3" s="38">
-        <v>0</v>
-      </c>
-      <c r="H3" s="38">
-        <v>0</v>
-      </c>
-      <c r="I3" s="38">
-        <v>0</v>
-      </c>
-      <c r="J3" s="38">
+      <c r="G3" s="39">
+        <v>0</v>
+      </c>
+      <c r="H3" s="39">
+        <v>0</v>
+      </c>
+      <c r="I3" s="39">
+        <v>0</v>
+      </c>
+      <c r="J3" s="39">
         <v>0</v>
       </c>
       <c r="K3" s="2"/>
@@ -940,10 +942,10 @@
       <c r="F4" s="11">
         <v>38.54</v>
       </c>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
       <c r="K4" s="2"/>
       <c r="L4" s="1"/>
       <c r="M4" s="2" t="s">
@@ -953,11 +955,11 @@
         <f>SUM(C3:C15)</f>
         <v>482.77999999999992</v>
       </c>
-      <c r="O4" s="38">
+      <c r="O4" s="39">
         <f>200+490.45</f>
         <v>690.45</v>
       </c>
-      <c r="P4" s="40">
+      <c r="P4" s="41">
         <f>N4+N5-O4</f>
         <v>-207.67000000000013</v>
       </c>
@@ -982,10 +984,10 @@
       <c r="F5" s="11">
         <v>38.229999999999997</v>
       </c>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
       <c r="K5" s="2"/>
       <c r="L5" s="1"/>
       <c r="M5" s="2" t="s">
@@ -995,8 +997,8 @@
         <f>SUM(J3:J15)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="39"/>
-      <c r="P5" s="41"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="42"/>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1018,10 +1020,10 @@
       <c r="F6" s="11">
         <v>38.54</v>
       </c>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
       <c r="K6" s="2"/>
       <c r="L6" s="1"/>
       <c r="M6" s="2" t="s">
@@ -1035,7 +1037,7 @@
         <f>368+80</f>
         <v>448</v>
       </c>
-      <c r="P6" s="19">
+      <c r="P6" s="32">
         <f t="shared" ref="P6:P11" si="0">N6-O6</f>
         <v>31.259999999999934</v>
       </c>
@@ -1060,10 +1062,10 @@
       <c r="F7" s="11">
         <v>38.69</v>
       </c>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
       <c r="K7" s="2"/>
       <c r="L7" s="1"/>
       <c r="M7" s="2" t="s">
@@ -1073,10 +1075,10 @@
         <f>SUM(F3:F15)</f>
         <v>491.13999999999993</v>
       </c>
-      <c r="O7" s="38">
+      <c r="O7" s="39">
         <v>1024.28</v>
       </c>
-      <c r="P7" s="40">
+      <c r="P7" s="41">
         <f>N7+N8-O7</f>
         <v>0</v>
       </c>
@@ -1101,10 +1103,10 @@
       <c r="F8" s="11">
         <v>39.799999999999997</v>
       </c>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
       <c r="K8" s="2"/>
       <c r="L8" s="1"/>
       <c r="M8" s="2" t="s">
@@ -1114,8 +1116,8 @@
         <f>SUM(E3:E14)</f>
         <v>533.14</v>
       </c>
-      <c r="O8" s="39"/>
-      <c r="P8" s="41"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="42"/>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1137,10 +1139,10 @@
       <c r="F9" s="11">
         <v>38.69</v>
       </c>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
       <c r="K9" s="2"/>
       <c r="L9" s="1"/>
       <c r="M9" s="2" t="s">
@@ -1150,11 +1152,11 @@
         <f>SUM(G3:G15)</f>
         <v>175.34</v>
       </c>
-      <c r="O9" s="38">
+      <c r="O9" s="39">
         <f>113.35+61.99+51.99</f>
         <v>227.33</v>
       </c>
-      <c r="P9" s="42">
+      <c r="P9" s="41">
         <f>N9+N10-O9</f>
         <v>0</v>
       </c>
@@ -1180,10 +1182,10 @@
       <c r="F10" s="11">
         <v>39.14</v>
       </c>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
       <c r="K10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1195,8 +1197,8 @@
         <f>SUM(I3:I15)</f>
         <v>51.99</v>
       </c>
-      <c r="O10" s="39"/>
-      <c r="P10" s="43"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="42"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
@@ -1219,10 +1221,10 @@
       <c r="F11" s="11">
         <v>38.92</v>
       </c>
-      <c r="G11" s="39"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
       <c r="K11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1237,7 +1239,7 @@
       <c r="O11" s="11">
         <v>0</v>
       </c>
-      <c r="P11" s="19">
+      <c r="P11" s="32">
         <f t="shared" si="0"/>
         <v>106.63</v>
       </c>
@@ -1266,9 +1268,9 @@
       <c r="G12" s="11">
         <v>52.78</v>
       </c>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
       <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1302,9 +1304,9 @@
       <c r="G13" s="11">
         <v>60.57</v>
       </c>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="44"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="43"/>
       <c r="K13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1350,7 +1352,7 @@
         <f>36.99+15</f>
         <v>51.99</v>
       </c>
-      <c r="J14" s="39"/>
+      <c r="J14" s="40"/>
       <c r="K14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1401,14 +1403,14 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="34" t="s">
+      <c r="M15" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="37"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -1429,10 +1431,10 @@
       <c r="N16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O16" s="37" t="s">
+      <c r="O16" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="P16" s="37"/>
+      <c r="P16" s="38"/>
       <c r="Q16" s="10" t="s">
         <v>23</v>
       </c>
@@ -1459,10 +1461,10 @@
       <c r="N17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O17" s="32">
+      <c r="O17" s="33">
         <v>42053</v>
       </c>
-      <c r="P17" s="32"/>
+      <c r="P17" s="33"/>
       <c r="Q17" s="13">
         <v>108</v>
       </c>
@@ -1488,10 +1490,10 @@
       <c r="N18" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O18" s="32">
+      <c r="O18" s="33">
         <v>42086</v>
       </c>
-      <c r="P18" s="32"/>
+      <c r="P18" s="33"/>
       <c r="Q18" s="13">
         <v>200</v>
       </c>
@@ -1517,10 +1519,10 @@
       <c r="N19" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O19" s="32">
+      <c r="O19" s="33">
         <v>42111</v>
       </c>
-      <c r="P19" s="32"/>
+      <c r="P19" s="33"/>
       <c r="Q19" s="13">
         <v>100</v>
       </c>
@@ -1545,10 +1547,10 @@
       <c r="N20" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O20" s="32">
+      <c r="O20" s="33">
         <v>42214</v>
       </c>
-      <c r="P20" s="32"/>
+      <c r="P20" s="33"/>
       <c r="Q20" s="13">
         <v>160</v>
       </c>
@@ -1567,10 +1569,10 @@
       <c r="N21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O21" s="32">
+      <c r="O21" s="33">
         <v>42325</v>
       </c>
-      <c r="P21" s="32"/>
+      <c r="P21" s="33"/>
       <c r="Q21" s="13">
         <v>113.35</v>
       </c>
@@ -1589,10 +1591,10 @@
       <c r="N22" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O22" s="32">
+      <c r="O22" s="33">
         <v>42325</v>
       </c>
-      <c r="P22" s="32"/>
+      <c r="P22" s="33"/>
       <c r="Q22" s="13">
         <v>80</v>
       </c>
@@ -1610,10 +1612,10 @@
       <c r="N23" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O23" s="32">
+      <c r="O23" s="33">
         <v>42341</v>
       </c>
-      <c r="P23" s="32"/>
+      <c r="P23" s="33"/>
       <c r="Q23" s="13">
         <v>490.45</v>
       </c>
@@ -1629,10 +1631,10 @@
       <c r="N24" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O24" s="32">
+      <c r="O24" s="33">
         <v>42364</v>
       </c>
-      <c r="P24" s="32"/>
+      <c r="P24" s="33"/>
       <c r="Q24" s="13">
         <v>113.98</v>
       </c>
@@ -1644,8 +1646,8 @@
       <c r="G25" s="1"/>
       <c r="M25" s="3"/>
       <c r="N25" s="14"/>
-      <c r="O25" s="32"/>
-      <c r="P25" s="32"/>
+      <c r="O25" s="33"/>
+      <c r="P25" s="33"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="3"/>
     </row>
@@ -1700,7 +1702,7 @@
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="L3" sqref="L3:P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1723,18 +1725,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
+      <c r="A1" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1743,34 +1745,34 @@
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="19" t="s">
         <v>10</v>
       </c>
       <c r="K2" s="1"/>
@@ -1785,34 +1787,34 @@
       <c r="A3" s="5">
         <v>42384</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="21">
         <v>45.96</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="30">
         <f>B3/6</f>
         <v>7.66</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="30">
         <f>B3/6</f>
         <v>7.66</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="30">
         <f>B3/6</f>
         <v>7.66</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="30">
         <f>B3/6</f>
         <v>7.66</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="30">
         <f>B3/6</f>
         <v>7.66</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="30">
         <f>B3/6</f>
         <v>7.66</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="30">
         <v>0</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -1840,32 +1842,32 @@
       <c r="A4" s="5">
         <v>42415</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="22">
         <v>263.16000000000003</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="22">
         <v>31.88</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <f>31.88</f>
         <v>31.88</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="22">
         <v>31.88</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="22">
         <f>31.88+15</f>
         <v>46.879999999999995</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="23">
         <f>31.88+25</f>
         <v>56.879999999999995</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="23">
         <f>31.88</f>
         <v>31.88</v>
       </c>
-      <c r="I4" s="24">
+      <c r="I4" s="23">
         <f>31.88</f>
         <v>31.88</v>
       </c>
@@ -1878,16 +1880,16 @@
       </c>
       <c r="M4" s="4">
         <f>SUM(C3:C14)</f>
-        <v>107.2</v>
-      </c>
-      <c r="N4" s="56">
+        <v>150.65</v>
+      </c>
+      <c r="N4" s="55">
         <v>207.67</v>
       </c>
-      <c r="O4" s="53">
+      <c r="O4" s="52">
         <f>SUM(M4:M5)-N4+P4</f>
-        <v>-60.929999999999978</v>
-      </c>
-      <c r="P4" s="45">
+        <v>-17.47999999999999</v>
+      </c>
+      <c r="P4" s="44">
         <v>0</v>
       </c>
       <c r="Q4" s="1"/>
@@ -1896,30 +1898,30 @@
       <c r="A5" s="5">
         <v>42444</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="21">
         <v>242.97</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="21">
         <v>33.83</v>
       </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="22">
+      <c r="D5" s="30">
+        <v>0</v>
+      </c>
+      <c r="E5" s="21">
         <v>33.83</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="21">
         <f>33.83+15</f>
         <v>48.83</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="30">
         <f>33.83+25</f>
         <v>58.83</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="30">
         <v>33.83</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="30">
         <v>33.83</v>
       </c>
       <c r="J5" s="2" t="s">
@@ -1933,39 +1935,39 @@
         <f>SUM(D3:D14)</f>
         <v>39.54</v>
       </c>
-      <c r="N5" s="56"/>
-      <c r="O5" s="53"/>
-      <c r="P5" s="46"/>
+      <c r="N5" s="55"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="45"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>42475</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="21">
         <v>242.97</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="21">
         <v>33.83</v>
       </c>
-      <c r="D6" s="27">
-        <v>0</v>
-      </c>
-      <c r="E6" s="22">
+      <c r="D6" s="30">
+        <v>0</v>
+      </c>
+      <c r="E6" s="21">
         <v>33.83</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="21">
         <f>33.83+15</f>
         <v>48.83</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="30">
         <f>33.83+25</f>
         <v>58.83</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="30">
         <v>33.83</v>
       </c>
-      <c r="I6" s="27">
+      <c r="I6" s="30">
         <v>33.83</v>
       </c>
       <c r="J6" s="2" t="s">
@@ -1977,49 +1979,72 @@
       </c>
       <c r="M6" s="4">
         <f>SUM(E3:E14)</f>
-        <v>107.2</v>
+        <v>135.65</v>
       </c>
       <c r="N6" s="4">
-        <v>120</v>
-      </c>
-      <c r="O6" s="28">
+        <f>SUM(O16,O18,O21)</f>
+        <v>220</v>
+      </c>
+      <c r="O6" s="31">
         <f>M6-N6+P6</f>
-        <v>18.460000000000004</v>
-      </c>
-      <c r="P6" s="30">
+        <v>-53.089999999999989</v>
+      </c>
+      <c r="P6" s="28">
         <v>31.26</v>
       </c>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>42505</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="2"/>
+      <c r="B7" s="21">
+        <v>225.68</v>
+      </c>
+      <c r="C7" s="21">
+        <f>28.45+15</f>
+        <v>43.45</v>
+      </c>
+      <c r="D7" s="30">
+        <v>0</v>
+      </c>
+      <c r="E7" s="21">
+        <v>28.45</v>
+      </c>
+      <c r="F7" s="21">
+        <f>28.45+15</f>
+        <v>43.45</v>
+      </c>
+      <c r="G7" s="30">
+        <f>28.45+25</f>
+        <v>53.45</v>
+      </c>
+      <c r="H7" s="30">
+        <f>28.45</f>
+        <v>28.45</v>
+      </c>
+      <c r="I7" s="30">
+        <v>28.45</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="L7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="M7" s="4">
         <f>SUM(F3:F14)</f>
-        <v>152.19999999999999</v>
+        <v>195.64999999999998</v>
       </c>
       <c r="N7" s="4">
-        <v>152.19999999999999</v>
-      </c>
-      <c r="O7" s="29">
+        <v>195.65</v>
+      </c>
+      <c r="O7" s="27">
         <f>M7-N7</f>
         <v>0</v>
       </c>
-      <c r="P7" s="30">
+      <c r="P7" s="28">
         <v>0</v>
       </c>
       <c r="Q7" s="1"/>
@@ -2028,14 +2053,14 @@
       <c r="A8" s="5">
         <v>42536</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
       <c r="J8" s="2"/>
       <c r="K8" s="1"/>
       <c r="L8" s="2" t="s">
@@ -2043,17 +2068,17 @@
       </c>
       <c r="M8" s="4">
         <f>SUM(G3:G14)</f>
-        <v>182.2</v>
-      </c>
-      <c r="N8" s="54">
-        <f>104.08+92.66</f>
-        <v>196.74</v>
-      </c>
-      <c r="O8" s="57">
+        <v>235.64999999999998</v>
+      </c>
+      <c r="N8" s="53">
+        <f>SUM(O17,O19:O20)</f>
+        <v>289.39999999999998</v>
+      </c>
+      <c r="O8" s="56">
         <f>M8+M9-N8</f>
-        <v>92.659999999999968</v>
-      </c>
-      <c r="P8" s="47">
+        <v>81.899999999999977</v>
+      </c>
+      <c r="P8" s="46">
         <v>0</v>
       </c>
       <c r="Q8" s="1"/>
@@ -2062,14 +2087,14 @@
       <c r="A9" s="5">
         <v>42566</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
       <c r="J9" s="2"/>
       <c r="K9" s="1"/>
       <c r="L9" s="2" t="s">
@@ -2077,25 +2102,25 @@
       </c>
       <c r="M9" s="4">
         <f>SUM(H3:H14)</f>
-        <v>107.2</v>
-      </c>
-      <c r="N9" s="55"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="48"/>
+        <v>135.65</v>
+      </c>
+      <c r="N9" s="54"/>
+      <c r="O9" s="57"/>
+      <c r="P9" s="47"/>
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>42597</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
       <c r="J10" s="2"/>
       <c r="K10" s="1"/>
       <c r="L10" s="2" t="s">
@@ -2103,16 +2128,16 @@
       </c>
       <c r="M10" s="4">
         <f>SUM(I3:I14)</f>
-        <v>99.539999999999992</v>
+        <v>127.99</v>
       </c>
       <c r="N10" s="4">
         <v>138.51</v>
       </c>
-      <c r="O10" s="28">
+      <c r="O10" s="26">
         <f>M10-N10+P10</f>
-        <v>67.66</v>
-      </c>
-      <c r="P10" s="31">
+        <v>96.11</v>
+      </c>
+      <c r="P10" s="29">
         <v>106.63</v>
       </c>
       <c r="Q10" s="1"/>
@@ -2121,14 +2146,14 @@
       <c r="A11" s="5">
         <v>42628</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
       <c r="J11" s="2"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -2142,14 +2167,14 @@
       <c r="A12" s="5">
         <v>42658</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
       <c r="J12" s="2"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1" t="s">
@@ -2165,14 +2190,14 @@
       <c r="A13" s="5">
         <v>42689</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
       <c r="J13" s="2"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -2186,23 +2211,23 @@
       <c r="A14" s="5">
         <v>42719</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="34" t="s">
+      <c r="K14" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="37"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -2215,20 +2240,20 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="21" t="s">
+      <c r="K15" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="21" t="s">
+      <c r="L15" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="34" t="s">
+      <c r="M15" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="N15" s="36"/>
-      <c r="O15" s="21" t="s">
+      <c r="N15" s="37"/>
+      <c r="O15" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="P15" s="21" t="s">
+      <c r="P15" s="20" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2249,11 +2274,11 @@
       <c r="L16" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="M16" s="49">
+      <c r="M16" s="48">
         <v>42401</v>
       </c>
-      <c r="N16" s="50"/>
-      <c r="O16" s="25">
+      <c r="N16" s="49"/>
+      <c r="O16" s="24">
         <v>100</v>
       </c>
       <c r="P16" s="3" t="s">
@@ -2263,9 +2288,9 @@
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="C17" s="8"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="8"/>
       <c r="F17" s="1"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
@@ -2276,11 +2301,11 @@
       <c r="L17" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="49">
+      <c r="M17" s="48">
         <v>42402</v>
       </c>
-      <c r="N17" s="50"/>
-      <c r="O17" s="25">
+      <c r="N17" s="49"/>
+      <c r="O17" s="24">
         <v>104.08</v>
       </c>
       <c r="P17" s="3" t="s">
@@ -2303,11 +2328,11 @@
       <c r="L18" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="M18" s="49">
+      <c r="M18" s="48">
         <v>42433</v>
       </c>
-      <c r="N18" s="50"/>
-      <c r="O18" s="25">
+      <c r="N18" s="49"/>
+      <c r="O18" s="24">
         <v>20</v>
       </c>
       <c r="P18" s="3" t="s">
@@ -2319,7 +2344,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="26"/>
+      <c r="E19" s="25"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="J19" s="1"/>
@@ -2329,11 +2354,11 @@
       <c r="L19" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M19" s="49">
+      <c r="M19" s="48">
         <v>42433</v>
       </c>
-      <c r="N19" s="50"/>
-      <c r="O19" s="25">
+      <c r="N19" s="49"/>
+      <c r="O19" s="24">
         <v>92.66</v>
       </c>
       <c r="P19" s="3" t="s">
@@ -2350,11 +2375,11 @@
       <c r="L20" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="49">
+      <c r="M20" s="48">
         <v>42465</v>
       </c>
-      <c r="N20" s="50"/>
-      <c r="O20" s="25">
+      <c r="N20" s="49"/>
+      <c r="O20" s="24">
         <v>92.66</v>
       </c>
       <c r="P20" s="3" t="s">
@@ -2368,11 +2393,19 @@
       <c r="K21" s="3">
         <v>6</v>
       </c>
-      <c r="L21" s="14"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="50"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="3"/>
+      <c r="L21" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="M21" s="48">
+        <v>42493</v>
+      </c>
+      <c r="N21" s="49"/>
+      <c r="O21" s="24">
+        <v>100</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
@@ -2382,9 +2415,9 @@
         <v>7</v>
       </c>
       <c r="L22" s="14"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="50"/>
-      <c r="O22" s="13"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="49"/>
+      <c r="O22" s="24"/>
       <c r="P22" s="3"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -2393,9 +2426,9 @@
         <v>8</v>
       </c>
       <c r="L23" s="14"/>
-      <c r="M23" s="49"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="13"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="24"/>
       <c r="P23" s="3"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -2404,9 +2437,9 @@
         <v>9</v>
       </c>
       <c r="L24" s="14"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="50"/>
-      <c r="O24" s="13"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="49"/>
+      <c r="O24" s="24"/>
       <c r="P24" s="3"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated June 2016 Bill
</commit_message>
<xml_diff>
--- a/ATT_Bill.xlsx
+++ b/ATT_Bill.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="35">
   <si>
     <t>ATT Family Plan Bill Details</t>
   </si>
@@ -134,6 +134,10 @@
     <t>Balaji Contract - $25 extra
 Giri India Calling - $15 extra
 Sundar roaming - $15 extra</t>
+  </si>
+  <si>
+    <t>Balaji Contract - $25 extra
+Giri India Calling and Roaming - $79 extra</t>
   </si>
 </sst>
 </file>
@@ -348,7 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -440,6 +444,24 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -458,53 +480,38 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="6" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="5" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -813,19 +820,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
+      <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -895,16 +902,16 @@
       <c r="F3" s="11">
         <v>53.44</v>
       </c>
-      <c r="G3" s="39">
-        <v>0</v>
-      </c>
-      <c r="H3" s="39">
-        <v>0</v>
-      </c>
-      <c r="I3" s="39">
-        <v>0</v>
-      </c>
-      <c r="J3" s="39">
+      <c r="G3" s="34">
+        <v>0</v>
+      </c>
+      <c r="H3" s="34">
+        <v>0</v>
+      </c>
+      <c r="I3" s="34">
+        <v>0</v>
+      </c>
+      <c r="J3" s="34">
         <v>0</v>
       </c>
       <c r="K3" s="2"/>
@@ -942,10 +949,10 @@
       <c r="F4" s="11">
         <v>38.54</v>
       </c>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
       <c r="K4" s="2"/>
       <c r="L4" s="1"/>
       <c r="M4" s="2" t="s">
@@ -955,11 +962,11 @@
         <f>SUM(C3:C15)</f>
         <v>482.77999999999992</v>
       </c>
-      <c r="O4" s="39">
+      <c r="O4" s="34">
         <f>200+490.45</f>
         <v>690.45</v>
       </c>
-      <c r="P4" s="41">
+      <c r="P4" s="37">
         <f>N4+N5-O4</f>
         <v>-207.67000000000013</v>
       </c>
@@ -984,10 +991,10 @@
       <c r="F5" s="11">
         <v>38.229999999999997</v>
       </c>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
       <c r="K5" s="2"/>
       <c r="L5" s="1"/>
       <c r="M5" s="2" t="s">
@@ -997,8 +1004,8 @@
         <f>SUM(J3:J15)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="40"/>
-      <c r="P5" s="42"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="38"/>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1020,10 +1027,10 @@
       <c r="F6" s="11">
         <v>38.54</v>
       </c>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
       <c r="K6" s="2"/>
       <c r="L6" s="1"/>
       <c r="M6" s="2" t="s">
@@ -1062,10 +1069,10 @@
       <c r="F7" s="11">
         <v>38.69</v>
       </c>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
       <c r="K7" s="2"/>
       <c r="L7" s="1"/>
       <c r="M7" s="2" t="s">
@@ -1075,10 +1082,10 @@
         <f>SUM(F3:F15)</f>
         <v>491.13999999999993</v>
       </c>
-      <c r="O7" s="39">
+      <c r="O7" s="34">
         <v>1024.28</v>
       </c>
-      <c r="P7" s="41">
+      <c r="P7" s="37">
         <f>N7+N8-O7</f>
         <v>0</v>
       </c>
@@ -1103,10 +1110,10 @@
       <c r="F8" s="11">
         <v>39.799999999999997</v>
       </c>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
       <c r="K8" s="2"/>
       <c r="L8" s="1"/>
       <c r="M8" s="2" t="s">
@@ -1116,8 +1123,8 @@
         <f>SUM(E3:E14)</f>
         <v>533.14</v>
       </c>
-      <c r="O8" s="40"/>
-      <c r="P8" s="42"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="38"/>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1139,10 +1146,10 @@
       <c r="F9" s="11">
         <v>38.69</v>
       </c>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
       <c r="K9" s="2"/>
       <c r="L9" s="1"/>
       <c r="M9" s="2" t="s">
@@ -1152,11 +1159,11 @@
         <f>SUM(G3:G15)</f>
         <v>175.34</v>
       </c>
-      <c r="O9" s="39">
+      <c r="O9" s="34">
         <f>113.35+61.99+51.99</f>
         <v>227.33</v>
       </c>
-      <c r="P9" s="41">
+      <c r="P9" s="37">
         <f>N9+N10-O9</f>
         <v>0</v>
       </c>
@@ -1182,10 +1189,10 @@
       <c r="F10" s="11">
         <v>39.14</v>
       </c>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
       <c r="K10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1197,8 +1204,8 @@
         <f>SUM(I3:I15)</f>
         <v>51.99</v>
       </c>
-      <c r="O10" s="40"/>
-      <c r="P10" s="42"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="38"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
@@ -1221,10 +1228,10 @@
       <c r="F11" s="11">
         <v>38.92</v>
       </c>
-      <c r="G11" s="40"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
       <c r="K11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1268,9 +1275,9 @@
       <c r="G12" s="11">
         <v>52.78</v>
       </c>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
       <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1304,9 +1311,9 @@
       <c r="G13" s="11">
         <v>60.57</v>
       </c>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="43"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="35"/>
       <c r="K13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1352,7 +1359,7 @@
         <f>36.99+15</f>
         <v>51.99</v>
       </c>
-      <c r="J14" s="40"/>
+      <c r="J14" s="36"/>
       <c r="K14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1403,14 +1410,14 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="35" t="s">
+      <c r="M15" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="37"/>
+      <c r="N15" s="42"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="42"/>
+      <c r="R15" s="43"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -1431,10 +1438,10 @@
       <c r="N16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O16" s="38" t="s">
+      <c r="O16" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="P16" s="38"/>
+      <c r="P16" s="44"/>
       <c r="Q16" s="10" t="s">
         <v>23</v>
       </c>
@@ -1461,10 +1468,10 @@
       <c r="N17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O17" s="33">
+      <c r="O17" s="39">
         <v>42053</v>
       </c>
-      <c r="P17" s="33"/>
+      <c r="P17" s="39"/>
       <c r="Q17" s="13">
         <v>108</v>
       </c>
@@ -1490,10 +1497,10 @@
       <c r="N18" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O18" s="33">
+      <c r="O18" s="39">
         <v>42086</v>
       </c>
-      <c r="P18" s="33"/>
+      <c r="P18" s="39"/>
       <c r="Q18" s="13">
         <v>200</v>
       </c>
@@ -1519,10 +1526,10 @@
       <c r="N19" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O19" s="33">
+      <c r="O19" s="39">
         <v>42111</v>
       </c>
-      <c r="P19" s="33"/>
+      <c r="P19" s="39"/>
       <c r="Q19" s="13">
         <v>100</v>
       </c>
@@ -1547,10 +1554,10 @@
       <c r="N20" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O20" s="33">
+      <c r="O20" s="39">
         <v>42214</v>
       </c>
-      <c r="P20" s="33"/>
+      <c r="P20" s="39"/>
       <c r="Q20" s="13">
         <v>160</v>
       </c>
@@ -1569,10 +1576,10 @@
       <c r="N21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O21" s="33">
+      <c r="O21" s="39">
         <v>42325</v>
       </c>
-      <c r="P21" s="33"/>
+      <c r="P21" s="39"/>
       <c r="Q21" s="13">
         <v>113.35</v>
       </c>
@@ -1591,10 +1598,10 @@
       <c r="N22" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O22" s="33">
+      <c r="O22" s="39">
         <v>42325</v>
       </c>
-      <c r="P22" s="33"/>
+      <c r="P22" s="39"/>
       <c r="Q22" s="13">
         <v>80</v>
       </c>
@@ -1612,10 +1619,10 @@
       <c r="N23" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O23" s="33">
+      <c r="O23" s="39">
         <v>42341</v>
       </c>
-      <c r="P23" s="33"/>
+      <c r="P23" s="39"/>
       <c r="Q23" s="13">
         <v>490.45</v>
       </c>
@@ -1631,10 +1638,10 @@
       <c r="N24" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O24" s="33">
+      <c r="O24" s="39">
         <v>42364</v>
       </c>
-      <c r="P24" s="33"/>
+      <c r="P24" s="39"/>
       <c r="Q24" s="13">
         <v>113.98</v>
       </c>
@@ -1646,8 +1653,8 @@
       <c r="G25" s="1"/>
       <c r="M25" s="3"/>
       <c r="N25" s="14"/>
-      <c r="O25" s="33"/>
-      <c r="P25" s="33"/>
+      <c r="O25" s="39"/>
+      <c r="P25" s="39"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="3"/>
     </row>
@@ -1668,12 +1675,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="G3:G11"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="J3:J14"/>
-    <mergeCell ref="I3:I13"/>
-    <mergeCell ref="H3:H13"/>
     <mergeCell ref="O25:P25"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M15:R15"/>
@@ -1690,6 +1691,12 @@
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="O9:O10"/>
     <mergeCell ref="P9:P10"/>
+    <mergeCell ref="G3:G11"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="J3:J14"/>
+    <mergeCell ref="I3:I13"/>
+    <mergeCell ref="H3:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1701,8 +1708,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:P10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1711,7 +1718,7 @@
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
@@ -1725,18 +1732,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
+      <c r="A1" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1880,16 +1887,16 @@
       </c>
       <c r="M4" s="4">
         <f>SUM(C3:C14)</f>
-        <v>150.65</v>
-      </c>
-      <c r="N4" s="55">
+        <v>184.91300000000001</v>
+      </c>
+      <c r="N4" s="47">
         <v>207.67</v>
       </c>
-      <c r="O4" s="52">
+      <c r="O4" s="58">
         <f>SUM(M4:M5)-N4+P4</f>
-        <v>-17.47999999999999</v>
-      </c>
-      <c r="P4" s="44">
+        <v>16.783000000000015</v>
+      </c>
+      <c r="P4" s="48">
         <v>0</v>
       </c>
       <c r="Q4" s="1"/>
@@ -1935,9 +1942,9 @@
         <f>SUM(D3:D14)</f>
         <v>39.54</v>
       </c>
-      <c r="N5" s="55"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="45"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="49"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -1979,7 +1986,7 @@
       </c>
       <c r="M6" s="4">
         <f>SUM(E3:E14)</f>
-        <v>135.65</v>
+        <v>169.91</v>
       </c>
       <c r="N6" s="4">
         <f>SUM(O16,O18,O21)</f>
@@ -1987,7 +1994,7 @@
       </c>
       <c r="O6" s="31">
         <f>M6-N6+P6</f>
-        <v>-53.089999999999989</v>
+        <v>-18.830000000000002</v>
       </c>
       <c r="P6" s="28">
         <v>31.26</v>
@@ -2035,10 +2042,10 @@
       </c>
       <c r="M7" s="4">
         <f>SUM(F3:F14)</f>
-        <v>195.64999999999998</v>
-      </c>
-      <c r="N7" s="4">
-        <v>195.65</v>
+        <v>308.90999999999997</v>
+      </c>
+      <c r="N7" s="33">
+        <v>308.91000000000003</v>
       </c>
       <c r="O7" s="27">
         <f>M7-N7</f>
@@ -2049,36 +2056,56 @@
       </c>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>42536</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="2"/>
+      <c r="B8" s="21">
+        <v>309.58</v>
+      </c>
+      <c r="C8" s="21">
+        <v>34.262999999999998</v>
+      </c>
+      <c r="D8" s="30">
+        <v>0</v>
+      </c>
+      <c r="E8" s="21">
+        <v>34.26</v>
+      </c>
+      <c r="F8" s="21">
+        <f>34.26+79</f>
+        <v>113.25999999999999</v>
+      </c>
+      <c r="G8" s="30">
+        <f>34.26+25</f>
+        <v>59.26</v>
+      </c>
+      <c r="H8" s="30">
+        <v>34.26</v>
+      </c>
+      <c r="I8" s="30">
+        <v>34.26</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="K8" s="1"/>
       <c r="L8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="M8" s="4">
         <f>SUM(G3:G14)</f>
-        <v>235.64999999999998</v>
-      </c>
-      <c r="N8" s="53">
-        <f>SUM(O17,O19:O20)</f>
-        <v>289.39999999999998</v>
+        <v>294.90999999999997</v>
+      </c>
+      <c r="N8" s="54">
+        <f>SUM(O17,O19:O20,O22)</f>
+        <v>371.29999999999995</v>
       </c>
       <c r="O8" s="56">
         <f>M8+M9-N8</f>
-        <v>81.899999999999977</v>
-      </c>
-      <c r="P8" s="46">
+        <v>93.519999999999982</v>
+      </c>
+      <c r="P8" s="50">
         <v>0</v>
       </c>
       <c r="Q8" s="1"/>
@@ -2102,11 +2129,11 @@
       </c>
       <c r="M9" s="4">
         <f>SUM(H3:H14)</f>
-        <v>135.65</v>
-      </c>
-      <c r="N9" s="54"/>
+        <v>169.91</v>
+      </c>
+      <c r="N9" s="55"/>
       <c r="O9" s="57"/>
-      <c r="P9" s="47"/>
+      <c r="P9" s="51"/>
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -2128,14 +2155,14 @@
       </c>
       <c r="M10" s="4">
         <f>SUM(I3:I14)</f>
-        <v>127.99</v>
+        <v>162.25</v>
       </c>
       <c r="N10" s="4">
         <v>138.51</v>
       </c>
       <c r="O10" s="26">
         <f>M10-N10+P10</f>
-        <v>96.11</v>
+        <v>130.37</v>
       </c>
       <c r="P10" s="29">
         <v>106.63</v>
@@ -2220,14 +2247,14 @@
       <c r="H14" s="30"/>
       <c r="I14" s="30"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="35" t="s">
+      <c r="K14" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="37"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="42"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="43"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -2246,10 +2273,10 @@
       <c r="L15" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="35" t="s">
+      <c r="M15" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="N15" s="37"/>
+      <c r="N15" s="43"/>
       <c r="O15" s="20" t="s">
         <v>23</v>
       </c>
@@ -2274,10 +2301,10 @@
       <c r="L16" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="M16" s="48">
+      <c r="M16" s="45">
         <v>42401</v>
       </c>
-      <c r="N16" s="49"/>
+      <c r="N16" s="46"/>
       <c r="O16" s="24">
         <v>100</v>
       </c>
@@ -2301,10 +2328,10 @@
       <c r="L17" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="48">
+      <c r="M17" s="45">
         <v>42402</v>
       </c>
-      <c r="N17" s="49"/>
+      <c r="N17" s="46"/>
       <c r="O17" s="24">
         <v>104.08</v>
       </c>
@@ -2328,10 +2355,10 @@
       <c r="L18" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="M18" s="48">
+      <c r="M18" s="45">
         <v>42433</v>
       </c>
-      <c r="N18" s="49"/>
+      <c r="N18" s="46"/>
       <c r="O18" s="24">
         <v>20</v>
       </c>
@@ -2354,10 +2381,10 @@
       <c r="L19" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M19" s="48">
+      <c r="M19" s="45">
         <v>42433</v>
       </c>
-      <c r="N19" s="49"/>
+      <c r="N19" s="46"/>
       <c r="O19" s="24">
         <v>92.66</v>
       </c>
@@ -2375,10 +2402,10 @@
       <c r="L20" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="48">
+      <c r="M20" s="45">
         <v>42465</v>
       </c>
-      <c r="N20" s="49"/>
+      <c r="N20" s="46"/>
       <c r="O20" s="24">
         <v>92.66</v>
       </c>
@@ -2396,10 +2423,10 @@
       <c r="L21" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="M21" s="48">
+      <c r="M21" s="45">
         <v>42493</v>
       </c>
-      <c r="N21" s="49"/>
+      <c r="N21" s="46"/>
       <c r="O21" s="24">
         <v>100</v>
       </c>
@@ -2414,11 +2441,19 @@
       <c r="K22" s="3">
         <v>7</v>
       </c>
-      <c r="L22" s="14"/>
-      <c r="M22" s="48"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="3"/>
+      <c r="L22" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" s="45">
+        <v>42494</v>
+      </c>
+      <c r="N22" s="46"/>
+      <c r="O22" s="24">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F23" s="1"/>
@@ -2426,8 +2461,8 @@
         <v>8</v>
       </c>
       <c r="L23" s="14"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="49"/>
+      <c r="M23" s="45"/>
+      <c r="N23" s="46"/>
       <c r="O23" s="24"/>
       <c r="P23" s="3"/>
     </row>
@@ -2437,8 +2472,8 @@
         <v>9</v>
       </c>
       <c r="L24" s="14"/>
-      <c r="M24" s="48"/>
-      <c r="N24" s="49"/>
+      <c r="M24" s="45"/>
+      <c r="N24" s="46"/>
       <c r="O24" s="24"/>
       <c r="P24" s="3"/>
     </row>
@@ -2459,6 +2494,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="K14:P14"/>
     <mergeCell ref="M23:N23"/>
     <mergeCell ref="M24:N24"/>
     <mergeCell ref="N4:N5"/>
@@ -2468,15 +2512,6 @@
     <mergeCell ref="M19:N19"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="M15:N15"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="K14:P14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated July 2016 Billing
</commit_message>
<xml_diff>
--- a/ATT_Bill.xlsx
+++ b/ATT_Bill.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="37">
   <si>
     <t>ATT Family Plan Bill Details</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Sankari</t>
   </si>
   <si>
-    <t>Previous Balance</t>
-  </si>
-  <si>
     <t>Balaji Contract - $25 extra
 Giri India Calling - $15 extra</t>
   </si>
@@ -138,6 +135,16 @@
   <si>
     <t>Balaji Contract - $25 extra
 Giri India Calling and Roaming - $79 extra</t>
+  </si>
+  <si>
+    <t>Balaji Contract - $25 extra
+Giri International Calling - $67.77 extra</t>
+  </si>
+  <si>
+    <t>Deposit</t>
+  </si>
+  <si>
+    <t>Previous Balance - 2015</t>
   </si>
 </sst>
 </file>
@@ -352,7 +359,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -438,67 +445,70 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="6" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="5" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -511,7 +521,7 @@
     <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -799,8 +809,8 @@
   <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q14" sqref="Q14"/>
+      <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,19 +830,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -902,16 +912,16 @@
       <c r="F3" s="11">
         <v>53.44</v>
       </c>
-      <c r="G3" s="34">
-        <v>0</v>
-      </c>
-      <c r="H3" s="34">
-        <v>0</v>
-      </c>
-      <c r="I3" s="34">
-        <v>0</v>
-      </c>
-      <c r="J3" s="34">
+      <c r="G3" s="41">
+        <v>0</v>
+      </c>
+      <c r="H3" s="41">
+        <v>0</v>
+      </c>
+      <c r="I3" s="41">
+        <v>0</v>
+      </c>
+      <c r="J3" s="41">
         <v>0</v>
       </c>
       <c r="K3" s="2"/>
@@ -949,10 +959,10 @@
       <c r="F4" s="11">
         <v>38.54</v>
       </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="2"/>
       <c r="L4" s="1"/>
       <c r="M4" s="2" t="s">
@@ -962,11 +972,11 @@
         <f>SUM(C3:C15)</f>
         <v>482.77999999999992</v>
       </c>
-      <c r="O4" s="34">
+      <c r="O4" s="41">
         <f>200+490.45</f>
         <v>690.45</v>
       </c>
-      <c r="P4" s="37">
+      <c r="P4" s="43">
         <f>N4+N5-O4</f>
         <v>-207.67000000000013</v>
       </c>
@@ -991,10 +1001,10 @@
       <c r="F5" s="11">
         <v>38.229999999999997</v>
       </c>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
       <c r="K5" s="2"/>
       <c r="L5" s="1"/>
       <c r="M5" s="2" t="s">
@@ -1004,8 +1014,8 @@
         <f>SUM(J3:J15)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="36"/>
-      <c r="P5" s="38"/>
+      <c r="O5" s="42"/>
+      <c r="P5" s="44"/>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1027,10 +1037,10 @@
       <c r="F6" s="11">
         <v>38.54</v>
       </c>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
       <c r="K6" s="2"/>
       <c r="L6" s="1"/>
       <c r="M6" s="2" t="s">
@@ -1044,7 +1054,7 @@
         <f>368+80</f>
         <v>448</v>
       </c>
-      <c r="P6" s="32">
+      <c r="P6" s="31">
         <f t="shared" ref="P6:P11" si="0">N6-O6</f>
         <v>31.259999999999934</v>
       </c>
@@ -1069,10 +1079,10 @@
       <c r="F7" s="11">
         <v>38.69</v>
       </c>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
       <c r="K7" s="2"/>
       <c r="L7" s="1"/>
       <c r="M7" s="2" t="s">
@@ -1082,10 +1092,10 @@
         <f>SUM(F3:F15)</f>
         <v>491.13999999999993</v>
       </c>
-      <c r="O7" s="34">
+      <c r="O7" s="41">
         <v>1024.28</v>
       </c>
-      <c r="P7" s="37">
+      <c r="P7" s="43">
         <f>N7+N8-O7</f>
         <v>0</v>
       </c>
@@ -1110,10 +1120,10 @@
       <c r="F8" s="11">
         <v>39.799999999999997</v>
       </c>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
       <c r="K8" s="2"/>
       <c r="L8" s="1"/>
       <c r="M8" s="2" t="s">
@@ -1123,8 +1133,8 @@
         <f>SUM(E3:E14)</f>
         <v>533.14</v>
       </c>
-      <c r="O8" s="36"/>
-      <c r="P8" s="38"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="44"/>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1146,10 +1156,10 @@
       <c r="F9" s="11">
         <v>38.69</v>
       </c>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
       <c r="K9" s="2"/>
       <c r="L9" s="1"/>
       <c r="M9" s="2" t="s">
@@ -1159,11 +1169,11 @@
         <f>SUM(G3:G15)</f>
         <v>175.34</v>
       </c>
-      <c r="O9" s="34">
+      <c r="O9" s="41">
         <f>113.35+61.99+51.99</f>
         <v>227.33</v>
       </c>
-      <c r="P9" s="37">
+      <c r="P9" s="43">
         <f>N9+N10-O9</f>
         <v>0</v>
       </c>
@@ -1189,10 +1199,10 @@
       <c r="F10" s="11">
         <v>39.14</v>
       </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
       <c r="K10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1204,8 +1214,8 @@
         <f>SUM(I3:I15)</f>
         <v>51.99</v>
       </c>
-      <c r="O10" s="36"/>
-      <c r="P10" s="38"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="44"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
@@ -1228,10 +1238,10 @@
       <c r="F11" s="11">
         <v>38.92</v>
       </c>
-      <c r="G11" s="36"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
       <c r="K11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1246,7 +1256,7 @@
       <c r="O11" s="11">
         <v>0</v>
       </c>
-      <c r="P11" s="32">
+      <c r="P11" s="31">
         <f t="shared" si="0"/>
         <v>106.63</v>
       </c>
@@ -1275,9 +1285,9 @@
       <c r="G12" s="11">
         <v>52.78</v>
       </c>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
       <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1311,9 +1321,9 @@
       <c r="G13" s="11">
         <v>60.57</v>
       </c>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="35"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="45"/>
       <c r="K13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1359,7 +1369,7 @@
         <f>36.99+15</f>
         <v>51.99</v>
       </c>
-      <c r="J14" s="36"/>
+      <c r="J14" s="42"/>
       <c r="K14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1410,14 +1420,14 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="41" t="s">
+      <c r="M15" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="42"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="43"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="39"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -1438,10 +1448,10 @@
       <c r="N16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O16" s="44" t="s">
+      <c r="O16" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="P16" s="44"/>
+      <c r="P16" s="40"/>
       <c r="Q16" s="10" t="s">
         <v>23</v>
       </c>
@@ -1468,10 +1478,10 @@
       <c r="N17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O17" s="39">
+      <c r="O17" s="35">
         <v>42053</v>
       </c>
-      <c r="P17" s="39"/>
+      <c r="P17" s="35"/>
       <c r="Q17" s="13">
         <v>108</v>
       </c>
@@ -1497,10 +1507,10 @@
       <c r="N18" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O18" s="39">
+      <c r="O18" s="35">
         <v>42086</v>
       </c>
-      <c r="P18" s="39"/>
+      <c r="P18" s="35"/>
       <c r="Q18" s="13">
         <v>200</v>
       </c>
@@ -1526,10 +1536,10 @@
       <c r="N19" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O19" s="39">
+      <c r="O19" s="35">
         <v>42111</v>
       </c>
-      <c r="P19" s="39"/>
+      <c r="P19" s="35"/>
       <c r="Q19" s="13">
         <v>100</v>
       </c>
@@ -1554,10 +1564,10 @@
       <c r="N20" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O20" s="39">
+      <c r="O20" s="35">
         <v>42214</v>
       </c>
-      <c r="P20" s="39"/>
+      <c r="P20" s="35"/>
       <c r="Q20" s="13">
         <v>160</v>
       </c>
@@ -1576,10 +1586,10 @@
       <c r="N21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O21" s="39">
+      <c r="O21" s="35">
         <v>42325</v>
       </c>
-      <c r="P21" s="39"/>
+      <c r="P21" s="35"/>
       <c r="Q21" s="13">
         <v>113.35</v>
       </c>
@@ -1598,10 +1608,10 @@
       <c r="N22" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O22" s="39">
+      <c r="O22" s="35">
         <v>42325</v>
       </c>
-      <c r="P22" s="39"/>
+      <c r="P22" s="35"/>
       <c r="Q22" s="13">
         <v>80</v>
       </c>
@@ -1619,10 +1629,10 @@
       <c r="N23" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O23" s="39">
+      <c r="O23" s="35">
         <v>42341</v>
       </c>
-      <c r="P23" s="39"/>
+      <c r="P23" s="35"/>
       <c r="Q23" s="13">
         <v>490.45</v>
       </c>
@@ -1638,10 +1648,10 @@
       <c r="N24" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O24" s="39">
+      <c r="O24" s="35">
         <v>42364</v>
       </c>
-      <c r="P24" s="39"/>
+      <c r="P24" s="35"/>
       <c r="Q24" s="13">
         <v>113.98</v>
       </c>
@@ -1653,8 +1663,8 @@
       <c r="G25" s="1"/>
       <c r="M25" s="3"/>
       <c r="N25" s="14"/>
-      <c r="O25" s="39"/>
-      <c r="P25" s="39"/>
+      <c r="O25" s="35"/>
+      <c r="P25" s="35"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="3"/>
     </row>
@@ -1675,6 +1685,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="G3:G11"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="J3:J14"/>
+    <mergeCell ref="I3:I13"/>
+    <mergeCell ref="H3:H13"/>
     <mergeCell ref="O25:P25"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M15:R15"/>
@@ -1691,12 +1707,6 @@
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="O9:O10"/>
     <mergeCell ref="P9:P10"/>
-    <mergeCell ref="G3:G11"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="J3:J14"/>
-    <mergeCell ref="I3:I13"/>
-    <mergeCell ref="H3:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1708,8 +1718,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4:P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,7 +1800,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>42384</v>
       </c>
@@ -1825,7 +1835,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="6" t="s">
@@ -1841,7 +1851,7 @@
         <v>14</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="Q3" s="1"/>
     </row>
@@ -1879,7 +1889,7 @@
         <v>31.88</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="2" t="s">
@@ -1887,16 +1897,16 @@
       </c>
       <c r="M4" s="4">
         <f>SUM(C3:C14)</f>
-        <v>184.91300000000001</v>
-      </c>
-      <c r="N4" s="47">
+        <v>217.96300000000002</v>
+      </c>
+      <c r="N4" s="59">
         <v>207.67</v>
       </c>
-      <c r="O4" s="58">
+      <c r="O4" s="54">
         <f>SUM(M4:M5)-N4+P4</f>
-        <v>16.783000000000015</v>
-      </c>
-      <c r="P4" s="48">
+        <v>49.833000000000055</v>
+      </c>
+      <c r="P4" s="46">
         <v>0</v>
       </c>
       <c r="Q4" s="1"/>
@@ -1932,7 +1942,7 @@
         <v>33.83</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="2" t="s">
@@ -1942,9 +1952,9 @@
         <f>SUM(D3:D14)</f>
         <v>39.54</v>
       </c>
-      <c r="N5" s="47"/>
-      <c r="O5" s="58"/>
-      <c r="P5" s="49"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="47"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -1978,7 +1988,7 @@
         <v>33.83</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="2" t="s">
@@ -1986,15 +1996,15 @@
       </c>
       <c r="M6" s="4">
         <f>SUM(E3:E14)</f>
-        <v>169.91</v>
+        <v>202.95999999999998</v>
       </c>
       <c r="N6" s="4">
-        <f>SUM(O16,O18,O21)</f>
+        <f>SUM(O16,O19,O22)</f>
         <v>220</v>
       </c>
-      <c r="O6" s="31">
+      <c r="O6" s="34">
         <f>M6-N6+P6</f>
-        <v>-18.830000000000002</v>
+        <v>14.219999999999981</v>
       </c>
       <c r="P6" s="28">
         <v>31.26</v>
@@ -2034,7 +2044,7 @@
         <v>28.45</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="2" t="s">
@@ -2042,10 +2052,10 @@
       </c>
       <c r="M7" s="4">
         <f>SUM(F3:F14)</f>
-        <v>308.90999999999997</v>
-      </c>
-      <c r="N7" s="33">
-        <v>308.91000000000003</v>
+        <v>409.72999999999996</v>
+      </c>
+      <c r="N7" s="32">
+        <v>409.73</v>
       </c>
       <c r="O7" s="27">
         <f>M7-N7</f>
@@ -2087,7 +2097,7 @@
         <v>34.26</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="2" t="s">
@@ -2095,45 +2105,65 @@
       </c>
       <c r="M8" s="4">
         <f>SUM(G3:G14)</f>
-        <v>294.90999999999997</v>
-      </c>
-      <c r="N8" s="54">
-        <f>SUM(O17,O19:O20,O22)</f>
-        <v>371.29999999999995</v>
-      </c>
-      <c r="O8" s="56">
+        <v>352.96</v>
+      </c>
+      <c r="N8" s="55">
+        <f>SUM(O17,O20:O21,O23:O24)</f>
+        <v>464.81999999999994</v>
+      </c>
+      <c r="O8" s="57">
         <f>M8+M9-N8</f>
-        <v>93.519999999999982</v>
-      </c>
-      <c r="P8" s="50">
+        <v>91.100000000000023</v>
+      </c>
+      <c r="P8" s="48">
         <v>0</v>
       </c>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>42566</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="2"/>
+      <c r="B9" s="21">
+        <v>291.07</v>
+      </c>
+      <c r="C9" s="21">
+        <v>33.049999999999997</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0</v>
+      </c>
+      <c r="E9" s="21">
+        <v>33.049999999999997</v>
+      </c>
+      <c r="F9" s="21">
+        <f>33.05+67.77</f>
+        <v>100.82</v>
+      </c>
+      <c r="G9" s="30">
+        <f>33.05+25</f>
+        <v>58.05</v>
+      </c>
+      <c r="H9" s="30">
+        <v>33.049999999999997</v>
+      </c>
+      <c r="I9" s="30">
+        <v>33.049999999999997</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="K9" s="1"/>
       <c r="L9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="M9" s="4">
         <f>SUM(H3:H14)</f>
-        <v>169.91</v>
-      </c>
-      <c r="N9" s="55"/>
-      <c r="O9" s="57"/>
-      <c r="P9" s="51"/>
+        <v>202.95999999999998</v>
+      </c>
+      <c r="N9" s="56"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="49"/>
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -2155,14 +2185,14 @@
       </c>
       <c r="M10" s="4">
         <f>SUM(I3:I14)</f>
-        <v>162.25</v>
+        <v>195.3</v>
       </c>
       <c r="N10" s="4">
         <v>138.51</v>
       </c>
       <c r="O10" s="26">
         <f>M10-N10+P10</f>
-        <v>130.37</v>
+        <v>163.42000000000002</v>
       </c>
       <c r="P10" s="29">
         <v>106.63</v>
@@ -2247,14 +2277,14 @@
       <c r="H14" s="30"/>
       <c r="I14" s="30"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="41" t="s">
+      <c r="K14" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="43"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="39"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -2273,10 +2303,10 @@
       <c r="L15" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="41" t="s">
+      <c r="M15" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="N15" s="43"/>
+      <c r="N15" s="39"/>
       <c r="O15" s="20" t="s">
         <v>23</v>
       </c>
@@ -2301,10 +2331,10 @@
       <c r="L16" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="M16" s="45">
+      <c r="M16" s="50">
         <v>42401</v>
       </c>
-      <c r="N16" s="46"/>
+      <c r="N16" s="51"/>
       <c r="O16" s="24">
         <v>100</v>
       </c>
@@ -2328,10 +2358,10 @@
       <c r="L17" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="45">
+      <c r="M17" s="50">
         <v>42402</v>
       </c>
-      <c r="N17" s="46"/>
+      <c r="N17" s="51"/>
       <c r="O17" s="24">
         <v>104.08</v>
       </c>
@@ -2347,23 +2377,23 @@
       <c r="E18" s="8"/>
       <c r="F18" s="1"/>
       <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
+      <c r="I18" s="18"/>
       <c r="J18" s="1"/>
       <c r="K18" s="3">
         <v>3</v>
       </c>
       <c r="L18" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="M18" s="45">
-        <v>42433</v>
-      </c>
-      <c r="N18" s="46"/>
+        <v>8</v>
+      </c>
+      <c r="M18" s="50">
+        <v>42402</v>
+      </c>
+      <c r="N18" s="51"/>
       <c r="O18" s="24">
-        <v>20</v>
+        <v>138.5</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -2379,17 +2409,17 @@
         <v>4</v>
       </c>
       <c r="L19" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="M19" s="45">
+        <v>4</v>
+      </c>
+      <c r="M19" s="50">
         <v>42433</v>
       </c>
-      <c r="N19" s="46"/>
+      <c r="N19" s="51"/>
       <c r="O19" s="24">
-        <v>92.66</v>
+        <v>20</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -2402,10 +2432,10 @@
       <c r="L20" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="45">
-        <v>42465</v>
-      </c>
-      <c r="N20" s="46"/>
+      <c r="M20" s="50">
+        <v>42433</v>
+      </c>
+      <c r="N20" s="51"/>
       <c r="O20" s="24">
         <v>92.66</v>
       </c>
@@ -2421,17 +2451,17 @@
         <v>6</v>
       </c>
       <c r="L21" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="M21" s="45">
-        <v>42493</v>
-      </c>
-      <c r="N21" s="46"/>
+        <v>7</v>
+      </c>
+      <c r="M21" s="50">
+        <v>42465</v>
+      </c>
+      <c r="N21" s="51"/>
       <c r="O21" s="24">
-        <v>100</v>
+        <v>92.66</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -2442,17 +2472,17 @@
         <v>7</v>
       </c>
       <c r="L22" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="M22" s="45">
-        <v>42494</v>
-      </c>
-      <c r="N22" s="46"/>
+        <v>4</v>
+      </c>
+      <c r="M22" s="50">
+        <v>42493</v>
+      </c>
+      <c r="N22" s="51"/>
       <c r="O22" s="24">
-        <v>81.900000000000006</v>
+        <v>100</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -2460,22 +2490,38 @@
       <c r="K23" s="3">
         <v>8</v>
       </c>
-      <c r="L23" s="14"/>
-      <c r="M23" s="45"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="3"/>
+      <c r="L23" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="M23" s="50">
+        <v>42494</v>
+      </c>
+      <c r="N23" s="51"/>
+      <c r="O23" s="24">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F24" s="1"/>
       <c r="K24" s="3">
         <v>9</v>
       </c>
-      <c r="L24" s="14"/>
-      <c r="M24" s="45"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="3"/>
+      <c r="L24" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="M24" s="50">
+        <v>42531</v>
+      </c>
+      <c r="N24" s="51"/>
+      <c r="O24" s="24">
+        <v>93.52</v>
+      </c>
+      <c r="P24" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F25" s="1"/>
@@ -2494,6 +2540,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M15:N15"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="P8:P9"/>
     <mergeCell ref="M21:N21"/>
@@ -2503,15 +2558,6 @@
     <mergeCell ref="N8:N9"/>
     <mergeCell ref="O8:O9"/>
     <mergeCell ref="K14:P14"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="M15:N15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated payment and refund
</commit_message>
<xml_diff>
--- a/ATT_Bill.xlsx
+++ b/ATT_Bill.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="47">
   <si>
     <t>ATT Family Plan Bill Details</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>Current month Calculation</t>
+  </si>
+  <si>
+    <t>Refund</t>
   </si>
 </sst>
 </file>
@@ -274,7 +277,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -391,12 +394,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -488,6 +522,16 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -527,11 +571,26 @@
     <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -543,25 +602,6 @@
     <xf numFmtId="44" fontId="6" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="5" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -868,19 +908,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -950,16 +990,16 @@
       <c r="F3" s="11">
         <v>53.44</v>
       </c>
-      <c r="G3" s="33">
+      <c r="G3" s="39">
         <v>0</v>
       </c>
-      <c r="H3" s="33">
+      <c r="H3" s="39">
         <v>0</v>
       </c>
-      <c r="I3" s="33">
+      <c r="I3" s="39">
         <v>0</v>
       </c>
-      <c r="J3" s="33">
+      <c r="J3" s="39">
         <v>0</v>
       </c>
       <c r="K3" s="2"/>
@@ -997,10 +1037,10 @@
       <c r="F4" s="11">
         <v>38.54</v>
       </c>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="2"/>
       <c r="L4" s="1"/>
       <c r="M4" s="2" t="s">
@@ -1010,11 +1050,11 @@
         <f>SUM(C3:C15)</f>
         <v>482.77999999999992</v>
       </c>
-      <c r="O4" s="33">
+      <c r="O4" s="39">
         <f>200+490.45</f>
         <v>690.45</v>
       </c>
-      <c r="P4" s="36">
+      <c r="P4" s="42">
         <f>N4+N5-O4</f>
         <v>-207.67000000000013</v>
       </c>
@@ -1039,10 +1079,10 @@
       <c r="F5" s="11">
         <v>38.229999999999997</v>
       </c>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
       <c r="K5" s="2"/>
       <c r="L5" s="1"/>
       <c r="M5" s="2" t="s">
@@ -1052,8 +1092,8 @@
         <f>SUM(J3:J15)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="35"/>
-      <c r="P5" s="37"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="43"/>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1075,10 +1115,10 @@
       <c r="F6" s="11">
         <v>38.54</v>
       </c>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
       <c r="K6" s="2"/>
       <c r="L6" s="1"/>
       <c r="M6" s="2" t="s">
@@ -1117,10 +1157,10 @@
       <c r="F7" s="11">
         <v>38.69</v>
       </c>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
       <c r="K7" s="2"/>
       <c r="L7" s="1"/>
       <c r="M7" s="2" t="s">
@@ -1130,10 +1170,10 @@
         <f>SUM(F3:F15)</f>
         <v>491.13999999999993</v>
       </c>
-      <c r="O7" s="33">
+      <c r="O7" s="39">
         <v>1024.28</v>
       </c>
-      <c r="P7" s="36">
+      <c r="P7" s="42">
         <f>N7+N8-O7</f>
         <v>0</v>
       </c>
@@ -1158,10 +1198,10 @@
       <c r="F8" s="11">
         <v>39.799999999999997</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
       <c r="K8" s="2"/>
       <c r="L8" s="1"/>
       <c r="M8" s="2" t="s">
@@ -1171,8 +1211,8 @@
         <f>SUM(E3:E14)</f>
         <v>533.14</v>
       </c>
-      <c r="O8" s="35"/>
-      <c r="P8" s="37"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="43"/>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1194,10 +1234,10 @@
       <c r="F9" s="11">
         <v>38.69</v>
       </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
       <c r="K9" s="2"/>
       <c r="L9" s="1"/>
       <c r="M9" s="2" t="s">
@@ -1207,11 +1247,11 @@
         <f>SUM(G3:G15)</f>
         <v>175.34</v>
       </c>
-      <c r="O9" s="33">
+      <c r="O9" s="39">
         <f>113.35+61.99+51.99</f>
         <v>227.33</v>
       </c>
-      <c r="P9" s="36">
+      <c r="P9" s="42">
         <f>N9+N10-O9</f>
         <v>0</v>
       </c>
@@ -1237,10 +1277,10 @@
       <c r="F10" s="11">
         <v>39.14</v>
       </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
       <c r="K10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1252,8 +1292,8 @@
         <f>SUM(I3:I15)</f>
         <v>51.99</v>
       </c>
-      <c r="O10" s="35"/>
-      <c r="P10" s="37"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="43"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
@@ -1276,10 +1316,10 @@
       <c r="F11" s="11">
         <v>38.92</v>
       </c>
-      <c r="G11" s="35"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
       <c r="K11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1323,9 +1363,9 @@
       <c r="G12" s="11">
         <v>52.78</v>
       </c>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
       <c r="K12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1359,9 +1399,9 @@
       <c r="G13" s="11">
         <v>60.57</v>
       </c>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="34"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="40"/>
       <c r="K13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1407,7 +1447,7 @@
         <f>36.99+15</f>
         <v>51.99</v>
       </c>
-      <c r="J14" s="35"/>
+      <c r="J14" s="41"/>
       <c r="K14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1458,14 +1498,14 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="40" t="s">
+      <c r="M15" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="41"/>
-      <c r="O15" s="41"/>
-      <c r="P15" s="41"/>
-      <c r="Q15" s="41"/>
-      <c r="R15" s="42"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="47"/>
+      <c r="R15" s="48"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -1486,10 +1526,10 @@
       <c r="N16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O16" s="43" t="s">
+      <c r="O16" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="P16" s="43"/>
+      <c r="P16" s="49"/>
       <c r="Q16" s="10" t="s">
         <v>23</v>
       </c>
@@ -1516,10 +1556,10 @@
       <c r="N17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O17" s="38">
+      <c r="O17" s="44">
         <v>42053</v>
       </c>
-      <c r="P17" s="38"/>
+      <c r="P17" s="44"/>
       <c r="Q17" s="13">
         <v>108</v>
       </c>
@@ -1545,10 +1585,10 @@
       <c r="N18" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O18" s="38">
+      <c r="O18" s="44">
         <v>42086</v>
       </c>
-      <c r="P18" s="38"/>
+      <c r="P18" s="44"/>
       <c r="Q18" s="13">
         <v>200</v>
       </c>
@@ -1574,10 +1614,10 @@
       <c r="N19" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O19" s="38">
+      <c r="O19" s="44">
         <v>42111</v>
       </c>
-      <c r="P19" s="38"/>
+      <c r="P19" s="44"/>
       <c r="Q19" s="13">
         <v>100</v>
       </c>
@@ -1602,10 +1642,10 @@
       <c r="N20" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O20" s="38">
+      <c r="O20" s="44">
         <v>42214</v>
       </c>
-      <c r="P20" s="38"/>
+      <c r="P20" s="44"/>
       <c r="Q20" s="13">
         <v>160</v>
       </c>
@@ -1624,10 +1664,10 @@
       <c r="N21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O21" s="38">
+      <c r="O21" s="44">
         <v>42325</v>
       </c>
-      <c r="P21" s="38"/>
+      <c r="P21" s="44"/>
       <c r="Q21" s="13">
         <v>113.35</v>
       </c>
@@ -1646,10 +1686,10 @@
       <c r="N22" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="O22" s="38">
+      <c r="O22" s="44">
         <v>42325</v>
       </c>
-      <c r="P22" s="38"/>
+      <c r="P22" s="44"/>
       <c r="Q22" s="13">
         <v>80</v>
       </c>
@@ -1667,10 +1707,10 @@
       <c r="N23" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O23" s="38">
+      <c r="O23" s="44">
         <v>42341</v>
       </c>
-      <c r="P23" s="38"/>
+      <c r="P23" s="44"/>
       <c r="Q23" s="13">
         <v>490.45</v>
       </c>
@@ -1686,10 +1726,10 @@
       <c r="N24" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O24" s="38">
+      <c r="O24" s="44">
         <v>42364</v>
       </c>
-      <c r="P24" s="38"/>
+      <c r="P24" s="44"/>
       <c r="Q24" s="13">
         <v>113.98</v>
       </c>
@@ -1701,8 +1741,8 @@
       <c r="G25" s="1"/>
       <c r="M25" s="3"/>
       <c r="N25" s="14"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
+      <c r="O25" s="44"/>
+      <c r="P25" s="44"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="3"/>
     </row>
@@ -1754,11 +1794,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1781,18 +1821,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1938,15 +1978,15 @@
         <f>SUM(C3:C14)</f>
         <v>282.22300000000001</v>
       </c>
-      <c r="N4" s="48">
+      <c r="N4" s="59">
         <f>207.67+O28</f>
         <v>407.66999999999996</v>
       </c>
-      <c r="O4" s="54">
+      <c r="O4" s="57">
         <f>SUM(M4:M5)-N4+P4</f>
-        <v>535.03300000000002</v>
-      </c>
-      <c r="P4" s="50">
+        <v>284.59299999999996</v>
+      </c>
+      <c r="P4" s="61">
         <v>0</v>
       </c>
       <c r="Q4" s="1"/>
@@ -1990,11 +2030,11 @@
       </c>
       <c r="M5" s="32">
         <f>SUM(D3:D14)</f>
-        <v>660.48</v>
-      </c>
-      <c r="N5" s="49"/>
-      <c r="O5" s="55"/>
-      <c r="P5" s="51"/>
+        <v>410.03999999999996</v>
+      </c>
+      <c r="N5" s="60"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="62"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -2147,15 +2187,15 @@
         <f>SUM(G3:G14)</f>
         <v>470.66999999999996</v>
       </c>
-      <c r="N8" s="48">
+      <c r="N8" s="59">
         <f>SUM(O17,O20:O21,O23:O24,O25,O27)</f>
         <v>647.31999999999994</v>
       </c>
-      <c r="O8" s="54">
+      <c r="O8" s="57">
         <f>M8+M9-N8</f>
         <v>90.569999999999936</v>
       </c>
-      <c r="P8" s="52">
+      <c r="P8" s="63">
         <v>0</v>
       </c>
       <c r="Q8" s="1"/>
@@ -2201,9 +2241,9 @@
         <f>SUM(H3:H14)</f>
         <v>267.21999999999997</v>
       </c>
-      <c r="N9" s="49"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="53"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="64"/>
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" ht="120" x14ac:dyDescent="0.25">
@@ -2273,7 +2313,7 @@
         <v>31.06</v>
       </c>
       <c r="D11" s="28">
-        <v>532.58000000000004</v>
+        <v>282.14</v>
       </c>
       <c r="E11" s="21">
         <v>31.06</v>
@@ -2358,14 +2398,14 @@
       <c r="H14" s="28"/>
       <c r="I14" s="28"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="40" t="s">
+      <c r="K14" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="42"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="47"/>
+      <c r="P14" s="48"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -2384,10 +2424,10 @@
       <c r="L15" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="40" t="s">
+      <c r="M15" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="N15" s="42"/>
+      <c r="N15" s="48"/>
       <c r="O15" s="20" t="s">
         <v>23</v>
       </c>
@@ -2412,10 +2452,10 @@
       <c r="L16" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="M16" s="44">
+      <c r="M16" s="50">
         <v>42401</v>
       </c>
-      <c r="N16" s="45"/>
+      <c r="N16" s="51"/>
       <c r="O16" s="24">
         <v>100</v>
       </c>
@@ -2423,18 +2463,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="8"/>
-      <c r="D17" s="58" t="s">
+      <c r="D17" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="1"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="54"/>
       <c r="J17" s="1"/>
       <c r="K17" s="3">
         <v>2</v>
@@ -2442,10 +2482,10 @@
       <c r="L17" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="44">
+      <c r="M17" s="50">
         <v>42402</v>
       </c>
-      <c r="N17" s="45"/>
+      <c r="N17" s="51"/>
       <c r="O17" s="24">
         <v>104.08</v>
       </c>
@@ -2457,22 +2497,24 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="59" t="s">
+      <c r="D18" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="60" t="s">
+      <c r="E18" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="59" t="s">
+      <c r="F18" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="59" t="s">
+      <c r="G18" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="H18" s="60" t="s">
+      <c r="H18" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I18" s="18"/>
+      <c r="I18" s="36" t="s">
+        <v>46</v>
+      </c>
       <c r="J18" s="1"/>
       <c r="K18" s="3">
         <v>3</v>
@@ -2480,10 +2522,10 @@
       <c r="L18" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="M18" s="44">
+      <c r="M18" s="50">
         <v>42402</v>
       </c>
-      <c r="N18" s="45"/>
+      <c r="N18" s="51"/>
       <c r="O18" s="24">
         <v>138.5</v>
       </c>
@@ -2499,7 +2541,7 @@
         <v>3</v>
       </c>
       <c r="E19" s="32">
-        <f>75/7</f>
+        <f t="shared" ref="E19:E25" si="0">75/7</f>
         <v>10.714285714285714</v>
       </c>
       <c r="F19" s="32">
@@ -2508,10 +2550,11 @@
       <c r="G19" s="32">
         <v>5.35</v>
       </c>
-      <c r="H19" s="56">
-        <f>SUM(E19:G19)</f>
+      <c r="H19" s="33">
+        <f t="shared" ref="H19:H25" si="1">SUM(E19:G19)</f>
         <v>31.064285714285717</v>
       </c>
+      <c r="I19" s="33"/>
       <c r="J19" s="1"/>
       <c r="K19" s="3">
         <v>4</v>
@@ -2519,10 +2562,10 @@
       <c r="L19" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="M19" s="44">
+      <c r="M19" s="50">
         <v>42433</v>
       </c>
-      <c r="N19" s="45"/>
+      <c r="N19" s="51"/>
       <c r="O19" s="24">
         <v>20</v>
       </c>
@@ -2533,34 +2576,36 @@
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="57" t="s">
+      <c r="D20" s="34" t="s">
         <v>29</v>
       </c>
       <c r="E20" s="32">
-        <f>75/7</f>
+        <f t="shared" si="0"/>
         <v>10.714285714285714</v>
       </c>
-      <c r="F20" s="56">
+      <c r="F20" s="33">
         <v>15</v>
       </c>
-      <c r="G20" s="56">
+      <c r="G20" s="33">
         <v>506.87</v>
       </c>
-      <c r="H20" s="56">
-        <f>SUM(E20:G20)</f>
+      <c r="H20" s="33">
+        <f t="shared" si="1"/>
         <v>532.58428571428567</v>
       </c>
-      <c r="I20" s="7"/>
+      <c r="I20" s="33">
+        <v>-250.44</v>
+      </c>
       <c r="K20" s="3">
         <v>5</v>
       </c>
       <c r="L20" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="44">
+      <c r="M20" s="50">
         <v>42433</v>
       </c>
-      <c r="N20" s="45"/>
+      <c r="N20" s="51"/>
       <c r="O20" s="24">
         <v>92.66</v>
       </c>
@@ -2571,33 +2616,34 @@
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="57" t="s">
+      <c r="D21" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E21" s="32">
-        <f>75/7</f>
+        <f t="shared" si="0"/>
         <v>10.714285714285714</v>
       </c>
-      <c r="F21" s="56">
+      <c r="F21" s="33">
         <v>15</v>
       </c>
-      <c r="G21" s="56">
+      <c r="G21" s="33">
         <v>5.35</v>
       </c>
-      <c r="H21" s="56">
-        <f>SUM(E21:G21)</f>
+      <c r="H21" s="33">
+        <f t="shared" si="1"/>
         <v>31.064285714285717</v>
       </c>
+      <c r="I21" s="33"/>
       <c r="K21" s="3">
         <v>6</v>
       </c>
       <c r="L21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M21" s="44">
+      <c r="M21" s="50">
         <v>42465</v>
       </c>
-      <c r="N21" s="45"/>
+      <c r="N21" s="51"/>
       <c r="O21" s="24">
         <v>92.66</v>
       </c>
@@ -2612,29 +2658,30 @@
         <v>6</v>
       </c>
       <c r="E22" s="32">
-        <f>75/7</f>
+        <f t="shared" si="0"/>
         <v>10.714285714285714</v>
       </c>
-      <c r="F22" s="56">
+      <c r="F22" s="33">
         <v>15</v>
       </c>
-      <c r="G22" s="56">
+      <c r="G22" s="33">
         <v>5.35</v>
       </c>
-      <c r="H22" s="56">
-        <f>SUM(E22:G22)</f>
+      <c r="H22" s="33">
+        <f t="shared" si="1"/>
         <v>31.064285714285717</v>
       </c>
+      <c r="I22" s="33"/>
       <c r="K22" s="3">
         <v>7</v>
       </c>
       <c r="L22" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="M22" s="44">
+      <c r="M22" s="50">
         <v>42493</v>
       </c>
-      <c r="N22" s="45"/>
+      <c r="N22" s="51"/>
       <c r="O22" s="24">
         <v>100</v>
       </c>
@@ -2647,29 +2694,30 @@
         <v>37</v>
       </c>
       <c r="E23" s="32">
-        <f>75/7</f>
+        <f t="shared" si="0"/>
         <v>10.714285714285714</v>
       </c>
-      <c r="F23" s="56">
+      <c r="F23" s="33">
         <v>15</v>
       </c>
-      <c r="G23" s="56">
+      <c r="G23" s="33">
         <v>4.7300000000000004</v>
       </c>
-      <c r="H23" s="56">
-        <f>SUM(E23:G23)</f>
+      <c r="H23" s="33">
+        <f t="shared" si="1"/>
         <v>30.444285714285716</v>
       </c>
+      <c r="I23" s="33"/>
       <c r="K23" s="3">
         <v>8</v>
       </c>
       <c r="L23" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M23" s="44">
+      <c r="M23" s="50">
         <v>42494</v>
       </c>
-      <c r="N23" s="45"/>
+      <c r="N23" s="51"/>
       <c r="O23" s="24">
         <v>81.900000000000006</v>
       </c>
@@ -2682,29 +2730,30 @@
         <v>7</v>
       </c>
       <c r="E24" s="32">
-        <f>75/7</f>
+        <f t="shared" si="0"/>
         <v>10.714285714285714</v>
       </c>
       <c r="F24" s="32">
         <v>40</v>
       </c>
-      <c r="G24" s="56">
+      <c r="G24" s="33">
         <v>8.8000000000000007</v>
       </c>
-      <c r="H24" s="56">
-        <f>SUM(E24:G24)</f>
+      <c r="H24" s="33">
+        <f t="shared" si="1"/>
         <v>59.51428571428572</v>
       </c>
+      <c r="I24" s="33"/>
       <c r="K24" s="3">
         <v>9</v>
       </c>
       <c r="L24" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M24" s="44">
+      <c r="M24" s="50">
         <v>42531</v>
       </c>
-      <c r="N24" s="45"/>
+      <c r="N24" s="51"/>
       <c r="O24" s="24">
         <v>93.52</v>
       </c>
@@ -2717,29 +2766,30 @@
         <v>39</v>
       </c>
       <c r="E25" s="32">
-        <f>75/7</f>
+        <f t="shared" si="0"/>
         <v>10.714285714285714</v>
       </c>
       <c r="F25" s="32">
         <v>15</v>
       </c>
-      <c r="G25" s="56">
+      <c r="G25" s="33">
         <v>5.35</v>
       </c>
-      <c r="H25" s="56">
-        <f>SUM(E25:G25)</f>
+      <c r="H25" s="33">
+        <f t="shared" si="1"/>
         <v>31.064285714285717</v>
       </c>
+      <c r="I25" s="33"/>
       <c r="K25" s="3">
         <v>10</v>
       </c>
       <c r="L25" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M25" s="44">
+      <c r="M25" s="50">
         <v>42558</v>
       </c>
-      <c r="N25" s="45"/>
+      <c r="N25" s="51"/>
       <c r="O25" s="24">
         <v>91.1</v>
       </c>
@@ -2749,12 +2799,12 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F26" s="1"/>
-      <c r="G26" s="61" t="s">
+      <c r="G26" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="62">
-        <f>SUM(H19:H25)</f>
-        <v>746.79999999999984</v>
+      <c r="H26" s="38">
+        <f>SUM(H19:I25)</f>
+        <v>496.36</v>
       </c>
       <c r="K26" s="3">
         <v>10</v>
@@ -2762,10 +2812,10 @@
       <c r="L26" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="M26" s="44">
+      <c r="M26" s="50">
         <v>42590</v>
       </c>
-      <c r="N26" s="45"/>
+      <c r="N26" s="51"/>
       <c r="O26" s="24">
         <v>100</v>
       </c>
@@ -2781,10 +2831,10 @@
       <c r="L27" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M27" s="44">
+      <c r="M27" s="50">
         <v>42598</v>
       </c>
-      <c r="N27" s="45"/>
+      <c r="N27" s="51"/>
       <c r="O27" s="24">
         <v>91.4</v>
       </c>
@@ -2800,10 +2850,10 @@
       <c r="L28" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="M28" s="44">
+      <c r="M28" s="50">
         <v>42599</v>
       </c>
-      <c r="N28" s="45"/>
+      <c r="N28" s="51"/>
       <c r="O28" s="24">
         <v>200</v>
       </c>
@@ -2818,10 +2868,10 @@
       <c r="L29" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="M29" s="44">
+      <c r="M29" s="50">
         <v>42600</v>
       </c>
-      <c r="N29" s="45"/>
+      <c r="N29" s="51"/>
       <c r="O29" s="24">
         <v>200</v>
       </c>
@@ -2829,29 +2879,48 @@
         <v>35</v>
       </c>
     </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K30" s="3">
+        <v>13</v>
+      </c>
+      <c r="L30" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="M30" s="50">
+        <v>42615</v>
+      </c>
+      <c r="N30" s="51"/>
+      <c r="O30" s="24">
+        <v>90.57</v>
+      </c>
+      <c r="P30" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
     <mergeCell ref="M15:N15"/>
-    <mergeCell ref="D17:H17"/>
     <mergeCell ref="M24:N24"/>
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="M17:N17"/>
     <mergeCell ref="M18:N18"/>
     <mergeCell ref="M19:N19"/>
     <mergeCell ref="M20:N20"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M27:N27"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="O4:O5"/>
     <mergeCell ref="N8:N9"/>
     <mergeCell ref="O8:O9"/>
     <mergeCell ref="K14:P14"/>
     <mergeCell ref="N4:N5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="D17:I17"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M27:N27"/>
     <mergeCell ref="M25:N25"/>
     <mergeCell ref="M26:N26"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="P8:P9"/>
     <mergeCell ref="M21:N21"/>
     <mergeCell ref="M22:N22"/>
     <mergeCell ref="M23:N23"/>

</xml_diff>

<commit_message>
updated Jan 2017 Bill
</commit_message>
<xml_diff>
--- a/ATT_Bill.xlsx
+++ b/ATT_Bill.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="1" r:id="rId1"/>
     <sheet name="2016" sheetId="2" r:id="rId2"/>
+    <sheet name="2017" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="51">
   <si>
     <t>ATT Family Plan Bill Details</t>
   </si>
@@ -192,6 +193,13 @@
   </si>
   <si>
     <t>Sankari - International calling - $15 extra</t>
+  </si>
+  <si>
+    <t>Giri - India calling extra $44.32
+Sankari - India calling extra $15</t>
+  </si>
+  <si>
+    <t>Previous Balance - 2016</t>
   </si>
 </sst>
 </file>
@@ -204,7 +212,7 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +255,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -443,7 +458,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -527,6 +542,18 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -560,12 +587,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -591,14 +612,22 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="6" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="5" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="44" fontId="7" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="7" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -906,19 +935,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -988,16 +1017,16 @@
       <c r="F3" s="8">
         <v>53.44</v>
       </c>
-      <c r="G3" s="33">
+      <c r="G3" s="37">
         <v>0</v>
       </c>
-      <c r="H3" s="33">
+      <c r="H3" s="37">
         <v>0</v>
       </c>
-      <c r="I3" s="33">
+      <c r="I3" s="37">
         <v>0</v>
       </c>
-      <c r="J3" s="33">
+      <c r="J3" s="37">
         <v>0</v>
       </c>
       <c r="K3" s="2"/>
@@ -1035,10 +1064,10 @@
       <c r="F4" s="8">
         <v>38.54</v>
       </c>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="2"/>
       <c r="L4" s="1"/>
       <c r="M4" s="2" t="s">
@@ -1048,11 +1077,11 @@
         <f>SUM(C3:C15)</f>
         <v>482.77999999999992</v>
       </c>
-      <c r="O4" s="33">
+      <c r="O4" s="37">
         <f>200+490.45</f>
         <v>690.45</v>
       </c>
-      <c r="P4" s="36">
+      <c r="P4" s="40">
         <f>N4+N5-O4</f>
         <v>-207.67000000000013</v>
       </c>
@@ -1077,10 +1106,10 @@
       <c r="F5" s="8">
         <v>38.229999999999997</v>
       </c>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
       <c r="K5" s="2"/>
       <c r="L5" s="1"/>
       <c r="M5" s="2" t="s">
@@ -1090,8 +1119,8 @@
         <f>SUM(J3:J15)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="35"/>
-      <c r="P5" s="37"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="41"/>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -1113,10 +1142,10 @@
       <c r="F6" s="8">
         <v>38.54</v>
       </c>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
       <c r="K6" s="2"/>
       <c r="L6" s="1"/>
       <c r="M6" s="2" t="s">
@@ -1155,10 +1184,10 @@
       <c r="F7" s="8">
         <v>38.69</v>
       </c>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
       <c r="K7" s="2"/>
       <c r="L7" s="1"/>
       <c r="M7" s="2" t="s">
@@ -1168,10 +1197,10 @@
         <f>SUM(F3:F15)</f>
         <v>491.13999999999993</v>
       </c>
-      <c r="O7" s="33">
+      <c r="O7" s="37">
         <v>1024.28</v>
       </c>
-      <c r="P7" s="36">
+      <c r="P7" s="40">
         <f>N7+N8-O7</f>
         <v>0</v>
       </c>
@@ -1196,10 +1225,10 @@
       <c r="F8" s="8">
         <v>39.799999999999997</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
       <c r="K8" s="2"/>
       <c r="L8" s="1"/>
       <c r="M8" s="2" t="s">
@@ -1209,8 +1238,8 @@
         <f>SUM(E3:E14)</f>
         <v>533.14</v>
       </c>
-      <c r="O8" s="35"/>
-      <c r="P8" s="37"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="41"/>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
@@ -1232,10 +1261,10 @@
       <c r="F9" s="8">
         <v>38.69</v>
       </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
       <c r="K9" s="2"/>
       <c r="L9" s="1"/>
       <c r="M9" s="2" t="s">
@@ -1245,11 +1274,11 @@
         <f>SUM(G3:G15)</f>
         <v>175.34</v>
       </c>
-      <c r="O9" s="33">
+      <c r="O9" s="37">
         <f>113.35+61.99+51.99</f>
         <v>227.33</v>
       </c>
-      <c r="P9" s="36">
+      <c r="P9" s="40">
         <f>N9+N10-O9</f>
         <v>0</v>
       </c>
@@ -1275,10 +1304,10 @@
       <c r="F10" s="8">
         <v>39.14</v>
       </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
       <c r="K10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1290,8 +1319,8 @@
         <f>SUM(I3:I15)</f>
         <v>51.99</v>
       </c>
-      <c r="O10" s="35"/>
-      <c r="P10" s="37"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="41"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
@@ -1314,10 +1343,10 @@
       <c r="F11" s="8">
         <v>38.92</v>
       </c>
-      <c r="G11" s="35"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
       <c r="K11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1361,9 +1390,9 @@
       <c r="G12" s="8">
         <v>52.78</v>
       </c>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
       <c r="K12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1397,9 +1426,9 @@
       <c r="G13" s="8">
         <v>60.57</v>
       </c>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="34"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="38"/>
       <c r="K13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1445,7 +1474,7 @@
         <f>36.99+15</f>
         <v>51.99</v>
       </c>
-      <c r="J14" s="35"/>
+      <c r="J14" s="39"/>
       <c r="K14" s="2" t="s">
         <v>21</v>
       </c>
@@ -1496,14 +1525,14 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="40" t="s">
+      <c r="M15" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="N15" s="41"/>
-      <c r="O15" s="41"/>
-      <c r="P15" s="41"/>
-      <c r="Q15" s="41"/>
-      <c r="R15" s="42"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="45"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="46"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
@@ -1524,10 +1553,10 @@
       <c r="N16" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="O16" s="43" t="s">
+      <c r="O16" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="P16" s="43"/>
+      <c r="P16" s="47"/>
       <c r="Q16" s="32" t="s">
         <v>25</v>
       </c>
@@ -1554,10 +1583,10 @@
       <c r="N17" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O17" s="38">
+      <c r="O17" s="42">
         <v>42053</v>
       </c>
-      <c r="P17" s="38"/>
+      <c r="P17" s="42"/>
       <c r="Q17" s="10">
         <v>108</v>
       </c>
@@ -1583,10 +1612,10 @@
       <c r="N18" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="O18" s="38">
+      <c r="O18" s="42">
         <v>42086</v>
       </c>
-      <c r="P18" s="38"/>
+      <c r="P18" s="42"/>
       <c r="Q18" s="10">
         <v>200</v>
       </c>
@@ -1612,10 +1641,10 @@
       <c r="N19" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O19" s="38">
+      <c r="O19" s="42">
         <v>42111</v>
       </c>
-      <c r="P19" s="38"/>
+      <c r="P19" s="42"/>
       <c r="Q19" s="10">
         <v>100</v>
       </c>
@@ -1640,10 +1669,10 @@
       <c r="N20" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O20" s="38">
+      <c r="O20" s="42">
         <v>42214</v>
       </c>
-      <c r="P20" s="38"/>
+      <c r="P20" s="42"/>
       <c r="Q20" s="10">
         <v>160</v>
       </c>
@@ -1662,10 +1691,10 @@
       <c r="N21" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="O21" s="38">
+      <c r="O21" s="42">
         <v>42325</v>
       </c>
-      <c r="P21" s="38"/>
+      <c r="P21" s="42"/>
       <c r="Q21" s="10">
         <v>113.35</v>
       </c>
@@ -1684,10 +1713,10 @@
       <c r="N22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O22" s="38">
+      <c r="O22" s="42">
         <v>42325</v>
       </c>
-      <c r="P22" s="38"/>
+      <c r="P22" s="42"/>
       <c r="Q22" s="10">
         <v>80</v>
       </c>
@@ -1705,10 +1734,10 @@
       <c r="N23" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="O23" s="38">
+      <c r="O23" s="42">
         <v>42341</v>
       </c>
-      <c r="P23" s="38"/>
+      <c r="P23" s="42"/>
       <c r="Q23" s="10">
         <v>490.45</v>
       </c>
@@ -1724,10 +1753,10 @@
       <c r="N24" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="O24" s="38">
+      <c r="O24" s="42">
         <v>42364</v>
       </c>
-      <c r="P24" s="38"/>
+      <c r="P24" s="42"/>
       <c r="Q24" s="10">
         <v>113.98</v>
       </c>
@@ -1739,8 +1768,8 @@
       <c r="G25" s="1"/>
       <c r="M25" s="3"/>
       <c r="N25" s="11"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="42"/>
       <c r="Q25" s="10"/>
       <c r="R25" s="3"/>
     </row>
@@ -1792,11 +1821,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:Q36"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" workbookViewId="0">
+    <sheetView zoomScale="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q8" sqref="Q8"/>
+      <selection pane="bottomLeft" activeCell="O4" sqref="O4:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1819,18 +1848,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1976,15 +2005,15 @@
         <f>SUM(C3:C14)</f>
         <v>375.303</v>
       </c>
-      <c r="N4" s="53">
+      <c r="N4" s="55">
         <f>207.67+O28+O31+O32</f>
         <v>807.67</v>
       </c>
-      <c r="O4" s="51">
+      <c r="O4" s="53">
         <f>SUM(M4:M5)-N4+P4</f>
         <v>144.58299999999997</v>
       </c>
-      <c r="P4" s="55">
+      <c r="P4" s="59">
         <v>0</v>
       </c>
       <c r="Q4" s="1"/>
@@ -2030,9 +2059,9 @@
         <f>SUM(D3:D14)</f>
         <v>576.94999999999993</v>
       </c>
-      <c r="N5" s="54"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="56"/>
+      <c r="N5" s="56"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="60"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.2">
@@ -2077,12 +2106,12 @@
         <v>360.29999999999995</v>
       </c>
       <c r="N6" s="24">
-        <f>SUM(O16,O19,O22,O26,O33,O35)</f>
-        <v>352</v>
-      </c>
-      <c r="O6" s="23">
+        <f>SUM(O16,O19,O22,O26,O33,O35,O38)</f>
+        <v>452</v>
+      </c>
+      <c r="O6" s="19">
         <f>M6-N6+P6</f>
-        <v>39.55999999999996</v>
+        <v>-60.44000000000004</v>
       </c>
       <c r="P6" s="20">
         <v>31.26</v>
@@ -2185,15 +2214,15 @@
         <f>SUM(G3:G14)</f>
         <v>620.59999999999991</v>
       </c>
-      <c r="N8" s="53">
-        <f>SUM(O17,O20:O21,O23:O24,O25,O27,O30,O34,O36)</f>
-        <v>918.87999999999977</v>
-      </c>
-      <c r="O8" s="51">
+      <c r="N8" s="55">
+        <f>SUM(O17,O20:O21,O23:O24,O25,O27,O30,O34,O36,O37)</f>
+        <v>980.89999999999975</v>
+      </c>
+      <c r="O8" s="57">
         <f>M8+M9-N8</f>
-        <v>62.020000000000095</v>
-      </c>
-      <c r="P8" s="57">
+        <v>0</v>
+      </c>
+      <c r="P8" s="61">
         <v>0</v>
       </c>
       <c r="Q8" s="1"/>
@@ -2239,9 +2268,9 @@
         <f>SUM(H3:H14)</f>
         <v>360.29999999999995</v>
       </c>
-      <c r="N9" s="54"/>
-      <c r="O9" s="52"/>
-      <c r="P9" s="58"/>
+      <c r="N9" s="56"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="62"/>
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" ht="120" x14ac:dyDescent="0.2">
@@ -2450,14 +2479,14 @@
       <c r="J14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K14" s="40" t="s">
+      <c r="K14" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="42"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="47"/>
+      <c r="P14" s="47"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
@@ -2470,20 +2499,20 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="32" t="s">
+      <c r="K15" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="L15" s="32" t="s">
+      <c r="L15" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="40" t="s">
+      <c r="M15" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="N15" s="42"/>
-      <c r="O15" s="32" t="s">
+      <c r="N15" s="47"/>
+      <c r="O15" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="P15" s="32" t="s">
+      <c r="P15" s="33" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2504,10 +2533,10 @@
       <c r="L16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M16" s="44">
+      <c r="M16" s="42">
         <v>42401</v>
       </c>
-      <c r="N16" s="45"/>
+      <c r="N16" s="42"/>
       <c r="O16" s="18">
         <v>100</v>
       </c>
@@ -2519,14 +2548,14 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="48"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="50"/>
       <c r="J17" s="1"/>
       <c r="K17" s="3">
         <v>2</v>
@@ -2534,10 +2563,10 @@
       <c r="L17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="44">
+      <c r="M17" s="42">
         <v>42402</v>
       </c>
-      <c r="N17" s="45"/>
+      <c r="N17" s="42"/>
       <c r="O17" s="18">
         <v>104.08</v>
       </c>
@@ -2574,10 +2603,10 @@
       <c r="L18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M18" s="44">
+      <c r="M18" s="42">
         <v>42402</v>
       </c>
-      <c r="N18" s="45"/>
+      <c r="N18" s="42"/>
       <c r="O18" s="18">
         <v>138.5</v>
       </c>
@@ -2614,10 +2643,10 @@
       <c r="L19" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M19" s="44">
+      <c r="M19" s="42">
         <v>42433</v>
       </c>
-      <c r="N19" s="45"/>
+      <c r="N19" s="42"/>
       <c r="O19" s="18">
         <v>20</v>
       </c>
@@ -2652,10 +2681,10 @@
       <c r="L20" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="44">
+      <c r="M20" s="42">
         <v>42433</v>
       </c>
-      <c r="N20" s="45"/>
+      <c r="N20" s="42"/>
       <c r="O20" s="18">
         <v>92.66</v>
       </c>
@@ -2690,10 +2719,10 @@
       <c r="L21" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M21" s="44">
+      <c r="M21" s="42">
         <v>42465</v>
       </c>
-      <c r="N21" s="45"/>
+      <c r="N21" s="42"/>
       <c r="O21" s="18">
         <v>92.66</v>
       </c>
@@ -2728,10 +2757,10 @@
       <c r="L22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M22" s="44">
+      <c r="M22" s="42">
         <v>42493</v>
       </c>
-      <c r="N22" s="45"/>
+      <c r="N22" s="42"/>
       <c r="O22" s="18">
         <v>100</v>
       </c>
@@ -2764,10 +2793,10 @@
       <c r="L23" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M23" s="44">
+      <c r="M23" s="42">
         <v>42494</v>
       </c>
-      <c r="N23" s="45"/>
+      <c r="N23" s="42"/>
       <c r="O23" s="18">
         <v>81.900000000000006</v>
       </c>
@@ -2800,10 +2829,10 @@
       <c r="L24" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M24" s="44">
+      <c r="M24" s="42">
         <v>42531</v>
       </c>
-      <c r="N24" s="45"/>
+      <c r="N24" s="42"/>
       <c r="O24" s="18">
         <v>93.52</v>
       </c>
@@ -2836,10 +2865,10 @@
       <c r="L25" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M25" s="44">
+      <c r="M25" s="42">
         <v>42558</v>
       </c>
-      <c r="N25" s="45"/>
+      <c r="N25" s="42"/>
       <c r="O25" s="18">
         <v>91.1</v>
       </c>
@@ -2862,10 +2891,10 @@
       <c r="L26" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M26" s="44">
+      <c r="M26" s="42">
         <v>42590</v>
       </c>
-      <c r="N26" s="45"/>
+      <c r="N26" s="42"/>
       <c r="O26" s="18">
         <v>100</v>
       </c>
@@ -2881,10 +2910,10 @@
       <c r="L27" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M27" s="44">
+      <c r="M27" s="42">
         <v>42598</v>
       </c>
-      <c r="N27" s="45"/>
+      <c r="N27" s="42"/>
       <c r="O27" s="18">
         <v>91.4</v>
       </c>
@@ -2900,10 +2929,10 @@
       <c r="L28" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="M28" s="44">
+      <c r="M28" s="42">
         <v>42599</v>
       </c>
-      <c r="N28" s="45"/>
+      <c r="N28" s="42"/>
       <c r="O28" s="18">
         <v>200</v>
       </c>
@@ -2918,10 +2947,10 @@
       <c r="L29" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M29" s="44">
+      <c r="M29" s="42">
         <v>42600</v>
       </c>
-      <c r="N29" s="45"/>
+      <c r="N29" s="42"/>
       <c r="O29" s="18">
         <v>200</v>
       </c>
@@ -2936,10 +2965,10 @@
       <c r="L30" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M30" s="44">
+      <c r="M30" s="42">
         <v>42615</v>
       </c>
-      <c r="N30" s="45"/>
+      <c r="N30" s="42"/>
       <c r="O30" s="18">
         <v>90.57</v>
       </c>
@@ -2954,10 +2983,10 @@
       <c r="L31" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="M31" s="44">
+      <c r="M31" s="42">
         <v>42648</v>
       </c>
-      <c r="N31" s="45"/>
+      <c r="N31" s="42"/>
       <c r="O31" s="18">
         <v>200</v>
       </c>
@@ -2972,10 +3001,10 @@
       <c r="L32" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="M32" s="44">
+      <c r="M32" s="42">
         <v>42656</v>
       </c>
-      <c r="N32" s="45"/>
+      <c r="N32" s="42"/>
       <c r="O32" s="18">
         <v>200</v>
       </c>
@@ -2990,10 +3019,10 @@
       <c r="L33" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M33" s="44">
+      <c r="M33" s="42">
         <v>42656</v>
       </c>
-      <c r="N33" s="45"/>
+      <c r="N33" s="42"/>
       <c r="O33" s="18">
         <v>22</v>
       </c>
@@ -3008,10 +3037,10 @@
       <c r="L34" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M34" s="44">
+      <c r="M34" s="42">
         <v>42657</v>
       </c>
-      <c r="N34" s="45"/>
+      <c r="N34" s="42"/>
       <c r="O34" s="18">
         <v>90.57</v>
       </c>
@@ -3026,10 +3055,10 @@
       <c r="L35" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M35" s="44">
+      <c r="M35" s="42">
         <v>42651</v>
       </c>
-      <c r="N35" s="45"/>
+      <c r="N35" s="42"/>
       <c r="O35" s="18">
         <v>10</v>
       </c>
@@ -3038,16 +3067,16 @@
       </c>
     </row>
     <row r="36" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K36" s="59">
+      <c r="K36" s="36">
         <v>19</v>
       </c>
       <c r="L36" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M36" s="44">
+      <c r="M36" s="42">
         <v>42687</v>
       </c>
-      <c r="N36" s="45"/>
+      <c r="N36" s="42"/>
       <c r="O36" s="18">
         <v>90.42</v>
       </c>
@@ -3055,9 +3084,46 @@
         <v>28</v>
       </c>
     </row>
+    <row r="37" spans="11:16" x14ac:dyDescent="0.2">
+      <c r="K37" s="36">
+        <v>20</v>
+      </c>
+      <c r="L37" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="M37" s="42">
+        <v>42717</v>
+      </c>
+      <c r="N37" s="42"/>
+      <c r="O37" s="18">
+        <v>62.02</v>
+      </c>
+      <c r="P37" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="11:16" x14ac:dyDescent="0.2">
+      <c r="K38" s="36">
+        <v>21</v>
+      </c>
+      <c r="L38" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="M38" s="42">
+        <v>42726</v>
+      </c>
+      <c r="N38" s="42"/>
+      <c r="O38" s="18">
+        <v>100</v>
+      </c>
+      <c r="P38" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="M36:N36"/>
+  <mergeCells count="33">
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="M30:N30"/>
     <mergeCell ref="M15:N15"/>
     <mergeCell ref="M24:N24"/>
     <mergeCell ref="M16:N16"/>
@@ -3073,7 +3139,8 @@
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="P8:P9"/>
-    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="M38:N38"/>
     <mergeCell ref="D17:I17"/>
     <mergeCell ref="M28:N28"/>
     <mergeCell ref="M29:N29"/>
@@ -3083,13 +3150,942 @@
     <mergeCell ref="M21:N21"/>
     <mergeCell ref="M22:N22"/>
     <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="M35:N35"/>
     <mergeCell ref="M32:N32"/>
     <mergeCell ref="M33:N33"/>
     <mergeCell ref="M34:N34"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="M30:N30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" customWidth="1"/>
+    <col min="10" max="10" width="27.83203125" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" customWidth="1"/>
+    <col min="15" max="15" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" ht="45" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>42750</v>
+      </c>
+      <c r="B3" s="15">
+        <v>279.58</v>
+      </c>
+      <c r="C3" s="24">
+        <v>31.01</v>
+      </c>
+      <c r="D3" s="24">
+        <v>49.9</v>
+      </c>
+      <c r="E3" s="24">
+        <v>31.01</v>
+      </c>
+      <c r="F3" s="24">
+        <v>75.33</v>
+      </c>
+      <c r="G3" s="24">
+        <v>31.01</v>
+      </c>
+      <c r="H3" s="24">
+        <v>31.01</v>
+      </c>
+      <c r="I3" s="24">
+        <v>30.28</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>42781</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="24">
+        <f>SUM(C3:C14)</f>
+        <v>31.01</v>
+      </c>
+      <c r="N4" s="55">
+        <v>0</v>
+      </c>
+      <c r="O4" s="53">
+        <f>SUM(M4:M5)-N4+P4</f>
+        <v>225.49</v>
+      </c>
+      <c r="P4" s="63">
+        <v>144.58000000000001</v>
+      </c>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>42809</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="24">
+        <f>SUM(D3:D14)</f>
+        <v>49.9</v>
+      </c>
+      <c r="N5" s="56"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="64"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>42840</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="24">
+        <f>SUM(E3:E14)</f>
+        <v>31.01</v>
+      </c>
+      <c r="N6" s="24">
+        <f>SUM(O16,O19,O22,O26,O33,O35,O38)</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="19">
+        <f>M6-N6+P6</f>
+        <v>-29.429999999999996</v>
+      </c>
+      <c r="P6" s="20">
+        <v>-60.44</v>
+      </c>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>42870</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" s="24">
+        <f>SUM(F3:F14)</f>
+        <v>75.33</v>
+      </c>
+      <c r="N7" s="24">
+        <v>75.33</v>
+      </c>
+      <c r="O7" s="19">
+        <f>M7-N7</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="20">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>42901</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="24">
+        <f>SUM(G3:G14)</f>
+        <v>31.01</v>
+      </c>
+      <c r="N8" s="55">
+        <f>SUM(O17,O20:O21,O23:O24,O25,O27,O30,O34,O36,O37)</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="53">
+        <f>M8+M9-N8</f>
+        <v>62.02</v>
+      </c>
+      <c r="P8" s="61">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>42931</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="24">
+        <f>SUM(H3:H14)</f>
+        <v>31.01</v>
+      </c>
+      <c r="N9" s="56"/>
+      <c r="O9" s="54"/>
+      <c r="P9" s="62"/>
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>42962</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="24">
+        <f>SUM(I3:I14)</f>
+        <v>30.28</v>
+      </c>
+      <c r="N10" s="24">
+        <v>0</v>
+      </c>
+      <c r="O10" s="23">
+        <f>M10-N10+P10</f>
+        <v>151.87</v>
+      </c>
+      <c r="P10" s="65">
+        <v>121.59</v>
+      </c>
+      <c r="Q10" s="1"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>42993</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>43023</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="1:17" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>43054</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" spans="1:17" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>43084</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="47"/>
+      <c r="P14" s="47"/>
+    </row>
+    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="M15" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="N15" s="47"/>
+      <c r="O15" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="P15" s="35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="3">
+        <v>1</v>
+      </c>
+      <c r="L16" s="11"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="42"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="3"/>
+    </row>
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="3">
+        <v>2</v>
+      </c>
+      <c r="L17" s="11"/>
+      <c r="M17" s="42"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="3"/>
+    </row>
+    <row r="18" spans="1:16" ht="30" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="3">
+        <v>3</v>
+      </c>
+      <c r="L18" s="11"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="3"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="24">
+        <f t="shared" ref="E19:E25" si="0">75/7</f>
+        <v>10.714285714285714</v>
+      </c>
+      <c r="F19" s="24">
+        <v>15</v>
+      </c>
+      <c r="G19" s="24">
+        <v>5.3</v>
+      </c>
+      <c r="H19" s="25">
+        <f t="shared" ref="H19:H25" si="1">SUM(E19:G19)</f>
+        <v>31.014285714285716</v>
+      </c>
+      <c r="I19" s="25"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="3">
+        <v>4</v>
+      </c>
+      <c r="L19" s="11"/>
+      <c r="M19" s="42"/>
+      <c r="N19" s="42"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="3"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="24">
+        <f t="shared" si="0"/>
+        <v>10.714285714285714</v>
+      </c>
+      <c r="F20" s="25">
+        <v>30</v>
+      </c>
+      <c r="G20" s="25">
+        <v>9.19</v>
+      </c>
+      <c r="H20" s="25">
+        <f t="shared" si="1"/>
+        <v>49.904285714285713</v>
+      </c>
+      <c r="I20" s="25"/>
+      <c r="K20" s="3">
+        <v>5</v>
+      </c>
+      <c r="L20" s="11"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="3"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="24">
+        <f t="shared" si="0"/>
+        <v>10.714285714285714</v>
+      </c>
+      <c r="F21" s="25">
+        <v>15</v>
+      </c>
+      <c r="G21" s="25">
+        <v>5.3</v>
+      </c>
+      <c r="H21" s="25">
+        <f t="shared" si="1"/>
+        <v>31.014285714285716</v>
+      </c>
+      <c r="I21" s="25"/>
+      <c r="K21" s="3">
+        <v>6</v>
+      </c>
+      <c r="L21" s="11"/>
+      <c r="M21" s="42"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="3"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="24">
+        <f t="shared" si="0"/>
+        <v>10.714285714285714</v>
+      </c>
+      <c r="F22" s="25">
+        <v>15</v>
+      </c>
+      <c r="G22" s="25">
+        <v>49.62</v>
+      </c>
+      <c r="H22" s="25">
+        <f t="shared" si="1"/>
+        <v>75.334285714285713</v>
+      </c>
+      <c r="I22" s="25"/>
+      <c r="K22" s="3">
+        <v>7</v>
+      </c>
+      <c r="L22" s="11"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="3"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="24">
+        <f t="shared" si="0"/>
+        <v>10.714285714285714</v>
+      </c>
+      <c r="F23" s="25">
+        <v>15</v>
+      </c>
+      <c r="G23" s="25">
+        <v>4.57</v>
+      </c>
+      <c r="H23" s="25">
+        <f t="shared" si="1"/>
+        <v>30.284285714285716</v>
+      </c>
+      <c r="I23" s="25"/>
+      <c r="K23" s="3">
+        <v>8</v>
+      </c>
+      <c r="L23" s="11"/>
+      <c r="M23" s="42"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="3"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="24">
+        <f t="shared" si="0"/>
+        <v>10.714285714285714</v>
+      </c>
+      <c r="F24" s="24">
+        <v>15</v>
+      </c>
+      <c r="G24" s="25">
+        <v>5.3</v>
+      </c>
+      <c r="H24" s="25">
+        <f t="shared" si="1"/>
+        <v>31.014285714285716</v>
+      </c>
+      <c r="I24" s="25"/>
+      <c r="K24" s="3">
+        <v>9</v>
+      </c>
+      <c r="L24" s="11"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="3"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="24">
+        <f t="shared" si="0"/>
+        <v>10.714285714285714</v>
+      </c>
+      <c r="F25" s="24">
+        <v>15</v>
+      </c>
+      <c r="G25" s="25">
+        <v>5.3</v>
+      </c>
+      <c r="H25" s="25">
+        <f t="shared" si="1"/>
+        <v>31.014285714285716</v>
+      </c>
+      <c r="I25" s="25"/>
+      <c r="K25" s="3">
+        <v>10</v>
+      </c>
+      <c r="L25" s="11"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="3"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F26" s="1"/>
+      <c r="G26" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="30">
+        <f>SUM(H19:I25)</f>
+        <v>279.58</v>
+      </c>
+      <c r="K26" s="3">
+        <v>10</v>
+      </c>
+      <c r="L26" s="11"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="42"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="3"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F27" s="1"/>
+      <c r="K27" s="3">
+        <v>11</v>
+      </c>
+      <c r="L27" s="11"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="3"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F28" s="1"/>
+      <c r="K28" s="3">
+        <v>11</v>
+      </c>
+      <c r="L28" s="11"/>
+      <c r="M28" s="42"/>
+      <c r="N28" s="42"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="3"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K29" s="3">
+        <v>12</v>
+      </c>
+      <c r="L29" s="11"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="3"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K30" s="3">
+        <v>13</v>
+      </c>
+      <c r="L30" s="11"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="42"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="3"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K31" s="3">
+        <v>14</v>
+      </c>
+      <c r="L31" s="11"/>
+      <c r="M31" s="42"/>
+      <c r="N31" s="42"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="3"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K32" s="3">
+        <v>15</v>
+      </c>
+      <c r="L32" s="11"/>
+      <c r="M32" s="42"/>
+      <c r="N32" s="42"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="3"/>
+    </row>
+    <row r="33" spans="11:16" x14ac:dyDescent="0.2">
+      <c r="K33" s="3">
+        <v>16</v>
+      </c>
+      <c r="L33" s="11"/>
+      <c r="M33" s="42"/>
+      <c r="N33" s="42"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="3"/>
+    </row>
+    <row r="34" spans="11:16" x14ac:dyDescent="0.2">
+      <c r="K34" s="3">
+        <v>17</v>
+      </c>
+      <c r="L34" s="11"/>
+      <c r="M34" s="42"/>
+      <c r="N34" s="42"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="3"/>
+    </row>
+    <row r="35" spans="11:16" x14ac:dyDescent="0.2">
+      <c r="K35" s="3">
+        <v>18</v>
+      </c>
+      <c r="L35" s="11"/>
+      <c r="M35" s="42"/>
+      <c r="N35" s="42"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="3"/>
+    </row>
+    <row r="36" spans="11:16" x14ac:dyDescent="0.2">
+      <c r="K36" s="36">
+        <v>19</v>
+      </c>
+      <c r="L36" s="11"/>
+      <c r="M36" s="42"/>
+      <c r="N36" s="42"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="3"/>
+    </row>
+    <row r="37" spans="11:16" x14ac:dyDescent="0.2">
+      <c r="K37" s="36">
+        <v>20</v>
+      </c>
+      <c r="L37" s="11"/>
+      <c r="M37" s="42"/>
+      <c r="N37" s="42"/>
+      <c r="O37" s="18"/>
+      <c r="P37" s="3"/>
+    </row>
+    <row r="38" spans="11:16" x14ac:dyDescent="0.2">
+      <c r="K38" s="36">
+        <v>21</v>
+      </c>
+      <c r="L38" s="11"/>
+      <c r="M38" s="42"/>
+      <c r="N38" s="42"/>
+      <c r="O38" s="18"/>
+      <c r="P38" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="33">
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="K14:P14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="D17:I17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Feb ATT bill
</commit_message>
<xml_diff>
--- a/ATT_Bill.xlsx
+++ b/ATT_Bill.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="52">
   <si>
     <t>ATT Family Plan Bill Details</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>Previous Balance - 2016</t>
+  </si>
+  <si>
+    <t>Sankari - India calling extra $15</t>
   </si>
 </sst>
 </file>
@@ -212,7 +215,7 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,13 +258,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -458,7 +454,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -554,12 +550,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -569,31 +583,7 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -624,10 +614,14 @@
     <xf numFmtId="44" fontId="6" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="5" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="7" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="7" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -935,19 +929,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -1017,16 +1011,16 @@
       <c r="F3" s="8">
         <v>53.44</v>
       </c>
-      <c r="G3" s="37">
+      <c r="G3" s="44">
         <v>0</v>
       </c>
-      <c r="H3" s="37">
+      <c r="H3" s="44">
         <v>0</v>
       </c>
-      <c r="I3" s="37">
+      <c r="I3" s="44">
         <v>0</v>
       </c>
-      <c r="J3" s="37">
+      <c r="J3" s="44">
         <v>0</v>
       </c>
       <c r="K3" s="2"/>
@@ -1064,10 +1058,10 @@
       <c r="F4" s="8">
         <v>38.54</v>
       </c>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
       <c r="K4" s="2"/>
       <c r="L4" s="1"/>
       <c r="M4" s="2" t="s">
@@ -1077,11 +1071,11 @@
         <f>SUM(C3:C15)</f>
         <v>482.77999999999992</v>
       </c>
-      <c r="O4" s="37">
+      <c r="O4" s="44">
         <f>200+490.45</f>
         <v>690.45</v>
       </c>
-      <c r="P4" s="40">
+      <c r="P4" s="46">
         <f>N4+N5-O4</f>
         <v>-207.67000000000013</v>
       </c>
@@ -1106,10 +1100,10 @@
       <c r="F5" s="8">
         <v>38.229999999999997</v>
       </c>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
       <c r="K5" s="2"/>
       <c r="L5" s="1"/>
       <c r="M5" s="2" t="s">
@@ -1119,8 +1113,8 @@
         <f>SUM(J3:J15)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="39"/>
-      <c r="P5" s="41"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="47"/>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -1142,10 +1136,10 @@
       <c r="F6" s="8">
         <v>38.54</v>
       </c>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
       <c r="K6" s="2"/>
       <c r="L6" s="1"/>
       <c r="M6" s="2" t="s">
@@ -1184,10 +1178,10 @@
       <c r="F7" s="8">
         <v>38.69</v>
       </c>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
       <c r="K7" s="2"/>
       <c r="L7" s="1"/>
       <c r="M7" s="2" t="s">
@@ -1197,10 +1191,10 @@
         <f>SUM(F3:F15)</f>
         <v>491.13999999999993</v>
       </c>
-      <c r="O7" s="37">
+      <c r="O7" s="44">
         <v>1024.28</v>
       </c>
-      <c r="P7" s="40">
+      <c r="P7" s="46">
         <f>N7+N8-O7</f>
         <v>0</v>
       </c>
@@ -1225,10 +1219,10 @@
       <c r="F8" s="8">
         <v>39.799999999999997</v>
       </c>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
       <c r="K8" s="2"/>
       <c r="L8" s="1"/>
       <c r="M8" s="2" t="s">
@@ -1238,8 +1232,8 @@
         <f>SUM(E3:E14)</f>
         <v>533.14</v>
       </c>
-      <c r="O8" s="39"/>
-      <c r="P8" s="41"/>
+      <c r="O8" s="45"/>
+      <c r="P8" s="47"/>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
@@ -1261,10 +1255,10 @@
       <c r="F9" s="8">
         <v>38.69</v>
       </c>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
       <c r="K9" s="2"/>
       <c r="L9" s="1"/>
       <c r="M9" s="2" t="s">
@@ -1274,11 +1268,11 @@
         <f>SUM(G3:G15)</f>
         <v>175.34</v>
       </c>
-      <c r="O9" s="37">
+      <c r="O9" s="44">
         <f>113.35+61.99+51.99</f>
         <v>227.33</v>
       </c>
-      <c r="P9" s="40">
+      <c r="P9" s="46">
         <f>N9+N10-O9</f>
         <v>0</v>
       </c>
@@ -1304,10 +1298,10 @@
       <c r="F10" s="8">
         <v>39.14</v>
       </c>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
       <c r="K10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1319,8 +1313,8 @@
         <f>SUM(I3:I15)</f>
         <v>51.99</v>
       </c>
-      <c r="O10" s="39"/>
-      <c r="P10" s="41"/>
+      <c r="O10" s="45"/>
+      <c r="P10" s="47"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
@@ -1343,10 +1337,10 @@
       <c r="F11" s="8">
         <v>38.92</v>
       </c>
-      <c r="G11" s="39"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
       <c r="K11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1390,9 +1384,9 @@
       <c r="G12" s="8">
         <v>52.78</v>
       </c>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
       <c r="K12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1426,9 +1420,9 @@
       <c r="G13" s="8">
         <v>60.57</v>
       </c>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="38"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="48"/>
       <c r="K13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1474,7 +1468,7 @@
         <f>36.99+15</f>
         <v>51.99</v>
       </c>
-      <c r="J14" s="39"/>
+      <c r="J14" s="45"/>
       <c r="K14" s="2" t="s">
         <v>21</v>
       </c>
@@ -1525,14 +1519,14 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="44" t="s">
+      <c r="M15" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="N15" s="45"/>
-      <c r="O15" s="45"/>
-      <c r="P15" s="45"/>
-      <c r="Q15" s="45"/>
-      <c r="R15" s="46"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="41"/>
+      <c r="R15" s="42"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
@@ -1553,10 +1547,10 @@
       <c r="N16" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="O16" s="47" t="s">
+      <c r="O16" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="P16" s="47"/>
+      <c r="P16" s="43"/>
       <c r="Q16" s="32" t="s">
         <v>25</v>
       </c>
@@ -1583,10 +1577,10 @@
       <c r="N17" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O17" s="42">
+      <c r="O17" s="38">
         <v>42053</v>
       </c>
-      <c r="P17" s="42"/>
+      <c r="P17" s="38"/>
       <c r="Q17" s="10">
         <v>108</v>
       </c>
@@ -1612,10 +1606,10 @@
       <c r="N18" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="O18" s="42">
+      <c r="O18" s="38">
         <v>42086</v>
       </c>
-      <c r="P18" s="42"/>
+      <c r="P18" s="38"/>
       <c r="Q18" s="10">
         <v>200</v>
       </c>
@@ -1641,10 +1635,10 @@
       <c r="N19" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O19" s="42">
+      <c r="O19" s="38">
         <v>42111</v>
       </c>
-      <c r="P19" s="42"/>
+      <c r="P19" s="38"/>
       <c r="Q19" s="10">
         <v>100</v>
       </c>
@@ -1669,10 +1663,10 @@
       <c r="N20" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O20" s="42">
+      <c r="O20" s="38">
         <v>42214</v>
       </c>
-      <c r="P20" s="42"/>
+      <c r="P20" s="38"/>
       <c r="Q20" s="10">
         <v>160</v>
       </c>
@@ -1691,10 +1685,10 @@
       <c r="N21" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="O21" s="42">
+      <c r="O21" s="38">
         <v>42325</v>
       </c>
-      <c r="P21" s="42"/>
+      <c r="P21" s="38"/>
       <c r="Q21" s="10">
         <v>113.35</v>
       </c>
@@ -1713,10 +1707,10 @@
       <c r="N22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O22" s="42">
+      <c r="O22" s="38">
         <v>42325</v>
       </c>
-      <c r="P22" s="42"/>
+      <c r="P22" s="38"/>
       <c r="Q22" s="10">
         <v>80</v>
       </c>
@@ -1734,10 +1728,10 @@
       <c r="N23" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="O23" s="42">
+      <c r="O23" s="38">
         <v>42341</v>
       </c>
-      <c r="P23" s="42"/>
+      <c r="P23" s="38"/>
       <c r="Q23" s="10">
         <v>490.45</v>
       </c>
@@ -1753,10 +1747,10 @@
       <c r="N24" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="O24" s="42">
+      <c r="O24" s="38">
         <v>42364</v>
       </c>
-      <c r="P24" s="42"/>
+      <c r="P24" s="38"/>
       <c r="Q24" s="10">
         <v>113.98</v>
       </c>
@@ -1768,8 +1762,8 @@
       <c r="G25" s="1"/>
       <c r="M25" s="3"/>
       <c r="N25" s="11"/>
-      <c r="O25" s="42"/>
-      <c r="P25" s="42"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
       <c r="Q25" s="10"/>
       <c r="R25" s="3"/>
     </row>
@@ -1790,6 +1784,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="G3:G11"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="J3:J14"/>
+    <mergeCell ref="I3:I13"/>
+    <mergeCell ref="H3:H13"/>
     <mergeCell ref="O25:P25"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M15:R15"/>
@@ -1806,12 +1806,6 @@
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="O9:O10"/>
     <mergeCell ref="P9:P10"/>
-    <mergeCell ref="G3:G11"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="J3:J14"/>
-    <mergeCell ref="I3:I13"/>
-    <mergeCell ref="H3:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1824,7 +1818,7 @@
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView zoomScale="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O4" sqref="O4:O5"/>
     </sheetView>
   </sheetViews>
@@ -1848,18 +1842,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -2005,15 +1999,15 @@
         <f>SUM(C3:C14)</f>
         <v>375.303</v>
       </c>
-      <c r="N4" s="55">
+      <c r="N4" s="53">
         <f>207.67+O28+O31+O32</f>
         <v>807.67</v>
       </c>
-      <c r="O4" s="53">
+      <c r="O4" s="51">
         <f>SUM(M4:M5)-N4+P4</f>
         <v>144.58299999999997</v>
       </c>
-      <c r="P4" s="59">
+      <c r="P4" s="57">
         <v>0</v>
       </c>
       <c r="Q4" s="1"/>
@@ -2059,9 +2053,9 @@
         <f>SUM(D3:D14)</f>
         <v>576.94999999999993</v>
       </c>
-      <c r="N5" s="56"/>
-      <c r="O5" s="54"/>
-      <c r="P5" s="60"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="58"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.2">
@@ -2214,15 +2208,15 @@
         <f>SUM(G3:G14)</f>
         <v>620.59999999999991</v>
       </c>
-      <c r="N8" s="55">
+      <c r="N8" s="53">
         <f>SUM(O17,O20:O21,O23:O24,O25,O27,O30,O34,O36,O37)</f>
         <v>980.89999999999975</v>
       </c>
-      <c r="O8" s="57">
+      <c r="O8" s="55">
         <f>M8+M9-N8</f>
         <v>0</v>
       </c>
-      <c r="P8" s="61">
+      <c r="P8" s="59">
         <v>0</v>
       </c>
       <c r="Q8" s="1"/>
@@ -2268,9 +2262,9 @@
         <f>SUM(H3:H14)</f>
         <v>360.29999999999995</v>
       </c>
-      <c r="N9" s="56"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="62"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="60"/>
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" ht="120" x14ac:dyDescent="0.2">
@@ -2479,14 +2473,14 @@
       <c r="J14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K14" s="47" t="s">
+      <c r="K14" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="47"/>
-      <c r="P14" s="47"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
@@ -2505,10 +2499,10 @@
       <c r="L15" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="47" t="s">
+      <c r="M15" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="N15" s="47"/>
+      <c r="N15" s="43"/>
       <c r="O15" s="33" t="s">
         <v>25</v>
       </c>
@@ -2533,10 +2527,10 @@
       <c r="L16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M16" s="42">
+      <c r="M16" s="38">
         <v>42401</v>
       </c>
-      <c r="N16" s="42"/>
+      <c r="N16" s="38"/>
       <c r="O16" s="18">
         <v>100</v>
       </c>
@@ -2548,14 +2542,14 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="48" t="s">
+      <c r="D17" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="50"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="63"/>
       <c r="J17" s="1"/>
       <c r="K17" s="3">
         <v>2</v>
@@ -2563,10 +2557,10 @@
       <c r="L17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="42">
+      <c r="M17" s="38">
         <v>42402</v>
       </c>
-      <c r="N17" s="42"/>
+      <c r="N17" s="38"/>
       <c r="O17" s="18">
         <v>104.08</v>
       </c>
@@ -2603,10 +2597,10 @@
       <c r="L18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M18" s="42">
+      <c r="M18" s="38">
         <v>42402</v>
       </c>
-      <c r="N18" s="42"/>
+      <c r="N18" s="38"/>
       <c r="O18" s="18">
         <v>138.5</v>
       </c>
@@ -2643,10 +2637,10 @@
       <c r="L19" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M19" s="42">
+      <c r="M19" s="38">
         <v>42433</v>
       </c>
-      <c r="N19" s="42"/>
+      <c r="N19" s="38"/>
       <c r="O19" s="18">
         <v>20</v>
       </c>
@@ -2681,10 +2675,10 @@
       <c r="L20" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="42">
+      <c r="M20" s="38">
         <v>42433</v>
       </c>
-      <c r="N20" s="42"/>
+      <c r="N20" s="38"/>
       <c r="O20" s="18">
         <v>92.66</v>
       </c>
@@ -2719,10 +2713,10 @@
       <c r="L21" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M21" s="42">
+      <c r="M21" s="38">
         <v>42465</v>
       </c>
-      <c r="N21" s="42"/>
+      <c r="N21" s="38"/>
       <c r="O21" s="18">
         <v>92.66</v>
       </c>
@@ -2757,10 +2751,10 @@
       <c r="L22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M22" s="42">
+      <c r="M22" s="38">
         <v>42493</v>
       </c>
-      <c r="N22" s="42"/>
+      <c r="N22" s="38"/>
       <c r="O22" s="18">
         <v>100</v>
       </c>
@@ -2793,10 +2787,10 @@
       <c r="L23" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M23" s="42">
+      <c r="M23" s="38">
         <v>42494</v>
       </c>
-      <c r="N23" s="42"/>
+      <c r="N23" s="38"/>
       <c r="O23" s="18">
         <v>81.900000000000006</v>
       </c>
@@ -2829,10 +2823,10 @@
       <c r="L24" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M24" s="42">
+      <c r="M24" s="38">
         <v>42531</v>
       </c>
-      <c r="N24" s="42"/>
+      <c r="N24" s="38"/>
       <c r="O24" s="18">
         <v>93.52</v>
       </c>
@@ -2865,10 +2859,10 @@
       <c r="L25" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M25" s="42">
+      <c r="M25" s="38">
         <v>42558</v>
       </c>
-      <c r="N25" s="42"/>
+      <c r="N25" s="38"/>
       <c r="O25" s="18">
         <v>91.1</v>
       </c>
@@ -2891,10 +2885,10 @@
       <c r="L26" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M26" s="42">
+      <c r="M26" s="38">
         <v>42590</v>
       </c>
-      <c r="N26" s="42"/>
+      <c r="N26" s="38"/>
       <c r="O26" s="18">
         <v>100</v>
       </c>
@@ -2910,10 +2904,10 @@
       <c r="L27" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M27" s="42">
+      <c r="M27" s="38">
         <v>42598</v>
       </c>
-      <c r="N27" s="42"/>
+      <c r="N27" s="38"/>
       <c r="O27" s="18">
         <v>91.4</v>
       </c>
@@ -2929,10 +2923,10 @@
       <c r="L28" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="M28" s="42">
+      <c r="M28" s="38">
         <v>42599</v>
       </c>
-      <c r="N28" s="42"/>
+      <c r="N28" s="38"/>
       <c r="O28" s="18">
         <v>200</v>
       </c>
@@ -2947,10 +2941,10 @@
       <c r="L29" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M29" s="42">
+      <c r="M29" s="38">
         <v>42600</v>
       </c>
-      <c r="N29" s="42"/>
+      <c r="N29" s="38"/>
       <c r="O29" s="18">
         <v>200</v>
       </c>
@@ -2965,10 +2959,10 @@
       <c r="L30" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M30" s="42">
+      <c r="M30" s="38">
         <v>42615</v>
       </c>
-      <c r="N30" s="42"/>
+      <c r="N30" s="38"/>
       <c r="O30" s="18">
         <v>90.57</v>
       </c>
@@ -2983,10 +2977,10 @@
       <c r="L31" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="M31" s="42">
+      <c r="M31" s="38">
         <v>42648</v>
       </c>
-      <c r="N31" s="42"/>
+      <c r="N31" s="38"/>
       <c r="O31" s="18">
         <v>200</v>
       </c>
@@ -3001,10 +2995,10 @@
       <c r="L32" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="M32" s="42">
+      <c r="M32" s="38">
         <v>42656</v>
       </c>
-      <c r="N32" s="42"/>
+      <c r="N32" s="38"/>
       <c r="O32" s="18">
         <v>200</v>
       </c>
@@ -3019,10 +3013,10 @@
       <c r="L33" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M33" s="42">
+      <c r="M33" s="38">
         <v>42656</v>
       </c>
-      <c r="N33" s="42"/>
+      <c r="N33" s="38"/>
       <c r="O33" s="18">
         <v>22</v>
       </c>
@@ -3037,10 +3031,10 @@
       <c r="L34" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M34" s="42">
+      <c r="M34" s="38">
         <v>42657</v>
       </c>
-      <c r="N34" s="42"/>
+      <c r="N34" s="38"/>
       <c r="O34" s="18">
         <v>90.57</v>
       </c>
@@ -3055,10 +3049,10 @@
       <c r="L35" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M35" s="42">
+      <c r="M35" s="38">
         <v>42651</v>
       </c>
-      <c r="N35" s="42"/>
+      <c r="N35" s="38"/>
       <c r="O35" s="18">
         <v>10</v>
       </c>
@@ -3073,10 +3067,10 @@
       <c r="L36" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M36" s="42">
+      <c r="M36" s="38">
         <v>42687</v>
       </c>
-      <c r="N36" s="42"/>
+      <c r="N36" s="38"/>
       <c r="O36" s="18">
         <v>90.42</v>
       </c>
@@ -3091,10 +3085,10 @@
       <c r="L37" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M37" s="42">
+      <c r="M37" s="38">
         <v>42717</v>
       </c>
-      <c r="N37" s="42"/>
+      <c r="N37" s="38"/>
       <c r="O37" s="18">
         <v>62.02</v>
       </c>
@@ -3109,10 +3103,10 @@
       <c r="L38" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M38" s="42">
+      <c r="M38" s="38">
         <v>42726</v>
       </c>
-      <c r="N38" s="42"/>
+      <c r="N38" s="38"/>
       <c r="O38" s="18">
         <v>100</v>
       </c>
@@ -3122,23 +3116,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="K14:P14"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="P8:P9"/>
     <mergeCell ref="M37:N37"/>
     <mergeCell ref="M38:N38"/>
     <mergeCell ref="D17:I17"/>
@@ -3155,6 +3132,23 @@
     <mergeCell ref="M32:N32"/>
     <mergeCell ref="M33:N33"/>
     <mergeCell ref="M34:N34"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="K14:P14"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M20:N20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3166,7 +3160,7 @@
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3182,25 +3176,25 @@
     <col min="10" max="10" width="27.83203125" customWidth="1"/>
     <col min="11" max="11" width="12.83203125" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.1640625" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" customWidth="1"/>
+    <col min="14" max="14" width="13.1640625" customWidth="1"/>
     <col min="15" max="15" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -3247,7 +3241,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>42750</v>
       </c>
@@ -3300,31 +3294,50 @@
       <c r="A4" s="4">
         <v>42781</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="2"/>
+      <c r="B4" s="16">
+        <v>234.97</v>
+      </c>
+      <c r="C4" s="16">
+        <v>30.99</v>
+      </c>
+      <c r="D4" s="17">
+        <v>49.77</v>
+      </c>
+      <c r="E4" s="16">
+        <v>30.99</v>
+      </c>
+      <c r="F4" s="16">
+        <v>30.99</v>
+      </c>
+      <c r="G4" s="17">
+        <v>30.99</v>
+      </c>
+      <c r="H4" s="17">
+        <v>30.99</v>
+      </c>
+      <c r="I4" s="17">
+        <v>30.22</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="M4" s="24">
         <f>SUM(C3:C14)</f>
-        <v>31.01</v>
-      </c>
-      <c r="N4" s="55">
-        <v>0</v>
-      </c>
-      <c r="O4" s="53">
+        <v>62</v>
+      </c>
+      <c r="N4" s="53">
+        <f>SUM(O17)</f>
+        <v>200</v>
+      </c>
+      <c r="O4" s="51">
         <f>SUM(M4:M5)-N4+P4</f>
-        <v>225.49</v>
-      </c>
-      <c r="P4" s="63">
+        <v>106.25000000000003</v>
+      </c>
+      <c r="P4" s="57">
         <v>144.58000000000001</v>
       </c>
       <c r="Q4" s="1"/>
@@ -3348,11 +3361,11 @@
       </c>
       <c r="M5" s="24">
         <f>SUM(D3:D14)</f>
-        <v>49.9</v>
-      </c>
-      <c r="N5" s="56"/>
-      <c r="O5" s="54"/>
-      <c r="P5" s="64"/>
+        <v>99.67</v>
+      </c>
+      <c r="N5" s="54"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="58"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -3374,15 +3387,14 @@
       </c>
       <c r="M6" s="24">
         <f>SUM(E3:E14)</f>
-        <v>31.01</v>
+        <v>62</v>
       </c>
       <c r="N6" s="24">
-        <f>SUM(O16,O19,O22,O26,O33,O35,O38)</f>
         <v>0</v>
       </c>
       <c r="O6" s="19">
         <f>M6-N6+P6</f>
-        <v>-29.429999999999996</v>
+        <v>1.5600000000000023</v>
       </c>
       <c r="P6" s="20">
         <v>-60.44</v>
@@ -3408,10 +3420,10 @@
       </c>
       <c r="M7" s="24">
         <f>SUM(F3:F14)</f>
-        <v>75.33</v>
+        <v>106.32</v>
       </c>
       <c r="N7" s="24">
-        <v>75.33</v>
+        <v>106.32</v>
       </c>
       <c r="O7" s="19">
         <f>M7-N7</f>
@@ -3441,17 +3453,17 @@
       </c>
       <c r="M8" s="24">
         <f>SUM(G3:G14)</f>
-        <v>31.01</v>
-      </c>
-      <c r="N8" s="55">
-        <f>SUM(O17,O20:O21,O23:O24,O25,O27,O30,O34,O36,O37)</f>
-        <v>0</v>
-      </c>
-      <c r="O8" s="53">
+        <v>62</v>
+      </c>
+      <c r="N8" s="53">
+        <f>SUM(O16)</f>
+        <v>62.02</v>
+      </c>
+      <c r="O8" s="51">
         <f>M8+M9-N8</f>
-        <v>62.02</v>
-      </c>
-      <c r="P8" s="61">
+        <v>61.98</v>
+      </c>
+      <c r="P8" s="59">
         <v>0</v>
       </c>
       <c r="Q8" s="1"/>
@@ -3475,11 +3487,11 @@
       </c>
       <c r="M9" s="24">
         <f>SUM(H3:H14)</f>
-        <v>31.01</v>
-      </c>
-      <c r="N9" s="56"/>
-      <c r="O9" s="54"/>
-      <c r="P9" s="62"/>
+        <v>62</v>
+      </c>
+      <c r="N9" s="54"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="60"/>
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -3501,16 +3513,16 @@
       </c>
       <c r="M10" s="24">
         <f>SUM(I3:I14)</f>
-        <v>30.28</v>
+        <v>60.5</v>
       </c>
       <c r="N10" s="24">
         <v>0</v>
       </c>
       <c r="O10" s="23">
         <f>M10-N10+P10</f>
-        <v>151.87</v>
-      </c>
-      <c r="P10" s="65">
+        <v>182.09</v>
+      </c>
+      <c r="P10" s="37">
         <v>121.59</v>
       </c>
       <c r="Q10" s="1"/>
@@ -3593,14 +3605,14 @@
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="47" t="s">
+      <c r="K14" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="47"/>
-      <c r="P14" s="47"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
@@ -3619,10 +3631,10 @@
       <c r="L15" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="47" t="s">
+      <c r="M15" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="N15" s="47"/>
+      <c r="N15" s="43"/>
       <c r="O15" s="35" t="s">
         <v>25</v>
       </c>
@@ -3644,33 +3656,49 @@
       <c r="K16" s="3">
         <v>1</v>
       </c>
-      <c r="L16" s="11"/>
-      <c r="M16" s="42"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="3"/>
+      <c r="L16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="M16" s="38">
+        <v>42750</v>
+      </c>
+      <c r="N16" s="38"/>
+      <c r="O16" s="18">
+        <v>62.02</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="48" t="s">
+      <c r="D17" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="50"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="63"/>
       <c r="J17" s="1"/>
       <c r="K17" s="3">
         <v>2</v>
       </c>
-      <c r="L17" s="11"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="3"/>
+      <c r="L17" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="M17" s="38">
+        <v>42751</v>
+      </c>
+      <c r="N17" s="38"/>
+      <c r="O17" s="18">
+        <v>200</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="18" spans="1:16" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
@@ -3699,8 +3727,8 @@
         <v>3</v>
       </c>
       <c r="L18" s="11"/>
-      <c r="M18" s="42"/>
-      <c r="N18" s="42"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
       <c r="O18" s="18"/>
       <c r="P18" s="3"/>
     </row>
@@ -3719,11 +3747,11 @@
         <v>15</v>
       </c>
       <c r="G19" s="24">
-        <v>5.3</v>
+        <v>5.28</v>
       </c>
       <c r="H19" s="25">
         <f t="shared" ref="H19:H25" si="1">SUM(E19:G19)</f>
-        <v>31.014285714285716</v>
+        <v>30.994285714285716</v>
       </c>
       <c r="I19" s="25"/>
       <c r="J19" s="1"/>
@@ -3731,8 +3759,8 @@
         <v>4</v>
       </c>
       <c r="L19" s="11"/>
-      <c r="M19" s="42"/>
-      <c r="N19" s="42"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
       <c r="O19" s="18"/>
       <c r="P19" s="3"/>
     </row>
@@ -3750,19 +3778,19 @@
         <v>30</v>
       </c>
       <c r="G20" s="25">
-        <v>9.19</v>
+        <v>9.06</v>
       </c>
       <c r="H20" s="25">
         <f t="shared" si="1"/>
-        <v>49.904285714285713</v>
+        <v>49.774285714285718</v>
       </c>
       <c r="I20" s="25"/>
       <c r="K20" s="3">
         <v>5</v>
       </c>
       <c r="L20" s="11"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="42"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
       <c r="O20" s="18"/>
       <c r="P20" s="3"/>
     </row>
@@ -3780,19 +3808,19 @@
         <v>15</v>
       </c>
       <c r="G21" s="25">
-        <v>5.3</v>
+        <v>5.28</v>
       </c>
       <c r="H21" s="25">
         <f t="shared" si="1"/>
-        <v>31.014285714285716</v>
+        <v>30.994285714285716</v>
       </c>
       <c r="I21" s="25"/>
       <c r="K21" s="3">
         <v>6</v>
       </c>
       <c r="L21" s="11"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="42"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
       <c r="O21" s="18"/>
       <c r="P21" s="3"/>
     </row>
@@ -3810,19 +3838,19 @@
         <v>15</v>
       </c>
       <c r="G22" s="25">
-        <v>49.62</v>
+        <v>5.28</v>
       </c>
       <c r="H22" s="25">
         <f t="shared" si="1"/>
-        <v>75.334285714285713</v>
+        <v>30.994285714285716</v>
       </c>
       <c r="I22" s="25"/>
       <c r="K22" s="3">
         <v>7</v>
       </c>
       <c r="L22" s="11"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="42"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
       <c r="O22" s="18"/>
       <c r="P22" s="3"/>
     </row>
@@ -3838,19 +3866,19 @@
         <v>15</v>
       </c>
       <c r="G23" s="25">
-        <v>4.57</v>
+        <v>4.51</v>
       </c>
       <c r="H23" s="25">
         <f t="shared" si="1"/>
-        <v>30.284285714285716</v>
+        <v>30.224285714285713</v>
       </c>
       <c r="I23" s="25"/>
       <c r="K23" s="3">
         <v>8</v>
       </c>
       <c r="L23" s="11"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="42"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="38"/>
       <c r="O23" s="18"/>
       <c r="P23" s="3"/>
     </row>
@@ -3866,19 +3894,19 @@
         <v>15</v>
       </c>
       <c r="G24" s="25">
-        <v>5.3</v>
+        <v>5.28</v>
       </c>
       <c r="H24" s="25">
         <f t="shared" si="1"/>
-        <v>31.014285714285716</v>
+        <v>30.994285714285716</v>
       </c>
       <c r="I24" s="25"/>
       <c r="K24" s="3">
         <v>9</v>
       </c>
       <c r="L24" s="11"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="42"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="38"/>
       <c r="O24" s="18"/>
       <c r="P24" s="3"/>
     </row>
@@ -3894,19 +3922,19 @@
         <v>15</v>
       </c>
       <c r="G25" s="25">
-        <v>5.3</v>
+        <v>5.28</v>
       </c>
       <c r="H25" s="25">
         <f t="shared" si="1"/>
-        <v>31.014285714285716</v>
+        <v>30.994285714285716</v>
       </c>
       <c r="I25" s="25"/>
       <c r="K25" s="3">
         <v>10</v>
       </c>
       <c r="L25" s="11"/>
-      <c r="M25" s="42"/>
-      <c r="N25" s="42"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
       <c r="O25" s="18"/>
       <c r="P25" s="3"/>
     </row>
@@ -3917,14 +3945,14 @@
       </c>
       <c r="H26" s="30">
         <f>SUM(H19:I25)</f>
-        <v>279.58</v>
+        <v>234.97000000000003</v>
       </c>
       <c r="K26" s="3">
         <v>10</v>
       </c>
       <c r="L26" s="11"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="42"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
       <c r="O26" s="18"/>
       <c r="P26" s="3"/>
     </row>
@@ -3934,8 +3962,8 @@
         <v>11</v>
       </c>
       <c r="L27" s="11"/>
-      <c r="M27" s="42"/>
-      <c r="N27" s="42"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="38"/>
       <c r="O27" s="18"/>
       <c r="P27" s="3"/>
     </row>
@@ -3945,8 +3973,8 @@
         <v>11</v>
       </c>
       <c r="L28" s="11"/>
-      <c r="M28" s="42"/>
-      <c r="N28" s="42"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="38"/>
       <c r="O28" s="18"/>
       <c r="P28" s="3"/>
     </row>
@@ -3955,8 +3983,8 @@
         <v>12</v>
       </c>
       <c r="L29" s="11"/>
-      <c r="M29" s="42"/>
-      <c r="N29" s="42"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="38"/>
       <c r="O29" s="18"/>
       <c r="P29" s="3"/>
     </row>
@@ -3965,8 +3993,8 @@
         <v>13</v>
       </c>
       <c r="L30" s="11"/>
-      <c r="M30" s="42"/>
-      <c r="N30" s="42"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
       <c r="O30" s="18"/>
       <c r="P30" s="3"/>
     </row>
@@ -3975,8 +4003,8 @@
         <v>14</v>
       </c>
       <c r="L31" s="11"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="42"/>
+      <c r="M31" s="38"/>
+      <c r="N31" s="38"/>
       <c r="O31" s="18"/>
       <c r="P31" s="3"/>
     </row>
@@ -3985,8 +4013,8 @@
         <v>15</v>
       </c>
       <c r="L32" s="11"/>
-      <c r="M32" s="42"/>
-      <c r="N32" s="42"/>
+      <c r="M32" s="38"/>
+      <c r="N32" s="38"/>
       <c r="O32" s="18"/>
       <c r="P32" s="3"/>
     </row>
@@ -3995,8 +4023,8 @@
         <v>16</v>
       </c>
       <c r="L33" s="11"/>
-      <c r="M33" s="42"/>
-      <c r="N33" s="42"/>
+      <c r="M33" s="38"/>
+      <c r="N33" s="38"/>
       <c r="O33" s="18"/>
       <c r="P33" s="3"/>
     </row>
@@ -4005,8 +4033,8 @@
         <v>17</v>
       </c>
       <c r="L34" s="11"/>
-      <c r="M34" s="42"/>
-      <c r="N34" s="42"/>
+      <c r="M34" s="38"/>
+      <c r="N34" s="38"/>
       <c r="O34" s="18"/>
       <c r="P34" s="3"/>
     </row>
@@ -4015,8 +4043,8 @@
         <v>18</v>
       </c>
       <c r="L35" s="11"/>
-      <c r="M35" s="42"/>
-      <c r="N35" s="42"/>
+      <c r="M35" s="38"/>
+      <c r="N35" s="38"/>
       <c r="O35" s="18"/>
       <c r="P35" s="3"/>
     </row>
@@ -4025,8 +4053,8 @@
         <v>19</v>
       </c>
       <c r="L36" s="11"/>
-      <c r="M36" s="42"/>
-      <c r="N36" s="42"/>
+      <c r="M36" s="38"/>
+      <c r="N36" s="38"/>
       <c r="O36" s="18"/>
       <c r="P36" s="3"/>
     </row>
@@ -4035,8 +4063,8 @@
         <v>20</v>
       </c>
       <c r="L37" s="11"/>
-      <c r="M37" s="42"/>
-      <c r="N37" s="42"/>
+      <c r="M37" s="38"/>
+      <c r="N37" s="38"/>
       <c r="O37" s="18"/>
       <c r="P37" s="3"/>
     </row>
@@ -4045,13 +4073,38 @@
         <v>21</v>
       </c>
       <c r="L38" s="11"/>
-      <c r="M38" s="42"/>
-      <c r="N38" s="42"/>
+      <c r="M38" s="38"/>
+      <c r="N38" s="38"/>
       <c r="O38" s="18"/>
       <c r="P38" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="K14:P14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="D17:I17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M29:N29"/>
     <mergeCell ref="M37:N37"/>
     <mergeCell ref="M38:N38"/>
     <mergeCell ref="M31:N31"/>
@@ -4060,31 +4113,6 @@
     <mergeCell ref="M34:N34"/>
     <mergeCell ref="M35:N35"/>
     <mergeCell ref="M36:N36"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="K14:P14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="D17:I17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Apr and May 2017 billing
</commit_message>
<xml_diff>
--- a/ATT_Bill.xlsx
+++ b/ATT_Bill.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="53">
   <si>
     <t>ATT Family Plan Bill Details</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>Sankari - India calling extra $15</t>
+  </si>
+  <si>
+    <t>Previous + Current month Calculation</t>
   </si>
 </sst>
 </file>
@@ -497,7 +500,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -584,6 +587,86 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="3" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="5" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="5" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -602,19 +685,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -645,13 +722,7 @@
     <xf numFmtId="44" fontId="6" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="5" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -660,79 +731,23 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="5" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="5" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -742,16 +757,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="3" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1058,19 +1075,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
+      <c r="A1" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -1140,16 +1157,16 @@
       <c r="F3" s="8">
         <v>53.44</v>
       </c>
-      <c r="G3" s="40">
-        <v>0</v>
-      </c>
-      <c r="H3" s="40">
-        <v>0</v>
-      </c>
-      <c r="I3" s="40">
-        <v>0</v>
-      </c>
-      <c r="J3" s="40">
+      <c r="G3" s="61">
+        <v>0</v>
+      </c>
+      <c r="H3" s="61">
+        <v>0</v>
+      </c>
+      <c r="I3" s="61">
+        <v>0</v>
+      </c>
+      <c r="J3" s="61">
         <v>0</v>
       </c>
       <c r="K3" s="2"/>
@@ -1187,10 +1204,10 @@
       <c r="F4" s="8">
         <v>38.54</v>
       </c>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
       <c r="K4" s="2"/>
       <c r="L4" s="1"/>
       <c r="M4" s="2" t="s">
@@ -1200,11 +1217,11 @@
         <f>SUM(C3:C15)</f>
         <v>482.77999999999992</v>
       </c>
-      <c r="O4" s="40">
+      <c r="O4" s="61">
         <f>200+490.45</f>
         <v>690.45</v>
       </c>
-      <c r="P4" s="42">
+      <c r="P4" s="64">
         <f>N4+N5-O4</f>
         <v>-207.67000000000013</v>
       </c>
@@ -1229,10 +1246,10 @@
       <c r="F5" s="8">
         <v>38.229999999999997</v>
       </c>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
       <c r="K5" s="2"/>
       <c r="L5" s="1"/>
       <c r="M5" s="2" t="s">
@@ -1242,8 +1259,8 @@
         <f>SUM(J3:J15)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="41"/>
-      <c r="P5" s="43"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="65"/>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -1265,10 +1282,10 @@
       <c r="F6" s="8">
         <v>38.54</v>
       </c>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
       <c r="K6" s="2"/>
       <c r="L6" s="1"/>
       <c r="M6" s="2" t="s">
@@ -1307,10 +1324,10 @@
       <c r="F7" s="8">
         <v>38.69</v>
       </c>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
       <c r="K7" s="2"/>
       <c r="L7" s="1"/>
       <c r="M7" s="2" t="s">
@@ -1320,10 +1337,10 @@
         <f>SUM(F3:F15)</f>
         <v>491.13999999999993</v>
       </c>
-      <c r="O7" s="40">
+      <c r="O7" s="61">
         <v>1024.28</v>
       </c>
-      <c r="P7" s="42">
+      <c r="P7" s="64">
         <f>N7+N8-O7</f>
         <v>0</v>
       </c>
@@ -1348,10 +1365,10 @@
       <c r="F8" s="8">
         <v>39.799999999999997</v>
       </c>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
       <c r="K8" s="2"/>
       <c r="L8" s="1"/>
       <c r="M8" s="2" t="s">
@@ -1361,8 +1378,8 @@
         <f>SUM(E3:E14)</f>
         <v>533.14</v>
       </c>
-      <c r="O8" s="41"/>
-      <c r="P8" s="43"/>
+      <c r="O8" s="63"/>
+      <c r="P8" s="65"/>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
@@ -1384,10 +1401,10 @@
       <c r="F9" s="8">
         <v>38.69</v>
       </c>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
       <c r="K9" s="2"/>
       <c r="L9" s="1"/>
       <c r="M9" s="2" t="s">
@@ -1397,11 +1414,11 @@
         <f>SUM(G3:G15)</f>
         <v>175.34</v>
       </c>
-      <c r="O9" s="40">
+      <c r="O9" s="61">
         <f>113.35+61.99+51.99</f>
         <v>227.33</v>
       </c>
-      <c r="P9" s="42">
+      <c r="P9" s="64">
         <f>N9+N10-O9</f>
         <v>0</v>
       </c>
@@ -1427,10 +1444,10 @@
       <c r="F10" s="8">
         <v>39.14</v>
       </c>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
       <c r="K10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1442,8 +1459,8 @@
         <f>SUM(I3:I15)</f>
         <v>51.99</v>
       </c>
-      <c r="O10" s="41"/>
-      <c r="P10" s="43"/>
+      <c r="O10" s="63"/>
+      <c r="P10" s="65"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
@@ -1466,10 +1483,10 @@
       <c r="F11" s="8">
         <v>38.92</v>
       </c>
-      <c r="G11" s="41"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
       <c r="K11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1513,9 +1530,9 @@
       <c r="G12" s="8">
         <v>52.78</v>
       </c>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
       <c r="K12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1549,9 +1566,9 @@
       <c r="G13" s="8">
         <v>60.57</v>
       </c>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="44"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="62"/>
       <c r="K13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1597,7 +1614,7 @@
         <f>36.99+15</f>
         <v>51.99</v>
       </c>
-      <c r="J14" s="41"/>
+      <c r="J14" s="63"/>
       <c r="K14" s="2" t="s">
         <v>21</v>
       </c>
@@ -1648,14 +1665,14 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="36" t="s">
+      <c r="M15" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="38"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="69"/>
+      <c r="Q15" s="69"/>
+      <c r="R15" s="70"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
@@ -1676,10 +1693,10 @@
       <c r="N16" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="O16" s="39" t="s">
+      <c r="O16" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="P16" s="39"/>
+      <c r="P16" s="71"/>
       <c r="Q16" s="33" t="s">
         <v>25</v>
       </c>
@@ -1706,10 +1723,10 @@
       <c r="N17" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O17" s="34">
+      <c r="O17" s="66">
         <v>42053</v>
       </c>
-      <c r="P17" s="34"/>
+      <c r="P17" s="66"/>
       <c r="Q17" s="10">
         <v>108</v>
       </c>
@@ -1735,10 +1752,10 @@
       <c r="N18" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="O18" s="34">
+      <c r="O18" s="66">
         <v>42086</v>
       </c>
-      <c r="P18" s="34"/>
+      <c r="P18" s="66"/>
       <c r="Q18" s="10">
         <v>200</v>
       </c>
@@ -1764,10 +1781,10 @@
       <c r="N19" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O19" s="34">
+      <c r="O19" s="66">
         <v>42111</v>
       </c>
-      <c r="P19" s="34"/>
+      <c r="P19" s="66"/>
       <c r="Q19" s="10">
         <v>100</v>
       </c>
@@ -1792,10 +1809,10 @@
       <c r="N20" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O20" s="34">
+      <c r="O20" s="66">
         <v>42214</v>
       </c>
-      <c r="P20" s="34"/>
+      <c r="P20" s="66"/>
       <c r="Q20" s="10">
         <v>160</v>
       </c>
@@ -1814,10 +1831,10 @@
       <c r="N21" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="O21" s="34">
+      <c r="O21" s="66">
         <v>42325</v>
       </c>
-      <c r="P21" s="34"/>
+      <c r="P21" s="66"/>
       <c r="Q21" s="10">
         <v>113.35</v>
       </c>
@@ -1836,10 +1853,10 @@
       <c r="N22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O22" s="34">
+      <c r="O22" s="66">
         <v>42325</v>
       </c>
-      <c r="P22" s="34"/>
+      <c r="P22" s="66"/>
       <c r="Q22" s="10">
         <v>80</v>
       </c>
@@ -1857,10 +1874,10 @@
       <c r="N23" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="O23" s="34">
+      <c r="O23" s="66">
         <v>42341</v>
       </c>
-      <c r="P23" s="34"/>
+      <c r="P23" s="66"/>
       <c r="Q23" s="10">
         <v>490.45</v>
       </c>
@@ -1876,10 +1893,10 @@
       <c r="N24" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="O24" s="34">
+      <c r="O24" s="66">
         <v>42364</v>
       </c>
-      <c r="P24" s="34"/>
+      <c r="P24" s="66"/>
       <c r="Q24" s="10">
         <v>113.98</v>
       </c>
@@ -1891,8 +1908,8 @@
       <c r="G25" s="1"/>
       <c r="M25" s="3"/>
       <c r="N25" s="11"/>
-      <c r="O25" s="34"/>
-      <c r="P25" s="34"/>
+      <c r="O25" s="66"/>
+      <c r="P25" s="66"/>
       <c r="Q25" s="10"/>
       <c r="R25" s="3"/>
     </row>
@@ -1913,12 +1930,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="G3:G11"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="J3:J14"/>
-    <mergeCell ref="I3:I13"/>
-    <mergeCell ref="H3:H13"/>
     <mergeCell ref="O25:P25"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="M15:R15"/>
@@ -1935,6 +1946,12 @@
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="O9:O10"/>
     <mergeCell ref="P9:P10"/>
+    <mergeCell ref="G3:G11"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="J3:J14"/>
+    <mergeCell ref="I3:I13"/>
+    <mergeCell ref="H3:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1971,18 +1988,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
+      <c r="A1" s="75" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -2128,15 +2145,15 @@
         <f>SUM(C3:C14)</f>
         <v>375.303</v>
       </c>
-      <c r="N4" s="49">
+      <c r="N4" s="79">
         <f>207.67+O28+O31+O32</f>
         <v>807.67</v>
       </c>
-      <c r="O4" s="47">
+      <c r="O4" s="77">
         <f>SUM(M4:M5)-N4+P4</f>
         <v>144.58299999999997</v>
       </c>
-      <c r="P4" s="53">
+      <c r="P4" s="83">
         <v>0</v>
       </c>
       <c r="Q4" s="1"/>
@@ -2182,9 +2199,9 @@
         <f>SUM(D3:D14)</f>
         <v>576.94999999999993</v>
       </c>
-      <c r="N5" s="50"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="54"/>
+      <c r="N5" s="80"/>
+      <c r="O5" s="78"/>
+      <c r="P5" s="84"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.2">
@@ -2337,15 +2354,15 @@
         <f>SUM(G3:G14)</f>
         <v>620.59999999999991</v>
       </c>
-      <c r="N8" s="49">
+      <c r="N8" s="79">
         <f>SUM(O17,O20:O21,O23:O24,O25,O27,O30,O34,O36,O37)</f>
         <v>980.89999999999975</v>
       </c>
-      <c r="O8" s="51">
+      <c r="O8" s="81">
         <f>M8+M9-N8</f>
         <v>0</v>
       </c>
-      <c r="P8" s="55">
+      <c r="P8" s="85">
         <v>0</v>
       </c>
       <c r="Q8" s="1"/>
@@ -2391,9 +2408,9 @@
         <f>SUM(H3:H14)</f>
         <v>360.29999999999995</v>
       </c>
-      <c r="N9" s="50"/>
-      <c r="O9" s="52"/>
-      <c r="P9" s="56"/>
+      <c r="N9" s="80"/>
+      <c r="O9" s="82"/>
+      <c r="P9" s="86"/>
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" ht="120" x14ac:dyDescent="0.2">
@@ -2602,14 +2619,14 @@
       <c r="J14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K14" s="39" t="s">
+      <c r="K14" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="39"/>
-      <c r="P14" s="39"/>
+      <c r="L14" s="71"/>
+      <c r="M14" s="71"/>
+      <c r="N14" s="71"/>
+      <c r="O14" s="71"/>
+      <c r="P14" s="71"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
@@ -2628,10 +2645,10 @@
       <c r="L15" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="39" t="s">
+      <c r="M15" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="N15" s="39"/>
+      <c r="N15" s="71"/>
       <c r="O15" s="33" t="s">
         <v>25</v>
       </c>
@@ -2656,10 +2673,10 @@
       <c r="L16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M16" s="34">
+      <c r="M16" s="66">
         <v>42401</v>
       </c>
-      <c r="N16" s="34"/>
+      <c r="N16" s="66"/>
       <c r="O16" s="18">
         <v>100</v>
       </c>
@@ -2671,14 +2688,14 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="57" t="s">
+      <c r="D17" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="59"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="74"/>
       <c r="J17" s="1"/>
       <c r="K17" s="3">
         <v>2</v>
@@ -2686,10 +2703,10 @@
       <c r="L17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="34">
+      <c r="M17" s="66">
         <v>42402</v>
       </c>
-      <c r="N17" s="34"/>
+      <c r="N17" s="66"/>
       <c r="O17" s="18">
         <v>104.08</v>
       </c>
@@ -2726,10 +2743,10 @@
       <c r="L18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M18" s="34">
+      <c r="M18" s="66">
         <v>42402</v>
       </c>
-      <c r="N18" s="34"/>
+      <c r="N18" s="66"/>
       <c r="O18" s="18">
         <v>138.5</v>
       </c>
@@ -2766,10 +2783,10 @@
       <c r="L19" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M19" s="34">
+      <c r="M19" s="66">
         <v>42433</v>
       </c>
-      <c r="N19" s="34"/>
+      <c r="N19" s="66"/>
       <c r="O19" s="18">
         <v>20</v>
       </c>
@@ -2804,10 +2821,10 @@
       <c r="L20" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="34">
+      <c r="M20" s="66">
         <v>42433</v>
       </c>
-      <c r="N20" s="34"/>
+      <c r="N20" s="66"/>
       <c r="O20" s="18">
         <v>92.66</v>
       </c>
@@ -2842,10 +2859,10 @@
       <c r="L21" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M21" s="34">
+      <c r="M21" s="66">
         <v>42465</v>
       </c>
-      <c r="N21" s="34"/>
+      <c r="N21" s="66"/>
       <c r="O21" s="18">
         <v>92.66</v>
       </c>
@@ -2880,10 +2897,10 @@
       <c r="L22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M22" s="34">
+      <c r="M22" s="66">
         <v>42493</v>
       </c>
-      <c r="N22" s="34"/>
+      <c r="N22" s="66"/>
       <c r="O22" s="18">
         <v>100</v>
       </c>
@@ -2916,10 +2933,10 @@
       <c r="L23" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M23" s="34">
+      <c r="M23" s="66">
         <v>42494</v>
       </c>
-      <c r="N23" s="34"/>
+      <c r="N23" s="66"/>
       <c r="O23" s="18">
         <v>81.900000000000006</v>
       </c>
@@ -2952,10 +2969,10 @@
       <c r="L24" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M24" s="34">
+      <c r="M24" s="66">
         <v>42531</v>
       </c>
-      <c r="N24" s="34"/>
+      <c r="N24" s="66"/>
       <c r="O24" s="18">
         <v>93.52</v>
       </c>
@@ -2988,10 +3005,10 @@
       <c r="L25" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M25" s="34">
+      <c r="M25" s="66">
         <v>42558</v>
       </c>
-      <c r="N25" s="34"/>
+      <c r="N25" s="66"/>
       <c r="O25" s="18">
         <v>91.1</v>
       </c>
@@ -3014,10 +3031,10 @@
       <c r="L26" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M26" s="34">
+      <c r="M26" s="66">
         <v>42590</v>
       </c>
-      <c r="N26" s="34"/>
+      <c r="N26" s="66"/>
       <c r="O26" s="18">
         <v>100</v>
       </c>
@@ -3033,10 +3050,10 @@
       <c r="L27" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M27" s="34">
+      <c r="M27" s="66">
         <v>42598</v>
       </c>
-      <c r="N27" s="34"/>
+      <c r="N27" s="66"/>
       <c r="O27" s="18">
         <v>91.4</v>
       </c>
@@ -3052,10 +3069,10 @@
       <c r="L28" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="M28" s="34">
+      <c r="M28" s="66">
         <v>42599</v>
       </c>
-      <c r="N28" s="34"/>
+      <c r="N28" s="66"/>
       <c r="O28" s="18">
         <v>200</v>
       </c>
@@ -3070,10 +3087,10 @@
       <c r="L29" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M29" s="34">
+      <c r="M29" s="66">
         <v>42600</v>
       </c>
-      <c r="N29" s="34"/>
+      <c r="N29" s="66"/>
       <c r="O29" s="18">
         <v>200</v>
       </c>
@@ -3088,10 +3105,10 @@
       <c r="L30" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M30" s="34">
+      <c r="M30" s="66">
         <v>42615</v>
       </c>
-      <c r="N30" s="34"/>
+      <c r="N30" s="66"/>
       <c r="O30" s="18">
         <v>90.57</v>
       </c>
@@ -3106,10 +3123,10 @@
       <c r="L31" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="M31" s="34">
+      <c r="M31" s="66">
         <v>42648</v>
       </c>
-      <c r="N31" s="34"/>
+      <c r="N31" s="66"/>
       <c r="O31" s="18">
         <v>200</v>
       </c>
@@ -3124,10 +3141,10 @@
       <c r="L32" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="M32" s="34">
+      <c r="M32" s="66">
         <v>42656</v>
       </c>
-      <c r="N32" s="34"/>
+      <c r="N32" s="66"/>
       <c r="O32" s="18">
         <v>200</v>
       </c>
@@ -3142,10 +3159,10 @@
       <c r="L33" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M33" s="34">
+      <c r="M33" s="66">
         <v>42656</v>
       </c>
-      <c r="N33" s="34"/>
+      <c r="N33" s="66"/>
       <c r="O33" s="18">
         <v>22</v>
       </c>
@@ -3160,10 +3177,10 @@
       <c r="L34" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M34" s="34">
+      <c r="M34" s="66">
         <v>42657</v>
       </c>
-      <c r="N34" s="34"/>
+      <c r="N34" s="66"/>
       <c r="O34" s="18">
         <v>90.57</v>
       </c>
@@ -3178,10 +3195,10 @@
       <c r="L35" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M35" s="34">
+      <c r="M35" s="66">
         <v>42651</v>
       </c>
-      <c r="N35" s="34"/>
+      <c r="N35" s="66"/>
       <c r="O35" s="18">
         <v>10</v>
       </c>
@@ -3196,10 +3213,10 @@
       <c r="L36" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M36" s="34">
+      <c r="M36" s="66">
         <v>42687</v>
       </c>
-      <c r="N36" s="34"/>
+      <c r="N36" s="66"/>
       <c r="O36" s="18">
         <v>90.42</v>
       </c>
@@ -3214,10 +3231,10 @@
       <c r="L37" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M37" s="34">
+      <c r="M37" s="66">
         <v>42717</v>
       </c>
-      <c r="N37" s="34"/>
+      <c r="N37" s="66"/>
       <c r="O37" s="18">
         <v>62.02</v>
       </c>
@@ -3232,10 +3249,10 @@
       <c r="L38" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M38" s="34">
+      <c r="M38" s="66">
         <v>42726</v>
       </c>
-      <c r="N38" s="34"/>
+      <c r="N38" s="66"/>
       <c r="O38" s="18">
         <v>100</v>
       </c>
@@ -3245,6 +3262,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="K14:P14"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="P8:P9"/>
     <mergeCell ref="M37:N37"/>
     <mergeCell ref="M38:N38"/>
     <mergeCell ref="D17:I17"/>
@@ -3261,23 +3295,6 @@
     <mergeCell ref="M32:N32"/>
     <mergeCell ref="M33:N33"/>
     <mergeCell ref="M34:N34"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="K14:P14"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M20:N20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3289,973 +3306,986 @@
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="63" customWidth="1"/>
-    <col min="2" max="2" width="12" style="63" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="63" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="63" customWidth="1"/>
-    <col min="5" max="6" width="11.5" style="63" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" style="63" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="63" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" style="63" customWidth="1"/>
-    <col min="10" max="10" width="27.83203125" style="63" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" style="63" customWidth="1"/>
-    <col min="12" max="12" width="15" style="63" customWidth="1"/>
-    <col min="13" max="13" width="12.1640625" style="63" customWidth="1"/>
-    <col min="14" max="14" width="13.1640625" style="63" customWidth="1"/>
-    <col min="15" max="15" width="10.1640625" style="63" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" style="63" customWidth="1"/>
-    <col min="17" max="16384" width="8.83203125" style="63"/>
+    <col min="1" max="1" width="9.6640625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="12" style="35" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="35" customWidth="1"/>
+    <col min="5" max="6" width="11.5" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="35" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="35" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" style="35" customWidth="1"/>
+    <col min="10" max="10" width="27.83203125" style="35" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" style="35" customWidth="1"/>
+    <col min="12" max="12" width="15" style="35" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" style="35" customWidth="1"/>
+    <col min="14" max="14" width="13.1640625" style="35" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" style="35" customWidth="1"/>
+    <col min="16" max="16" width="19.5" style="35" customWidth="1"/>
+    <col min="17" max="16384" width="8.83203125" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
+      <c r="A1" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="64" t="s">
+      <c r="E2" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="F2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="64" t="s">
+      <c r="G2" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="64" t="s">
+      <c r="H2" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="64" t="s">
+      <c r="J2" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
     </row>
     <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.2">
-      <c r="A3" s="65">
+      <c r="A3" s="37">
         <v>42750</v>
       </c>
-      <c r="B3" s="66">
+      <c r="B3" s="38">
         <v>279.58</v>
       </c>
-      <c r="C3" s="67">
+      <c r="C3" s="39">
         <v>31.01</v>
       </c>
-      <c r="D3" s="67">
+      <c r="D3" s="39">
         <v>49.9</v>
       </c>
-      <c r="E3" s="67">
+      <c r="E3" s="39">
         <v>31.01</v>
       </c>
-      <c r="F3" s="67">
+      <c r="F3" s="39">
         <v>75.33</v>
       </c>
-      <c r="G3" s="67">
+      <c r="G3" s="39">
         <v>31.01</v>
       </c>
-      <c r="H3" s="67">
+      <c r="H3" s="39">
         <v>31.01</v>
       </c>
-      <c r="I3" s="67">
+      <c r="I3" s="39">
         <v>30.28</v>
       </c>
-      <c r="J3" s="68" t="s">
+      <c r="J3" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="K3" s="62"/>
-      <c r="L3" s="69" t="s">
+      <c r="K3" s="34"/>
+      <c r="L3" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="69" t="s">
+      <c r="M3" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="69" t="s">
+      <c r="N3" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="69" t="s">
+      <c r="O3" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="69" t="s">
+      <c r="P3" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="Q3" s="62"/>
+      <c r="Q3" s="34"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="65">
+      <c r="A4" s="37">
         <v>42781</v>
       </c>
-      <c r="B4" s="70">
+      <c r="B4" s="42">
         <v>234.97</v>
       </c>
-      <c r="C4" s="70">
+      <c r="C4" s="42">
         <v>30.99</v>
       </c>
-      <c r="D4" s="71">
+      <c r="D4" s="43">
         <v>49.77</v>
       </c>
-      <c r="E4" s="70">
+      <c r="E4" s="42">
         <v>30.99</v>
       </c>
-      <c r="F4" s="70">
+      <c r="F4" s="42">
         <v>30.99</v>
       </c>
-      <c r="G4" s="71">
+      <c r="G4" s="43">
         <v>30.99</v>
       </c>
-      <c r="H4" s="71">
+      <c r="H4" s="43">
         <v>30.99</v>
       </c>
-      <c r="I4" s="71">
+      <c r="I4" s="43">
         <v>30.22</v>
       </c>
-      <c r="J4" s="68" t="s">
+      <c r="J4" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="K4" s="62"/>
-      <c r="L4" s="68" t="s">
+      <c r="K4" s="34"/>
+      <c r="L4" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="39">
+        <f>SUM(E3:E14)</f>
+        <v>163.58999999999997</v>
+      </c>
+      <c r="N4" s="39">
+        <f>SUM(O19)</f>
+        <v>150</v>
+      </c>
+      <c r="O4" s="44">
+        <f>M4-N4+P4</f>
+        <v>-46.850000000000023</v>
+      </c>
+      <c r="P4" s="45">
+        <v>-60.44</v>
+      </c>
+      <c r="Q4" s="34"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="37">
+        <v>42809</v>
+      </c>
+      <c r="B5" s="38">
+        <v>179.07</v>
+      </c>
+      <c r="C5" s="38">
+        <v>14.11</v>
+      </c>
+      <c r="D5" s="39">
+        <v>10.71</v>
+      </c>
+      <c r="E5" s="38">
+        <v>30.99</v>
+      </c>
+      <c r="F5" s="38">
+        <v>30.99</v>
+      </c>
+      <c r="G5" s="39">
+        <v>30.99</v>
+      </c>
+      <c r="H5" s="39">
+        <v>30.99</v>
+      </c>
+      <c r="I5" s="39">
+        <v>30.26</v>
+      </c>
+      <c r="J5" s="40"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="39">
+        <f>SUM(F3:F14)</f>
+        <v>207.91</v>
+      </c>
+      <c r="N5" s="39">
+        <v>207.91</v>
+      </c>
+      <c r="O5" s="44">
+        <f>M5-N5</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="34"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="37">
+        <v>42840</v>
+      </c>
+      <c r="B6" s="38">
+        <v>176.13</v>
+      </c>
+      <c r="C6" s="38">
+        <v>0</v>
+      </c>
+      <c r="D6" s="39">
+        <v>0</v>
+      </c>
+      <c r="E6" s="38">
+        <v>35.28</v>
+      </c>
+      <c r="F6" s="38">
+        <v>35.28</v>
+      </c>
+      <c r="G6" s="39">
+        <v>35.28</v>
+      </c>
+      <c r="H6" s="39">
+        <v>35.28</v>
+      </c>
+      <c r="I6" s="39">
+        <v>35.01</v>
+      </c>
+      <c r="J6" s="40"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" s="39">
+        <f>SUM(G3:G14)</f>
+        <v>163.58999999999997</v>
+      </c>
+      <c r="N6" s="100">
+        <f>SUM(O16,O18,O20)</f>
+        <v>185.98</v>
+      </c>
+      <c r="O6" s="102">
+        <f>M6+M7-N6</f>
+        <v>141.19999999999996</v>
+      </c>
+      <c r="P6" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="34"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="37">
+        <v>42870</v>
+      </c>
+      <c r="B7" s="38">
+        <v>176.33</v>
+      </c>
+      <c r="C7" s="38">
+        <v>0</v>
+      </c>
+      <c r="D7" s="39">
+        <v>0</v>
+      </c>
+      <c r="E7" s="38">
+        <v>35.32</v>
+      </c>
+      <c r="F7" s="38">
+        <v>35.32</v>
+      </c>
+      <c r="G7" s="38">
+        <v>35.32</v>
+      </c>
+      <c r="H7" s="38">
+        <v>35.32</v>
+      </c>
+      <c r="I7" s="39">
+        <v>35.049999999999997</v>
+      </c>
+      <c r="J7" s="40"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="39">
+        <f>SUM(H3:H14)</f>
+        <v>163.58999999999997</v>
+      </c>
+      <c r="N7" s="101"/>
+      <c r="O7" s="103"/>
+      <c r="P7" s="60"/>
+      <c r="Q7" s="34"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="37">
+        <v>42901</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38">
+        <v>0</v>
+      </c>
+      <c r="D8" s="39">
+        <v>0</v>
+      </c>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="39">
+        <f>SUM(I3:I14)</f>
+        <v>160.82</v>
+      </c>
+      <c r="N8" s="39">
+        <v>0</v>
+      </c>
+      <c r="O8" s="46">
+        <f>M8-N8+P8</f>
+        <v>282.40999999999997</v>
+      </c>
+      <c r="P8" s="47">
+        <v>121.59</v>
+      </c>
+      <c r="Q8" s="34"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="37">
+        <v>42931</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38">
+        <v>0</v>
+      </c>
+      <c r="D9" s="39">
+        <v>0</v>
+      </c>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="67">
+      <c r="M9" s="39">
         <f>SUM(C3:C14)</f>
         <v>76.11</v>
       </c>
-      <c r="N4" s="72">
+      <c r="N9" s="90">
         <f>SUM(O17)</f>
         <v>200</v>
       </c>
-      <c r="O4" s="73">
-        <f>SUM(M4:M5)-N4+P4</f>
+      <c r="O9" s="92">
+        <f>SUM(M9:M10)-N9+P9</f>
         <v>131.07000000000002</v>
       </c>
-      <c r="P4" s="74">
+      <c r="P9" s="94">
         <v>144.58000000000001</v>
       </c>
-      <c r="Q4" s="62"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="65">
-        <v>42809</v>
-      </c>
-      <c r="B5" s="66">
-        <v>179.07</v>
-      </c>
-      <c r="C5" s="66">
-        <v>14.11</v>
-      </c>
-      <c r="D5" s="67">
-        <v>10.71</v>
-      </c>
-      <c r="E5" s="66">
-        <v>30.99</v>
-      </c>
-      <c r="F5" s="66">
-        <v>30.99</v>
-      </c>
-      <c r="G5" s="67">
-        <v>30.99</v>
-      </c>
-      <c r="H5" s="67">
-        <v>30.99</v>
-      </c>
-      <c r="I5" s="67">
-        <v>30.26</v>
-      </c>
-      <c r="J5" s="68"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="68" t="s">
+      <c r="Q9" s="34"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="37">
+        <v>42962</v>
+      </c>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38">
+        <v>0</v>
+      </c>
+      <c r="D10" s="39">
+        <v>0</v>
+      </c>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="67">
+      <c r="M10" s="39">
         <f>SUM(D3:D14)</f>
         <v>110.38</v>
       </c>
-      <c r="N5" s="75"/>
-      <c r="O5" s="76"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="62"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="65">
-        <v>42840</v>
-      </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="67"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="68" t="s">
-        <v>4</v>
-      </c>
-      <c r="M6" s="67">
-        <f>SUM(E3:E14)</f>
-        <v>92.99</v>
-      </c>
-      <c r="N6" s="67">
-        <f>SUM(O19)</f>
-        <v>150</v>
-      </c>
-      <c r="O6" s="78">
-        <f>M6-N6+P6</f>
-        <v>-117.45</v>
-      </c>
-      <c r="P6" s="79">
-        <v>-60.44</v>
-      </c>
-      <c r="Q6" s="62"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="65">
-        <v>42870</v>
-      </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="68" t="s">
-        <v>6</v>
-      </c>
-      <c r="M7" s="67">
-        <f>SUM(F3:F14)</f>
-        <v>137.31</v>
-      </c>
-      <c r="N7" s="67">
-        <v>137.31</v>
-      </c>
-      <c r="O7" s="78">
-        <f>M7-N7</f>
-        <v>0</v>
-      </c>
-      <c r="P7" s="79">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="62"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="65">
-        <v>42901</v>
-      </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="68"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="68" t="s">
-        <v>7</v>
-      </c>
-      <c r="M8" s="67">
-        <f>SUM(G3:G14)</f>
-        <v>92.99</v>
-      </c>
-      <c r="N8" s="72">
-        <f>SUM(O16,O18)</f>
-        <v>124</v>
-      </c>
-      <c r="O8" s="73">
-        <f>M8+M9-N8</f>
-        <v>61.97999999999999</v>
-      </c>
-      <c r="P8" s="74">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="62"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="65">
-        <v>42931</v>
-      </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="68"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="68" t="s">
-        <v>9</v>
-      </c>
-      <c r="M9" s="67">
-        <f>SUM(H3:H14)</f>
-        <v>92.99</v>
-      </c>
-      <c r="N9" s="75"/>
-      <c r="O9" s="76"/>
-      <c r="P9" s="77"/>
-      <c r="Q9" s="62"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="65">
-        <v>42962</v>
-      </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="68"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="68" t="s">
-        <v>8</v>
-      </c>
-      <c r="M10" s="67">
-        <f>SUM(I3:I14)</f>
-        <v>90.76</v>
-      </c>
-      <c r="N10" s="67">
-        <v>0</v>
-      </c>
-      <c r="O10" s="80">
-        <f>M10-N10+P10</f>
-        <v>212.35000000000002</v>
-      </c>
-      <c r="P10" s="81">
-        <v>121.59</v>
-      </c>
-      <c r="Q10" s="62"/>
+      <c r="N10" s="91"/>
+      <c r="O10" s="93"/>
+      <c r="P10" s="95"/>
+      <c r="Q10" s="34"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="65">
+      <c r="A11" s="37">
         <v>42993</v>
       </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="66"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="68"/>
-      <c r="K11" s="62"/>
-      <c r="L11" s="62"/>
-      <c r="M11" s="62"/>
-      <c r="N11" s="62"/>
-      <c r="O11" s="62"/>
-      <c r="P11" s="62"/>
-      <c r="Q11" s="62"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38">
+        <v>0</v>
+      </c>
+      <c r="D11" s="39">
+        <v>0</v>
+      </c>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="34"/>
+      <c r="Q11" s="34"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="65">
+      <c r="A12" s="37">
         <v>43023</v>
       </c>
-      <c r="B12" s="66"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="62"/>
-      <c r="L12" s="62" t="s">
-        <v>20</v>
-      </c>
-      <c r="M12" s="62"/>
-      <c r="N12" s="82"/>
-      <c r="O12" s="62"/>
-      <c r="P12" s="62"/>
-      <c r="Q12" s="62"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38">
+        <v>0</v>
+      </c>
+      <c r="D12" s="39">
+        <v>0</v>
+      </c>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="34"/>
+      <c r="Q12" s="34"/>
     </row>
     <row r="13" spans="1:17" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="65">
+      <c r="A13" s="37">
         <v>43054</v>
       </c>
-      <c r="B13" s="67"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="62"/>
-      <c r="O13" s="62"/>
-      <c r="P13" s="62"/>
-      <c r="Q13" s="62"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="38">
+        <v>0</v>
+      </c>
+      <c r="D13" s="39">
+        <v>0</v>
+      </c>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="48"/>
     </row>
     <row r="14" spans="1:17" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="65">
+      <c r="A14" s="37">
         <v>43084</v>
       </c>
-      <c r="B14" s="67"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="67"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="83" t="s">
+      <c r="B14" s="39"/>
+      <c r="C14" s="38">
+        <v>0</v>
+      </c>
+      <c r="D14" s="39">
+        <v>0</v>
+      </c>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="83"/>
-      <c r="M14" s="83"/>
-      <c r="N14" s="83"/>
-      <c r="O14" s="83"/>
-      <c r="P14" s="83"/>
+      <c r="L14" s="96"/>
+      <c r="M14" s="96"/>
+      <c r="N14" s="96"/>
+      <c r="O14" s="96"/>
+      <c r="P14" s="96"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="62"/>
-      <c r="B15" s="62"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="84" t="s">
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="L15" s="84" t="s">
+      <c r="L15" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="83" t="s">
+      <c r="M15" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="N15" s="83"/>
-      <c r="O15" s="84" t="s">
+      <c r="N15" s="96"/>
+      <c r="O15" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="P15" s="84" t="s">
+      <c r="P15" s="49" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="62"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="85">
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="50">
         <v>1</v>
       </c>
-      <c r="L16" s="86" t="s">
+      <c r="L16" s="51" t="s">
         <v>7</v>
       </c>
       <c r="M16" s="87">
         <v>42750</v>
       </c>
       <c r="N16" s="87"/>
-      <c r="O16" s="88">
+      <c r="O16" s="52">
         <v>62.02</v>
       </c>
-      <c r="P16" s="85" t="s">
+      <c r="P16" s="50" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="62"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="89" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="90"/>
-      <c r="F17" s="90"/>
-      <c r="G17" s="90"/>
-      <c r="H17" s="90"/>
-      <c r="I17" s="91"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="85">
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="97" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="98"/>
+      <c r="F17" s="98"/>
+      <c r="G17" s="98"/>
+      <c r="H17" s="98"/>
+      <c r="I17" s="99"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="50">
         <v>2</v>
       </c>
-      <c r="L17" s="86" t="s">
+      <c r="L17" s="51" t="s">
         <v>3</v>
       </c>
       <c r="M17" s="87">
         <v>42751</v>
       </c>
       <c r="N17" s="87"/>
-      <c r="O17" s="88">
+      <c r="O17" s="52">
         <v>200</v>
       </c>
-      <c r="P17" s="85" t="s">
+      <c r="P17" s="50" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="30" x14ac:dyDescent="0.2">
-      <c r="A18" s="62"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="92" t="s">
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="93" t="s">
+      <c r="E18" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="92" t="s">
+      <c r="F18" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="92" t="s">
+      <c r="G18" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="H18" s="93" t="s">
+      <c r="H18" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="93" t="s">
+      <c r="I18" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="J18" s="62"/>
-      <c r="K18" s="85">
+      <c r="J18" s="34"/>
+      <c r="K18" s="50">
         <v>3</v>
       </c>
-      <c r="L18" s="86" t="s">
+      <c r="L18" s="51" t="s">
         <v>7</v>
       </c>
       <c r="M18" s="87">
         <v>42768</v>
       </c>
       <c r="N18" s="87"/>
-      <c r="O18" s="88">
+      <c r="O18" s="52">
         <v>61.98</v>
       </c>
-      <c r="P18" s="85" t="s">
+      <c r="P18" s="50" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="62"/>
-      <c r="B19" s="62"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="68" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="67">
-        <f t="shared" ref="E19:E25" si="0">75/7</f>
-        <v>10.714285714285714</v>
-      </c>
-      <c r="F19" s="67">
-        <v>3</v>
-      </c>
-      <c r="G19" s="67">
-        <v>0.4</v>
-      </c>
-      <c r="H19" s="94">
-        <f t="shared" ref="H19:H25" si="1">SUM(E19:G19)</f>
-        <v>14.114285714285714</v>
-      </c>
-      <c r="I19" s="94"/>
-      <c r="J19" s="62"/>
-      <c r="K19" s="85">
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="L19" s="86" t="s">
+      <c r="E19" s="39">
+        <v>30</v>
+      </c>
+      <c r="F19" s="55">
+        <v>30</v>
+      </c>
+      <c r="G19" s="55">
+        <f>5.28+5.32</f>
+        <v>10.600000000000001</v>
+      </c>
+      <c r="H19" s="55">
+        <f t="shared" ref="H19:H23" si="0">SUM(E19:G19)</f>
+        <v>70.599999999999994</v>
+      </c>
+      <c r="I19" s="55"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="50">
+        <v>4</v>
+      </c>
+      <c r="L19" s="51" t="s">
         <v>4</v>
       </c>
       <c r="M19" s="87">
         <v>42793</v>
       </c>
       <c r="N19" s="87"/>
-      <c r="O19" s="88">
+      <c r="O19" s="52">
         <v>150</v>
       </c>
-      <c r="P19" s="85" t="s">
+      <c r="P19" s="50" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B20" s="62"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="95" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="67">
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="39">
+        <v>30</v>
+      </c>
+      <c r="F20" s="55">
+        <v>30</v>
+      </c>
+      <c r="G20" s="55">
+        <f>5.28+5.32</f>
+        <v>10.600000000000001</v>
+      </c>
+      <c r="H20" s="55">
         <f t="shared" si="0"/>
-        <v>10.714285714285714</v>
-      </c>
-      <c r="F20" s="94">
-        <v>0</v>
-      </c>
-      <c r="G20" s="94">
-        <v>0</v>
-      </c>
-      <c r="H20" s="94">
-        <f t="shared" si="1"/>
-        <v>10.714285714285714</v>
-      </c>
-      <c r="I20" s="94"/>
-      <c r="K20" s="85">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="I20" s="55"/>
+      <c r="K20" s="50">
         <v>5</v>
       </c>
-      <c r="L20" s="86"/>
-      <c r="M20" s="87"/>
+      <c r="L20" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20" s="87">
+        <v>42797</v>
+      </c>
       <c r="N20" s="87"/>
-      <c r="O20" s="88"/>
-      <c r="P20" s="85"/>
+      <c r="O20" s="52">
+        <v>61.98</v>
+      </c>
+      <c r="P20" s="50" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B21" s="62"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="95" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="67">
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="39">
+        <v>30</v>
+      </c>
+      <c r="F21" s="55">
+        <v>30</v>
+      </c>
+      <c r="G21" s="55">
+        <f>5.01+5.05</f>
+        <v>10.059999999999999</v>
+      </c>
+      <c r="H21" s="55">
         <f t="shared" si="0"/>
-        <v>10.714285714285714</v>
-      </c>
-      <c r="F21" s="94">
-        <v>15</v>
-      </c>
-      <c r="G21" s="94">
-        <v>5.28</v>
-      </c>
-      <c r="H21" s="94">
-        <f t="shared" si="1"/>
-        <v>30.994285714285716</v>
-      </c>
-      <c r="I21" s="94"/>
-      <c r="K21" s="85">
+        <v>70.06</v>
+      </c>
+      <c r="I21" s="55"/>
+      <c r="K21" s="50">
         <v>6</v>
       </c>
-      <c r="L21" s="86"/>
+      <c r="L21" s="51"/>
       <c r="M21" s="87"/>
       <c r="N21" s="87"/>
-      <c r="O21" s="88"/>
-      <c r="P21" s="85"/>
+      <c r="O21" s="52"/>
+      <c r="P21" s="50"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B22" s="62"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="68" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="67">
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="39">
+        <v>30</v>
+      </c>
+      <c r="F22" s="39">
+        <v>30</v>
+      </c>
+      <c r="G22" s="55">
+        <v>10.6</v>
+      </c>
+      <c r="H22" s="55">
         <f t="shared" si="0"/>
-        <v>10.714285714285714</v>
-      </c>
-      <c r="F22" s="94">
-        <v>15</v>
-      </c>
-      <c r="G22" s="94">
-        <v>5.28</v>
-      </c>
-      <c r="H22" s="94">
-        <f t="shared" si="1"/>
-        <v>30.994285714285716</v>
-      </c>
-      <c r="I22" s="94"/>
-      <c r="K22" s="85">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="I22" s="55"/>
+      <c r="K22" s="50">
         <v>7</v>
       </c>
-      <c r="L22" s="86"/>
+      <c r="L22" s="51"/>
       <c r="M22" s="87"/>
       <c r="N22" s="87"/>
-      <c r="O22" s="88"/>
-      <c r="P22" s="85"/>
+      <c r="O22" s="52"/>
+      <c r="P22" s="50"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D23" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="67">
+      <c r="D23" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="39">
+        <v>30</v>
+      </c>
+      <c r="F23" s="39">
+        <v>30</v>
+      </c>
+      <c r="G23" s="55">
+        <v>10.6</v>
+      </c>
+      <c r="H23" s="55">
         <f t="shared" si="0"/>
-        <v>10.714285714285714</v>
-      </c>
-      <c r="F23" s="94">
-        <v>15</v>
-      </c>
-      <c r="G23" s="94">
-        <v>4.55</v>
-      </c>
-      <c r="H23" s="94">
-        <f t="shared" si="1"/>
-        <v>30.264285714285716</v>
-      </c>
-      <c r="I23" s="94"/>
-      <c r="K23" s="85">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="I23" s="55"/>
+      <c r="K23" s="50">
         <v>8</v>
       </c>
-      <c r="L23" s="86"/>
+      <c r="L23" s="51"/>
       <c r="M23" s="87"/>
       <c r="N23" s="87"/>
-      <c r="O23" s="88"/>
-      <c r="P23" s="85"/>
+      <c r="O23" s="52"/>
+      <c r="P23" s="50"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D24" s="68" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="67">
-        <f t="shared" si="0"/>
-        <v>10.714285714285714</v>
-      </c>
-      <c r="F24" s="67">
-        <v>15</v>
-      </c>
-      <c r="G24" s="94">
-        <v>5.28</v>
-      </c>
-      <c r="H24" s="94">
-        <f t="shared" si="1"/>
-        <v>30.994285714285716</v>
-      </c>
-      <c r="I24" s="94"/>
-      <c r="K24" s="85">
+      <c r="F24" s="34"/>
+      <c r="G24" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="58">
+        <f>SUM(H19:I23)</f>
+        <v>352.46000000000004</v>
+      </c>
+      <c r="K24" s="50">
         <v>9</v>
       </c>
-      <c r="L24" s="86"/>
+      <c r="L24" s="51"/>
       <c r="M24" s="87"/>
       <c r="N24" s="87"/>
-      <c r="O24" s="88"/>
-      <c r="P24" s="85"/>
+      <c r="O24" s="52"/>
+      <c r="P24" s="50"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D25" s="68" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="67">
-        <f t="shared" si="0"/>
-        <v>10.714285714285714</v>
-      </c>
-      <c r="F25" s="67">
-        <v>15</v>
-      </c>
-      <c r="G25" s="94">
-        <v>5.28</v>
-      </c>
-      <c r="H25" s="94">
-        <f t="shared" si="1"/>
-        <v>30.994285714285716</v>
-      </c>
-      <c r="I25" s="94"/>
-      <c r="K25" s="85">
+      <c r="F25" s="34"/>
+      <c r="K25" s="50">
         <v>10</v>
       </c>
-      <c r="L25" s="86"/>
+      <c r="L25" s="51"/>
       <c r="M25" s="87"/>
       <c r="N25" s="87"/>
-      <c r="O25" s="88"/>
-      <c r="P25" s="85"/>
+      <c r="O25" s="52"/>
+      <c r="P25" s="50"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="F26" s="62"/>
-      <c r="G26" s="96" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26" s="97">
-        <f>SUM(H19:I25)</f>
-        <v>179.07000000000002</v>
-      </c>
-      <c r="K26" s="85">
+      <c r="F26" s="34"/>
+      <c r="K26" s="50">
         <v>10</v>
       </c>
-      <c r="L26" s="86"/>
+      <c r="L26" s="51"/>
       <c r="M26" s="87"/>
       <c r="N26" s="87"/>
-      <c r="O26" s="88"/>
-      <c r="P26" s="85"/>
+      <c r="O26" s="52"/>
+      <c r="P26" s="50"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="F27" s="62"/>
-      <c r="K27" s="85">
+      <c r="K27" s="50">
         <v>11</v>
       </c>
-      <c r="L27" s="86"/>
+      <c r="L27" s="51"/>
       <c r="M27" s="87"/>
       <c r="N27" s="87"/>
-      <c r="O27" s="88"/>
-      <c r="P27" s="85"/>
+      <c r="O27" s="52"/>
+      <c r="P27" s="50"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="F28" s="62"/>
-      <c r="K28" s="85">
+      <c r="K28" s="50">
         <v>11</v>
       </c>
-      <c r="L28" s="86"/>
+      <c r="L28" s="51"/>
       <c r="M28" s="87"/>
       <c r="N28" s="87"/>
-      <c r="O28" s="88"/>
-      <c r="P28" s="85"/>
+      <c r="O28" s="52"/>
+      <c r="P28" s="50"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="K29" s="85">
+      <c r="K29" s="50">
         <v>12</v>
       </c>
-      <c r="L29" s="86"/>
+      <c r="L29" s="51"/>
       <c r="M29" s="87"/>
       <c r="N29" s="87"/>
-      <c r="O29" s="88"/>
-      <c r="P29" s="85"/>
+      <c r="O29" s="52"/>
+      <c r="P29" s="50"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="K30" s="85">
+      <c r="K30" s="50">
         <v>13</v>
       </c>
-      <c r="L30" s="86"/>
+      <c r="L30" s="51"/>
       <c r="M30" s="87"/>
       <c r="N30" s="87"/>
-      <c r="O30" s="88"/>
-      <c r="P30" s="85"/>
+      <c r="O30" s="52"/>
+      <c r="P30" s="50"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="K31" s="85">
+      <c r="K31" s="50">
         <v>14</v>
       </c>
-      <c r="L31" s="86"/>
+      <c r="L31" s="51"/>
       <c r="M31" s="87"/>
       <c r="N31" s="87"/>
-      <c r="O31" s="88"/>
-      <c r="P31" s="85"/>
+      <c r="O31" s="52"/>
+      <c r="P31" s="50"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="K32" s="85">
+      <c r="K32" s="50">
         <v>15</v>
       </c>
-      <c r="L32" s="86"/>
+      <c r="L32" s="51"/>
       <c r="M32" s="87"/>
       <c r="N32" s="87"/>
-      <c r="O32" s="88"/>
-      <c r="P32" s="85"/>
+      <c r="O32" s="52"/>
+      <c r="P32" s="50"/>
     </row>
     <row r="33" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K33" s="85">
+      <c r="K33" s="50">
         <v>16</v>
       </c>
-      <c r="L33" s="86"/>
+      <c r="L33" s="51"/>
       <c r="M33" s="87"/>
       <c r="N33" s="87"/>
-      <c r="O33" s="88"/>
-      <c r="P33" s="85"/>
+      <c r="O33" s="52"/>
+      <c r="P33" s="50"/>
     </row>
     <row r="34" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K34" s="85">
+      <c r="K34" s="50">
         <v>17</v>
       </c>
-      <c r="L34" s="86"/>
+      <c r="L34" s="51"/>
       <c r="M34" s="87"/>
       <c r="N34" s="87"/>
-      <c r="O34" s="88"/>
-      <c r="P34" s="85"/>
+      <c r="O34" s="52"/>
+      <c r="P34" s="50"/>
     </row>
     <row r="35" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K35" s="85">
+      <c r="K35" s="50">
         <v>18</v>
       </c>
-      <c r="L35" s="86"/>
+      <c r="L35" s="51"/>
       <c r="M35" s="87"/>
       <c r="N35" s="87"/>
-      <c r="O35" s="88"/>
-      <c r="P35" s="85"/>
+      <c r="O35" s="52"/>
+      <c r="P35" s="50"/>
     </row>
     <row r="36" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K36" s="85">
+      <c r="K36" s="50">
         <v>19</v>
       </c>
-      <c r="L36" s="86"/>
+      <c r="L36" s="51"/>
       <c r="M36" s="87"/>
       <c r="N36" s="87"/>
-      <c r="O36" s="88"/>
-      <c r="P36" s="85"/>
+      <c r="O36" s="52"/>
+      <c r="P36" s="50"/>
     </row>
     <row r="37" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K37" s="85">
+      <c r="K37" s="50">
         <v>20</v>
       </c>
-      <c r="L37" s="86"/>
+      <c r="L37" s="51"/>
       <c r="M37" s="87"/>
       <c r="N37" s="87"/>
-      <c r="O37" s="88"/>
-      <c r="P37" s="85"/>
+      <c r="O37" s="52"/>
+      <c r="P37" s="50"/>
     </row>
     <row r="38" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K38" s="85">
+      <c r="K38" s="50">
         <v>21</v>
       </c>
-      <c r="L38" s="86"/>
+      <c r="L38" s="51"/>
       <c r="M38" s="87"/>
       <c r="N38" s="87"/>
-      <c r="O38" s="88"/>
-      <c r="P38" s="85"/>
+      <c r="O38" s="52"/>
+      <c r="P38" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="K14:P14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="D17:I17"/>
-    <mergeCell ref="M17:N17"/>
+  <mergeCells count="32">
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M36:N36"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="M19:N19"/>
     <mergeCell ref="M20:N20"/>
@@ -4268,14 +4298,18 @@
     <mergeCell ref="M27:N27"/>
     <mergeCell ref="M28:N28"/>
     <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="K14:P14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="D17:I17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated June and July 2017 Bill
</commit_message>
<xml_diff>
--- a/ATT_Bill.xlsx
+++ b/ATT_Bill.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="53">
   <si>
     <t>ATT Family Plan Bill Details</t>
   </si>
@@ -3306,7 +3306,7 @@
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3474,7 +3474,7 @@
       </c>
       <c r="M4" s="39">
         <f>SUM(E3:E14)</f>
-        <v>163.58999999999997</v>
+        <v>234.22999999999996</v>
       </c>
       <c r="N4" s="39">
         <f>SUM(O19)</f>
@@ -3482,7 +3482,7 @@
       </c>
       <c r="O4" s="44">
         <f>M4-N4+P4</f>
-        <v>-46.850000000000023</v>
+        <v>23.789999999999964</v>
       </c>
       <c r="P4" s="45">
         <v>-60.44</v>
@@ -3524,10 +3524,10 @@
       </c>
       <c r="M5" s="39">
         <f>SUM(F3:F14)</f>
-        <v>207.91</v>
+        <v>278.55</v>
       </c>
       <c r="N5" s="39">
-        <v>207.91</v>
+        <v>278.55</v>
       </c>
       <c r="O5" s="44">
         <f>M5-N5</f>
@@ -3573,15 +3573,15 @@
       </c>
       <c r="M6" s="39">
         <f>SUM(G3:G14)</f>
-        <v>163.58999999999997</v>
+        <v>234.22999999999996</v>
       </c>
       <c r="N6" s="100">
-        <f>SUM(O16,O18,O20)</f>
-        <v>185.98</v>
+        <f>SUM(O16,O18,O20:O21)</f>
+        <v>327.17999999999995</v>
       </c>
       <c r="O6" s="102">
         <f>M6+M7-N6</f>
-        <v>141.19999999999996</v>
+        <v>141.27999999999997</v>
       </c>
       <c r="P6" s="59">
         <v>0</v>
@@ -3623,7 +3623,7 @@
       </c>
       <c r="M7" s="39">
         <f>SUM(H3:H14)</f>
-        <v>163.58999999999997</v>
+        <v>234.22999999999996</v>
       </c>
       <c r="N7" s="101"/>
       <c r="O7" s="103"/>
@@ -3634,18 +3634,30 @@
       <c r="A8" s="37">
         <v>42901</v>
       </c>
-      <c r="B8" s="38"/>
+      <c r="B8" s="38">
+        <v>176.33</v>
+      </c>
       <c r="C8" s="38">
         <v>0</v>
       </c>
       <c r="D8" s="39">
         <v>0</v>
       </c>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
+      <c r="E8" s="38">
+        <v>35.32</v>
+      </c>
+      <c r="F8" s="38">
+        <v>35.32</v>
+      </c>
+      <c r="G8" s="38">
+        <v>35.32</v>
+      </c>
+      <c r="H8" s="38">
+        <v>35.32</v>
+      </c>
+      <c r="I8" s="39">
+        <v>35.049999999999997</v>
+      </c>
       <c r="J8" s="40"/>
       <c r="K8" s="34"/>
       <c r="L8" s="40" t="s">
@@ -3653,14 +3665,14 @@
       </c>
       <c r="M8" s="39">
         <f>SUM(I3:I14)</f>
-        <v>160.82</v>
+        <v>230.92000000000002</v>
       </c>
       <c r="N8" s="39">
         <v>0</v>
       </c>
       <c r="O8" s="46">
         <f>M8-N8+P8</f>
-        <v>282.40999999999997</v>
+        <v>352.51</v>
       </c>
       <c r="P8" s="47">
         <v>121.59</v>
@@ -3671,18 +3683,30 @@
       <c r="A9" s="37">
         <v>42931</v>
       </c>
-      <c r="B9" s="38"/>
+      <c r="B9" s="38">
+        <v>176.33</v>
+      </c>
       <c r="C9" s="38">
         <v>0</v>
       </c>
       <c r="D9" s="39">
         <v>0</v>
       </c>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
+      <c r="E9" s="38">
+        <v>35.32</v>
+      </c>
+      <c r="F9" s="38">
+        <v>35.32</v>
+      </c>
+      <c r="G9" s="38">
+        <v>35.32</v>
+      </c>
+      <c r="H9" s="38">
+        <v>35.32</v>
+      </c>
+      <c r="I9" s="39">
+        <v>35.049999999999997</v>
+      </c>
       <c r="J9" s="40"/>
       <c r="K9" s="34"/>
       <c r="L9" s="40" t="s">
@@ -3966,12 +3990,12 @@
         <v>30</v>
       </c>
       <c r="G19" s="55">
-        <f>5.28+5.32</f>
-        <v>10.600000000000001</v>
+        <f>5.32*2</f>
+        <v>10.64</v>
       </c>
       <c r="H19" s="55">
         <f t="shared" ref="H19:H23" si="0">SUM(E19:G19)</f>
-        <v>70.599999999999994</v>
+        <v>70.64</v>
       </c>
       <c r="I19" s="55"/>
       <c r="J19" s="34"/>
@@ -4005,12 +4029,12 @@
         <v>30</v>
       </c>
       <c r="G20" s="55">
-        <f>5.28+5.32</f>
-        <v>10.600000000000001</v>
+        <f>5.32*2</f>
+        <v>10.64</v>
       </c>
       <c r="H20" s="55">
         <f t="shared" si="0"/>
-        <v>70.599999999999994</v>
+        <v>70.64</v>
       </c>
       <c r="I20" s="55"/>
       <c r="K20" s="50">
@@ -4043,21 +4067,27 @@
         <v>30</v>
       </c>
       <c r="G21" s="55">
-        <f>5.01+5.05</f>
-        <v>10.059999999999999</v>
+        <f>5.05*2</f>
+        <v>10.1</v>
       </c>
       <c r="H21" s="55">
         <f t="shared" si="0"/>
-        <v>70.06</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="I21" s="55"/>
       <c r="K21" s="50">
         <v>6</v>
       </c>
-      <c r="L21" s="51"/>
-      <c r="M21" s="87"/>
+      <c r="L21" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="M21" s="87">
+        <v>42858</v>
+      </c>
       <c r="N21" s="87"/>
-      <c r="O21" s="52"/>
+      <c r="O21" s="52">
+        <v>141.19999999999999</v>
+      </c>
       <c r="P21" s="50"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
@@ -4069,15 +4099,16 @@
       <c r="E22" s="39">
         <v>30</v>
       </c>
-      <c r="F22" s="39">
+      <c r="F22" s="55">
         <v>30</v>
       </c>
       <c r="G22" s="55">
-        <v>10.6</v>
+        <f>5.32*2</f>
+        <v>10.64</v>
       </c>
       <c r="H22" s="55">
         <f t="shared" si="0"/>
-        <v>70.599999999999994</v>
+        <v>70.64</v>
       </c>
       <c r="I22" s="55"/>
       <c r="K22" s="50">
@@ -4096,15 +4127,16 @@
       <c r="E23" s="39">
         <v>30</v>
       </c>
-      <c r="F23" s="39">
+      <c r="F23" s="55">
         <v>30</v>
       </c>
       <c r="G23" s="55">
-        <v>10.6</v>
+        <f>5.32*2</f>
+        <v>10.64</v>
       </c>
       <c r="H23" s="55">
         <f t="shared" si="0"/>
-        <v>70.599999999999994</v>
+        <v>70.64</v>
       </c>
       <c r="I23" s="55"/>
       <c r="K23" s="50">
@@ -4123,7 +4155,7 @@
       </c>
       <c r="H24" s="58">
         <f>SUM(H19:I23)</f>
-        <v>352.46000000000004</v>
+        <v>352.65999999999997</v>
       </c>
       <c r="K24" s="50">
         <v>9</v>

</xml_diff>

<commit_message>
updated 2017 and 2018 bill
</commit_message>
<xml_diff>
--- a/ATT_Bill.xlsx
+++ b/ATT_Bill.xlsx
@@ -1,38 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/girias/OneDrive/ATT_Bill/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4EC8FCB0-DBE5-EF46-9423-47268135CDF4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="32680" windowHeight="19120" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015" sheetId="1" r:id="rId1"/>
     <sheet name="2016" sheetId="2" r:id="rId2"/>
     <sheet name="2017" sheetId="3" r:id="rId3"/>
+    <sheet name="2018" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="58">
   <si>
     <t>ATT Family Plan Bill Details</t>
   </si>
@@ -207,11 +209,26 @@
   <si>
     <t>Previous + Current month Calculation</t>
   </si>
+  <si>
+    <t>Mugunthan India vacation</t>
+  </si>
+  <si>
+    <t>Previous Balance - 2017</t>
+  </si>
+  <si>
+    <t>Mugunthan Extra for new connection</t>
+  </si>
+  <si>
+    <t>Ravi</t>
+  </si>
+  <si>
+    <t>Allen</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
@@ -500,7 +517,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -652,6 +669,11 @@
     <xf numFmtId="44" fontId="3" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="5" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="5" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="5" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="5" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -767,6 +789,31 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1049,8 +1096,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -1075,19 +1122,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="67" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
+      <c r="A1" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -1157,16 +1204,16 @@
       <c r="F3" s="8">
         <v>53.44</v>
       </c>
-      <c r="G3" s="61">
-        <v>0</v>
-      </c>
-      <c r="H3" s="61">
-        <v>0</v>
-      </c>
-      <c r="I3" s="61">
-        <v>0</v>
-      </c>
-      <c r="J3" s="61">
+      <c r="G3" s="64">
+        <v>0</v>
+      </c>
+      <c r="H3" s="64">
+        <v>0</v>
+      </c>
+      <c r="I3" s="64">
+        <v>0</v>
+      </c>
+      <c r="J3" s="64">
         <v>0</v>
       </c>
       <c r="K3" s="2"/>
@@ -1204,10 +1251,10 @@
       <c r="F4" s="8">
         <v>38.54</v>
       </c>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
       <c r="K4" s="2"/>
       <c r="L4" s="1"/>
       <c r="M4" s="2" t="s">
@@ -1217,11 +1264,11 @@
         <f>SUM(C3:C15)</f>
         <v>482.77999999999992</v>
       </c>
-      <c r="O4" s="61">
+      <c r="O4" s="64">
         <f>200+490.45</f>
         <v>690.45</v>
       </c>
-      <c r="P4" s="64">
+      <c r="P4" s="67">
         <f>N4+N5-O4</f>
         <v>-207.67000000000013</v>
       </c>
@@ -1246,10 +1293,10 @@
       <c r="F5" s="8">
         <v>38.229999999999997</v>
       </c>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
       <c r="K5" s="2"/>
       <c r="L5" s="1"/>
       <c r="M5" s="2" t="s">
@@ -1259,8 +1306,8 @@
         <f>SUM(J3:J15)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="63"/>
-      <c r="P5" s="65"/>
+      <c r="O5" s="66"/>
+      <c r="P5" s="68"/>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -1282,10 +1329,10 @@
       <c r="F6" s="8">
         <v>38.54</v>
       </c>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
       <c r="K6" s="2"/>
       <c r="L6" s="1"/>
       <c r="M6" s="2" t="s">
@@ -1324,10 +1371,10 @@
       <c r="F7" s="8">
         <v>38.69</v>
       </c>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
       <c r="K7" s="2"/>
       <c r="L7" s="1"/>
       <c r="M7" s="2" t="s">
@@ -1337,10 +1384,10 @@
         <f>SUM(F3:F15)</f>
         <v>491.13999999999993</v>
       </c>
-      <c r="O7" s="61">
+      <c r="O7" s="64">
         <v>1024.28</v>
       </c>
-      <c r="P7" s="64">
+      <c r="P7" s="67">
         <f>N7+N8-O7</f>
         <v>0</v>
       </c>
@@ -1365,10 +1412,10 @@
       <c r="F8" s="8">
         <v>39.799999999999997</v>
       </c>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
       <c r="K8" s="2"/>
       <c r="L8" s="1"/>
       <c r="M8" s="2" t="s">
@@ -1378,8 +1425,8 @@
         <f>SUM(E3:E14)</f>
         <v>533.14</v>
       </c>
-      <c r="O8" s="63"/>
-      <c r="P8" s="65"/>
+      <c r="O8" s="66"/>
+      <c r="P8" s="68"/>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
@@ -1401,10 +1448,10 @@
       <c r="F9" s="8">
         <v>38.69</v>
       </c>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="62"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
       <c r="K9" s="2"/>
       <c r="L9" s="1"/>
       <c r="M9" s="2" t="s">
@@ -1414,11 +1461,11 @@
         <f>SUM(G3:G15)</f>
         <v>175.34</v>
       </c>
-      <c r="O9" s="61">
+      <c r="O9" s="64">
         <f>113.35+61.99+51.99</f>
         <v>227.33</v>
       </c>
-      <c r="P9" s="64">
+      <c r="P9" s="67">
         <f>N9+N10-O9</f>
         <v>0</v>
       </c>
@@ -1444,10 +1491,10 @@
       <c r="F10" s="8">
         <v>39.14</v>
       </c>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
       <c r="K10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1459,8 +1506,8 @@
         <f>SUM(I3:I15)</f>
         <v>51.99</v>
       </c>
-      <c r="O10" s="63"/>
-      <c r="P10" s="65"/>
+      <c r="O10" s="66"/>
+      <c r="P10" s="68"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
@@ -1483,10 +1530,10 @@
       <c r="F11" s="8">
         <v>38.92</v>
       </c>
-      <c r="G11" s="63"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="62"/>
-      <c r="J11" s="62"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="65"/>
       <c r="K11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1530,9 +1577,9 @@
       <c r="G12" s="8">
         <v>52.78</v>
       </c>
-      <c r="H12" s="62"/>
-      <c r="I12" s="62"/>
-      <c r="J12" s="62"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
       <c r="K12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1566,9 +1613,9 @@
       <c r="G13" s="8">
         <v>60.57</v>
       </c>
-      <c r="H13" s="63"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="62"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="65"/>
       <c r="K13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1582,7 +1629,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" ht="90" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="105" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>42323</v>
       </c>
@@ -1614,7 +1661,7 @@
         <f>36.99+15</f>
         <v>51.99</v>
       </c>
-      <c r="J14" s="63"/>
+      <c r="J14" s="66"/>
       <c r="K14" s="2" t="s">
         <v>21</v>
       </c>
@@ -1665,14 +1712,14 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="68" t="s">
+      <c r="M15" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="N15" s="69"/>
-      <c r="O15" s="69"/>
-      <c r="P15" s="69"/>
-      <c r="Q15" s="69"/>
-      <c r="R15" s="70"/>
+      <c r="N15" s="72"/>
+      <c r="O15" s="72"/>
+      <c r="P15" s="72"/>
+      <c r="Q15" s="72"/>
+      <c r="R15" s="73"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
@@ -1693,10 +1740,10 @@
       <c r="N16" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="O16" s="71" t="s">
+      <c r="O16" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="P16" s="71"/>
+      <c r="P16" s="74"/>
       <c r="Q16" s="33" t="s">
         <v>25</v>
       </c>
@@ -1723,10 +1770,10 @@
       <c r="N17" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O17" s="66">
+      <c r="O17" s="69">
         <v>42053</v>
       </c>
-      <c r="P17" s="66"/>
+      <c r="P17" s="69"/>
       <c r="Q17" s="10">
         <v>108</v>
       </c>
@@ -1752,10 +1799,10 @@
       <c r="N18" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="O18" s="66">
+      <c r="O18" s="69">
         <v>42086</v>
       </c>
-      <c r="P18" s="66"/>
+      <c r="P18" s="69"/>
       <c r="Q18" s="10">
         <v>200</v>
       </c>
@@ -1781,10 +1828,10 @@
       <c r="N19" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O19" s="66">
+      <c r="O19" s="69">
         <v>42111</v>
       </c>
-      <c r="P19" s="66"/>
+      <c r="P19" s="69"/>
       <c r="Q19" s="10">
         <v>100</v>
       </c>
@@ -1809,10 +1856,10 @@
       <c r="N20" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O20" s="66">
+      <c r="O20" s="69">
         <v>42214</v>
       </c>
-      <c r="P20" s="66"/>
+      <c r="P20" s="69"/>
       <c r="Q20" s="10">
         <v>160</v>
       </c>
@@ -1831,10 +1878,10 @@
       <c r="N21" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="O21" s="66">
+      <c r="O21" s="69">
         <v>42325</v>
       </c>
-      <c r="P21" s="66"/>
+      <c r="P21" s="69"/>
       <c r="Q21" s="10">
         <v>113.35</v>
       </c>
@@ -1853,10 +1900,10 @@
       <c r="N22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="O22" s="66">
+      <c r="O22" s="69">
         <v>42325</v>
       </c>
-      <c r="P22" s="66"/>
+      <c r="P22" s="69"/>
       <c r="Q22" s="10">
         <v>80</v>
       </c>
@@ -1874,10 +1921,10 @@
       <c r="N23" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="O23" s="66">
+      <c r="O23" s="69">
         <v>42341</v>
       </c>
-      <c r="P23" s="66"/>
+      <c r="P23" s="69"/>
       <c r="Q23" s="10">
         <v>490.45</v>
       </c>
@@ -1893,10 +1940,10 @@
       <c r="N24" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="O24" s="66">
+      <c r="O24" s="69">
         <v>42364</v>
       </c>
-      <c r="P24" s="66"/>
+      <c r="P24" s="69"/>
       <c r="Q24" s="10">
         <v>113.98</v>
       </c>
@@ -1908,8 +1955,8 @@
       <c r="G25" s="1"/>
       <c r="M25" s="3"/>
       <c r="N25" s="11"/>
-      <c r="O25" s="66"/>
-      <c r="P25" s="66"/>
+      <c r="O25" s="69"/>
+      <c r="P25" s="69"/>
       <c r="Q25" s="10"/>
       <c r="R25" s="3"/>
     </row>
@@ -1959,8 +2006,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView zoomScale="115" workbookViewId="0">
@@ -1988,18 +2035,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="75" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
+      <c r="A1" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -2145,15 +2192,15 @@
         <f>SUM(C3:C14)</f>
         <v>375.303</v>
       </c>
-      <c r="N4" s="79">
+      <c r="N4" s="82">
         <f>207.67+O28+O31+O32</f>
         <v>807.67</v>
       </c>
-      <c r="O4" s="77">
+      <c r="O4" s="80">
         <f>SUM(M4:M5)-N4+P4</f>
         <v>144.58299999999997</v>
       </c>
-      <c r="P4" s="83">
+      <c r="P4" s="86">
         <v>0</v>
       </c>
       <c r="Q4" s="1"/>
@@ -2199,9 +2246,9 @@
         <f>SUM(D3:D14)</f>
         <v>576.94999999999993</v>
       </c>
-      <c r="N5" s="80"/>
-      <c r="O5" s="78"/>
-      <c r="P5" s="84"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="87"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.2">
@@ -2354,15 +2401,15 @@
         <f>SUM(G3:G14)</f>
         <v>620.59999999999991</v>
       </c>
-      <c r="N8" s="79">
+      <c r="N8" s="82">
         <f>SUM(O17,O20:O21,O23:O24,O25,O27,O30,O34,O36,O37)</f>
         <v>980.89999999999975</v>
       </c>
-      <c r="O8" s="81">
+      <c r="O8" s="84">
         <f>M8+M9-N8</f>
         <v>0</v>
       </c>
-      <c r="P8" s="85">
+      <c r="P8" s="88">
         <v>0</v>
       </c>
       <c r="Q8" s="1"/>
@@ -2408,9 +2455,9 @@
         <f>SUM(H3:H14)</f>
         <v>360.29999999999995</v>
       </c>
-      <c r="N9" s="80"/>
-      <c r="O9" s="82"/>
-      <c r="P9" s="86"/>
+      <c r="N9" s="83"/>
+      <c r="O9" s="85"/>
+      <c r="P9" s="89"/>
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" ht="120" x14ac:dyDescent="0.2">
@@ -2619,14 +2666,14 @@
       <c r="J14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K14" s="71" t="s">
+      <c r="K14" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="71"/>
-      <c r="M14" s="71"/>
-      <c r="N14" s="71"/>
-      <c r="O14" s="71"/>
-      <c r="P14" s="71"/>
+      <c r="L14" s="74"/>
+      <c r="M14" s="74"/>
+      <c r="N14" s="74"/>
+      <c r="O14" s="74"/>
+      <c r="P14" s="74"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
@@ -2645,10 +2692,10 @@
       <c r="L15" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="71" t="s">
+      <c r="M15" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="N15" s="71"/>
+      <c r="N15" s="74"/>
       <c r="O15" s="33" t="s">
         <v>25</v>
       </c>
@@ -2673,10 +2720,10 @@
       <c r="L16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M16" s="66">
+      <c r="M16" s="69">
         <v>42401</v>
       </c>
-      <c r="N16" s="66"/>
+      <c r="N16" s="69"/>
       <c r="O16" s="18">
         <v>100</v>
       </c>
@@ -2688,14 +2735,14 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="72" t="s">
+      <c r="D17" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="73"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="74"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="76"/>
+      <c r="I17" s="77"/>
       <c r="J17" s="1"/>
       <c r="K17" s="3">
         <v>2</v>
@@ -2703,10 +2750,10 @@
       <c r="L17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="66">
+      <c r="M17" s="69">
         <v>42402</v>
       </c>
-      <c r="N17" s="66"/>
+      <c r="N17" s="69"/>
       <c r="O17" s="18">
         <v>104.08</v>
       </c>
@@ -2743,10 +2790,10 @@
       <c r="L18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M18" s="66">
+      <c r="M18" s="69">
         <v>42402</v>
       </c>
-      <c r="N18" s="66"/>
+      <c r="N18" s="69"/>
       <c r="O18" s="18">
         <v>138.5</v>
       </c>
@@ -2783,10 +2830,10 @@
       <c r="L19" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M19" s="66">
+      <c r="M19" s="69">
         <v>42433</v>
       </c>
-      <c r="N19" s="66"/>
+      <c r="N19" s="69"/>
       <c r="O19" s="18">
         <v>20</v>
       </c>
@@ -2821,10 +2868,10 @@
       <c r="L20" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="66">
+      <c r="M20" s="69">
         <v>42433</v>
       </c>
-      <c r="N20" s="66"/>
+      <c r="N20" s="69"/>
       <c r="O20" s="18">
         <v>92.66</v>
       </c>
@@ -2859,10 +2906,10 @@
       <c r="L21" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M21" s="66">
+      <c r="M21" s="69">
         <v>42465</v>
       </c>
-      <c r="N21" s="66"/>
+      <c r="N21" s="69"/>
       <c r="O21" s="18">
         <v>92.66</v>
       </c>
@@ -2897,10 +2944,10 @@
       <c r="L22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M22" s="66">
+      <c r="M22" s="69">
         <v>42493</v>
       </c>
-      <c r="N22" s="66"/>
+      <c r="N22" s="69"/>
       <c r="O22" s="18">
         <v>100</v>
       </c>
@@ -2933,10 +2980,10 @@
       <c r="L23" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M23" s="66">
+      <c r="M23" s="69">
         <v>42494</v>
       </c>
-      <c r="N23" s="66"/>
+      <c r="N23" s="69"/>
       <c r="O23" s="18">
         <v>81.900000000000006</v>
       </c>
@@ -2969,10 +3016,10 @@
       <c r="L24" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M24" s="66">
+      <c r="M24" s="69">
         <v>42531</v>
       </c>
-      <c r="N24" s="66"/>
+      <c r="N24" s="69"/>
       <c r="O24" s="18">
         <v>93.52</v>
       </c>
@@ -3005,10 +3052,10 @@
       <c r="L25" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M25" s="66">
+      <c r="M25" s="69">
         <v>42558</v>
       </c>
-      <c r="N25" s="66"/>
+      <c r="N25" s="69"/>
       <c r="O25" s="18">
         <v>91.1</v>
       </c>
@@ -3031,10 +3078,10 @@
       <c r="L26" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M26" s="66">
+      <c r="M26" s="69">
         <v>42590</v>
       </c>
-      <c r="N26" s="66"/>
+      <c r="N26" s="69"/>
       <c r="O26" s="18">
         <v>100</v>
       </c>
@@ -3050,10 +3097,10 @@
       <c r="L27" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M27" s="66">
+      <c r="M27" s="69">
         <v>42598</v>
       </c>
-      <c r="N27" s="66"/>
+      <c r="N27" s="69"/>
       <c r="O27" s="18">
         <v>91.4</v>
       </c>
@@ -3069,10 +3116,10 @@
       <c r="L28" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="M28" s="66">
+      <c r="M28" s="69">
         <v>42599</v>
       </c>
-      <c r="N28" s="66"/>
+      <c r="N28" s="69"/>
       <c r="O28" s="18">
         <v>200</v>
       </c>
@@ -3087,10 +3134,10 @@
       <c r="L29" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M29" s="66">
+      <c r="M29" s="69">
         <v>42600</v>
       </c>
-      <c r="N29" s="66"/>
+      <c r="N29" s="69"/>
       <c r="O29" s="18">
         <v>200</v>
       </c>
@@ -3105,10 +3152,10 @@
       <c r="L30" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M30" s="66">
+      <c r="M30" s="69">
         <v>42615</v>
       </c>
-      <c r="N30" s="66"/>
+      <c r="N30" s="69"/>
       <c r="O30" s="18">
         <v>90.57</v>
       </c>
@@ -3123,10 +3170,10 @@
       <c r="L31" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="M31" s="66">
+      <c r="M31" s="69">
         <v>42648</v>
       </c>
-      <c r="N31" s="66"/>
+      <c r="N31" s="69"/>
       <c r="O31" s="18">
         <v>200</v>
       </c>
@@ -3141,10 +3188,10 @@
       <c r="L32" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="M32" s="66">
+      <c r="M32" s="69">
         <v>42656</v>
       </c>
-      <c r="N32" s="66"/>
+      <c r="N32" s="69"/>
       <c r="O32" s="18">
         <v>200</v>
       </c>
@@ -3159,10 +3206,10 @@
       <c r="L33" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M33" s="66">
+      <c r="M33" s="69">
         <v>42656</v>
       </c>
-      <c r="N33" s="66"/>
+      <c r="N33" s="69"/>
       <c r="O33" s="18">
         <v>22</v>
       </c>
@@ -3177,10 +3224,10 @@
       <c r="L34" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M34" s="66">
+      <c r="M34" s="69">
         <v>42657</v>
       </c>
-      <c r="N34" s="66"/>
+      <c r="N34" s="69"/>
       <c r="O34" s="18">
         <v>90.57</v>
       </c>
@@ -3195,10 +3242,10 @@
       <c r="L35" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M35" s="66">
+      <c r="M35" s="69">
         <v>42651</v>
       </c>
-      <c r="N35" s="66"/>
+      <c r="N35" s="69"/>
       <c r="O35" s="18">
         <v>10</v>
       </c>
@@ -3213,10 +3260,10 @@
       <c r="L36" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M36" s="66">
+      <c r="M36" s="69">
         <v>42687</v>
       </c>
-      <c r="N36" s="66"/>
+      <c r="N36" s="69"/>
       <c r="O36" s="18">
         <v>90.42</v>
       </c>
@@ -3231,10 +3278,10 @@
       <c r="L37" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M37" s="66">
+      <c r="M37" s="69">
         <v>42717</v>
       </c>
-      <c r="N37" s="66"/>
+      <c r="N37" s="69"/>
       <c r="O37" s="18">
         <v>62.02</v>
       </c>
@@ -3249,10 +3296,10 @@
       <c r="L38" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M38" s="66">
+      <c r="M38" s="69">
         <v>42726</v>
       </c>
-      <c r="N38" s="66"/>
+      <c r="N38" s="69"/>
       <c r="O38" s="18">
         <v>100</v>
       </c>
@@ -3302,11 +3349,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView zoomScale="117" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3330,18 +3377,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="88" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
+      <c r="A1" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
       <c r="K1" s="34"/>
       <c r="L1" s="34"/>
       <c r="M1" s="34"/>
@@ -3474,15 +3521,15 @@
       </c>
       <c r="M4" s="39">
         <f>SUM(E3:E14)</f>
-        <v>234.22999999999996</v>
+        <v>375.90999999999991</v>
       </c>
       <c r="N4" s="39">
-        <f>SUM(O19)</f>
-        <v>150</v>
-      </c>
-      <c r="O4" s="44">
+        <f>SUM(O19,O26)</f>
+        <v>250</v>
+      </c>
+      <c r="O4" s="46">
         <f>M4-N4+P4</f>
-        <v>23.789999999999964</v>
+        <v>65.469999999999914</v>
       </c>
       <c r="P4" s="45">
         <v>-60.44</v>
@@ -3524,10 +3571,10 @@
       </c>
       <c r="M5" s="39">
         <f>SUM(F3:F14)</f>
-        <v>278.55</v>
+        <v>459.55999999999995</v>
       </c>
       <c r="N5" s="39">
-        <v>278.55</v>
+        <v>459.56</v>
       </c>
       <c r="O5" s="44">
         <f>M5-N5</f>
@@ -3573,15 +3620,15 @@
       </c>
       <c r="M6" s="39">
         <f>SUM(G3:G14)</f>
-        <v>234.22999999999996</v>
-      </c>
-      <c r="N6" s="100">
-        <f>SUM(O16,O18,O20:O21)</f>
-        <v>327.17999999999995</v>
-      </c>
-      <c r="O6" s="102">
+        <v>415.17999999999989</v>
+      </c>
+      <c r="N6" s="103">
+        <f>SUM(O16,O18,O20:O25)</f>
+        <v>918.45999999999992</v>
+      </c>
+      <c r="O6" s="105">
         <f>M6+M7-N6</f>
-        <v>141.27999999999997</v>
+        <v>-88.100000000000136</v>
       </c>
       <c r="P6" s="59">
         <v>0</v>
@@ -3623,10 +3670,10 @@
       </c>
       <c r="M7" s="39">
         <f>SUM(H3:H14)</f>
-        <v>234.22999999999996</v>
-      </c>
-      <c r="N7" s="101"/>
-      <c r="O7" s="103"/>
+        <v>415.17999999999989</v>
+      </c>
+      <c r="N7" s="104"/>
+      <c r="O7" s="106"/>
       <c r="P7" s="60"/>
       <c r="Q7" s="34"/>
     </row>
@@ -3665,14 +3712,14 @@
       </c>
       <c r="M8" s="39">
         <f>SUM(I3:I14)</f>
-        <v>230.92000000000002</v>
+        <v>410.65000000000003</v>
       </c>
       <c r="N8" s="39">
         <v>0</v>
       </c>
       <c r="O8" s="46">
         <f>M8-N8+P8</f>
-        <v>352.51</v>
+        <v>532.24</v>
       </c>
       <c r="P8" s="47">
         <v>121.59</v>
@@ -3716,15 +3763,15 @@
         <f>SUM(C3:C14)</f>
         <v>76.11</v>
       </c>
-      <c r="N9" s="90">
+      <c r="N9" s="93">
         <f>SUM(O17)</f>
         <v>200</v>
       </c>
-      <c r="O9" s="92">
+      <c r="O9" s="95">
         <f>SUM(M9:M10)-N9+P9</f>
         <v>131.07000000000002</v>
       </c>
-      <c r="P9" s="94">
+      <c r="P9" s="97">
         <v>144.58000000000001</v>
       </c>
       <c r="Q9" s="34"/>
@@ -3733,18 +3780,30 @@
       <c r="A10" s="37">
         <v>42962</v>
       </c>
-      <c r="B10" s="38"/>
+      <c r="B10" s="38">
+        <v>176.23</v>
+      </c>
       <c r="C10" s="38">
         <v>0</v>
       </c>
       <c r="D10" s="39">
         <v>0</v>
       </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
+      <c r="E10" s="38">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="F10" s="38">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="G10" s="39">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="H10" s="39">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="I10" s="39">
+        <v>35.03</v>
+      </c>
       <c r="J10" s="40"/>
       <c r="K10" s="34"/>
       <c r="L10" s="40" t="s">
@@ -3754,27 +3813,39 @@
         <f>SUM(D3:D14)</f>
         <v>110.38</v>
       </c>
-      <c r="N10" s="91"/>
-      <c r="O10" s="93"/>
-      <c r="P10" s="95"/>
+      <c r="N10" s="94"/>
+      <c r="O10" s="96"/>
+      <c r="P10" s="98"/>
       <c r="Q10" s="34"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="37">
         <v>42993</v>
       </c>
-      <c r="B11" s="38"/>
+      <c r="B11" s="38">
+        <v>177.1</v>
+      </c>
       <c r="C11" s="38">
         <v>0</v>
       </c>
       <c r="D11" s="39">
         <v>0</v>
       </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
+      <c r="E11" s="38">
+        <v>35.46</v>
+      </c>
+      <c r="F11" s="38">
+        <v>35.57</v>
+      </c>
+      <c r="G11" s="38">
+        <v>35.46</v>
+      </c>
+      <c r="H11" s="39">
+        <v>35.46</v>
+      </c>
+      <c r="I11" s="39">
+        <v>35.15</v>
+      </c>
       <c r="J11" s="40"/>
       <c r="K11" s="34"/>
       <c r="Q11" s="34"/>
@@ -3783,18 +3854,30 @@
       <c r="A12" s="37">
         <v>43023</v>
       </c>
-      <c r="B12" s="38"/>
+      <c r="B12" s="38">
+        <v>177.09</v>
+      </c>
       <c r="C12" s="38">
         <v>0</v>
       </c>
       <c r="D12" s="39">
         <v>0</v>
       </c>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="E12" s="38">
+        <v>35.46</v>
+      </c>
+      <c r="F12" s="38">
+        <v>35.46</v>
+      </c>
+      <c r="G12" s="38">
+        <v>35.46</v>
+      </c>
+      <c r="H12" s="39">
+        <v>35.46</v>
+      </c>
+      <c r="I12" s="39">
+        <v>35.25</v>
+      </c>
       <c r="J12" s="40"/>
       <c r="K12" s="34"/>
       <c r="Q12" s="34"/>
@@ -3803,18 +3886,30 @@
       <c r="A13" s="37">
         <v>43054</v>
       </c>
-      <c r="B13" s="39"/>
+      <c r="B13" s="39">
+        <v>177.09</v>
+      </c>
       <c r="C13" s="38">
         <v>0</v>
       </c>
       <c r="D13" s="39">
         <v>0</v>
       </c>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
+      <c r="E13" s="38">
+        <v>35.46</v>
+      </c>
+      <c r="F13" s="38">
+        <v>35.46</v>
+      </c>
+      <c r="G13" s="38">
+        <v>35.46</v>
+      </c>
+      <c r="H13" s="39">
+        <v>35.46</v>
+      </c>
+      <c r="I13" s="39">
+        <v>35.25</v>
+      </c>
       <c r="J13" s="40"/>
       <c r="K13" s="34"/>
       <c r="L13" s="34"/>
@@ -3828,7 +3923,9 @@
       <c r="A14" s="37">
         <v>43084</v>
       </c>
-      <c r="B14" s="39"/>
+      <c r="B14" s="39">
+        <v>156.82</v>
+      </c>
       <c r="C14" s="38">
         <v>0</v>
       </c>
@@ -3836,19 +3933,29 @@
         <v>0</v>
       </c>
       <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="96" t="s">
+      <c r="F14" s="39">
+        <v>39.22</v>
+      </c>
+      <c r="G14" s="39">
+        <v>39.270000000000003</v>
+      </c>
+      <c r="H14" s="39">
+        <v>39.270000000000003</v>
+      </c>
+      <c r="I14" s="39">
+        <v>39.049999999999997</v>
+      </c>
+      <c r="J14" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="K14" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="96"/>
-      <c r="M14" s="96"/>
-      <c r="N14" s="96"/>
-      <c r="O14" s="96"/>
-      <c r="P14" s="96"/>
+      <c r="L14" s="99"/>
+      <c r="M14" s="99"/>
+      <c r="N14" s="99"/>
+      <c r="O14" s="99"/>
+      <c r="P14" s="99"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="34"/>
@@ -3867,10 +3974,10 @@
       <c r="L15" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="96" t="s">
+      <c r="M15" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="N15" s="96"/>
+      <c r="N15" s="99"/>
       <c r="O15" s="49" t="s">
         <v>25</v>
       </c>
@@ -3895,10 +4002,10 @@
       <c r="L16" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="M16" s="87">
+      <c r="M16" s="90">
         <v>42750</v>
       </c>
-      <c r="N16" s="87"/>
+      <c r="N16" s="90"/>
       <c r="O16" s="52">
         <v>62.02</v>
       </c>
@@ -3910,14 +4017,14 @@
       <c r="A17" s="34"/>
       <c r="B17" s="34"/>
       <c r="C17" s="48"/>
-      <c r="D17" s="97" t="s">
+      <c r="D17" s="100" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="98"/>
-      <c r="F17" s="98"/>
-      <c r="G17" s="98"/>
-      <c r="H17" s="98"/>
-      <c r="I17" s="99"/>
+      <c r="E17" s="101"/>
+      <c r="F17" s="101"/>
+      <c r="G17" s="101"/>
+      <c r="H17" s="101"/>
+      <c r="I17" s="102"/>
       <c r="J17" s="34"/>
       <c r="K17" s="50">
         <v>2</v>
@@ -3925,10 +4032,10 @@
       <c r="L17" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="M17" s="87">
+      <c r="M17" s="90">
         <v>42751</v>
       </c>
-      <c r="N17" s="87"/>
+      <c r="N17" s="90"/>
       <c r="O17" s="52">
         <v>200</v>
       </c>
@@ -3965,10 +4072,10 @@
       <c r="L18" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="M18" s="87">
+      <c r="M18" s="90">
         <v>42768</v>
       </c>
-      <c r="N18" s="87"/>
+      <c r="N18" s="90"/>
       <c r="O18" s="52">
         <v>61.98</v>
       </c>
@@ -3984,19 +4091,15 @@
         <v>4</v>
       </c>
       <c r="E19" s="39">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F19" s="55">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G19" s="55">
-        <f>5.32*2</f>
-        <v>10.64</v>
-      </c>
-      <c r="H19" s="55">
-        <f t="shared" ref="H19:H23" si="0">SUM(E19:G19)</f>
-        <v>70.64</v>
-      </c>
+        <v>5.46</v>
+      </c>
+      <c r="H19" s="55"/>
       <c r="I19" s="55"/>
       <c r="J19" s="34"/>
       <c r="K19" s="50">
@@ -4005,10 +4108,10 @@
       <c r="L19" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="M19" s="87">
+      <c r="M19" s="90">
         <v>42793</v>
       </c>
-      <c r="N19" s="87"/>
+      <c r="N19" s="90"/>
       <c r="O19" s="52">
         <v>150</v>
       </c>
@@ -4023,18 +4126,17 @@
         <v>6</v>
       </c>
       <c r="E20" s="39">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F20" s="55">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G20" s="55">
-        <f>5.32*2</f>
-        <v>10.64</v>
+        <v>5.46</v>
       </c>
       <c r="H20" s="55">
-        <f t="shared" si="0"/>
-        <v>70.64</v>
+        <f t="shared" ref="H19:H23" si="0">SUM(E20:G20)</f>
+        <v>35.46</v>
       </c>
       <c r="I20" s="55"/>
       <c r="K20" s="50">
@@ -4043,10 +4145,10 @@
       <c r="L20" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="87">
+      <c r="M20" s="90">
         <v>42797</v>
       </c>
-      <c r="N20" s="87"/>
+      <c r="N20" s="90"/>
       <c r="O20" s="52">
         <v>61.98</v>
       </c>
@@ -4061,18 +4163,17 @@
         <v>47</v>
       </c>
       <c r="E21" s="39">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F21" s="55">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G21" s="55">
-        <f>5.05*2</f>
-        <v>10.1</v>
+        <v>5.29</v>
       </c>
       <c r="H21" s="55">
         <f t="shared" si="0"/>
-        <v>70.099999999999994</v>
+        <v>35.29</v>
       </c>
       <c r="I21" s="55"/>
       <c r="K21" s="50">
@@ -4081,14 +4182,16 @@
       <c r="L21" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="M21" s="87">
+      <c r="M21" s="90">
         <v>42858</v>
       </c>
-      <c r="N21" s="87"/>
+      <c r="N21" s="90"/>
       <c r="O21" s="52">
         <v>141.19999999999999</v>
       </c>
-      <c r="P21" s="50"/>
+      <c r="P21" s="50" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B22" s="34"/>
@@ -4097,56 +4200,70 @@
         <v>7</v>
       </c>
       <c r="E22" s="39">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F22" s="55">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G22" s="55">
-        <f>5.32*2</f>
-        <v>10.64</v>
+        <v>5.51</v>
       </c>
       <c r="H22" s="55">
         <f t="shared" si="0"/>
-        <v>70.64</v>
+        <v>35.51</v>
       </c>
       <c r="I22" s="55"/>
       <c r="K22" s="50">
         <v>7</v>
       </c>
-      <c r="L22" s="51"/>
-      <c r="M22" s="87"/>
-      <c r="N22" s="87"/>
-      <c r="O22" s="52"/>
-      <c r="P22" s="50"/>
+      <c r="L22" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" s="90">
+        <v>42931</v>
+      </c>
+      <c r="N22" s="90"/>
+      <c r="O22" s="52">
+        <v>141.28</v>
+      </c>
+      <c r="P22" s="50" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D23" s="40" t="s">
         <v>48</v>
       </c>
       <c r="E23" s="39">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F23" s="55">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G23" s="55">
-        <f>5.32*2</f>
-        <v>10.64</v>
+        <v>5.51</v>
       </c>
       <c r="H23" s="55">
         <f t="shared" si="0"/>
-        <v>70.64</v>
+        <v>35.51</v>
       </c>
       <c r="I23" s="55"/>
       <c r="K23" s="50">
         <v>8</v>
       </c>
-      <c r="L23" s="51"/>
-      <c r="M23" s="87"/>
-      <c r="N23" s="87"/>
-      <c r="O23" s="52"/>
-      <c r="P23" s="50"/>
+      <c r="L23" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="M23" s="90">
+        <v>43001</v>
+      </c>
+      <c r="N23" s="90"/>
+      <c r="O23" s="52">
+        <v>150</v>
+      </c>
+      <c r="P23" s="50" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F24" s="34"/>
@@ -4155,46 +4272,68 @@
       </c>
       <c r="H24" s="58">
         <f>SUM(H19:I23)</f>
-        <v>352.65999999999997</v>
+        <v>141.76999999999998</v>
       </c>
       <c r="K24" s="50">
         <v>9</v>
       </c>
-      <c r="L24" s="51"/>
-      <c r="M24" s="87"/>
-      <c r="N24" s="87"/>
-      <c r="O24" s="52"/>
-      <c r="P24" s="50"/>
+      <c r="L24" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="M24" s="90">
+        <v>43053</v>
+      </c>
+      <c r="N24" s="90"/>
+      <c r="O24" s="52">
+        <v>150</v>
+      </c>
+      <c r="P24" s="50" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F25" s="34"/>
       <c r="K25" s="50">
         <v>10</v>
       </c>
-      <c r="L25" s="51"/>
-      <c r="M25" s="87"/>
-      <c r="N25" s="87"/>
-      <c r="O25" s="52"/>
-      <c r="P25" s="50"/>
+      <c r="L25" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="M25" s="90">
+        <v>43128</v>
+      </c>
+      <c r="N25" s="90"/>
+      <c r="O25" s="52">
+        <v>150</v>
+      </c>
+      <c r="P25" s="50" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F26" s="34"/>
       <c r="K26" s="50">
         <v>10</v>
       </c>
-      <c r="L26" s="51"/>
-      <c r="M26" s="87"/>
-      <c r="N26" s="87"/>
-      <c r="O26" s="52"/>
-      <c r="P26" s="50"/>
+      <c r="L26" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="M26" s="90"/>
+      <c r="N26" s="90"/>
+      <c r="O26" s="52">
+        <v>100</v>
+      </c>
+      <c r="P26" s="50" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="K27" s="50">
         <v>11</v>
       </c>
       <c r="L27" s="51"/>
-      <c r="M27" s="87"/>
-      <c r="N27" s="87"/>
+      <c r="M27" s="90"/>
+      <c r="N27" s="90"/>
       <c r="O27" s="52"/>
       <c r="P27" s="50"/>
     </row>
@@ -4203,8 +4342,8 @@
         <v>11</v>
       </c>
       <c r="L28" s="51"/>
-      <c r="M28" s="87"/>
-      <c r="N28" s="87"/>
+      <c r="M28" s="90"/>
+      <c r="N28" s="90"/>
       <c r="O28" s="52"/>
       <c r="P28" s="50"/>
     </row>
@@ -4213,8 +4352,8 @@
         <v>12</v>
       </c>
       <c r="L29" s="51"/>
-      <c r="M29" s="87"/>
-      <c r="N29" s="87"/>
+      <c r="M29" s="90"/>
+      <c r="N29" s="90"/>
       <c r="O29" s="52"/>
       <c r="P29" s="50"/>
     </row>
@@ -4223,8 +4362,8 @@
         <v>13</v>
       </c>
       <c r="L30" s="51"/>
-      <c r="M30" s="87"/>
-      <c r="N30" s="87"/>
+      <c r="M30" s="90"/>
+      <c r="N30" s="90"/>
       <c r="O30" s="52"/>
       <c r="P30" s="50"/>
     </row>
@@ -4233,8 +4372,8 @@
         <v>14</v>
       </c>
       <c r="L31" s="51"/>
-      <c r="M31" s="87"/>
-      <c r="N31" s="87"/>
+      <c r="M31" s="90"/>
+      <c r="N31" s="90"/>
       <c r="O31" s="52"/>
       <c r="P31" s="50"/>
     </row>
@@ -4243,8 +4382,8 @@
         <v>15</v>
       </c>
       <c r="L32" s="51"/>
-      <c r="M32" s="87"/>
-      <c r="N32" s="87"/>
+      <c r="M32" s="90"/>
+      <c r="N32" s="90"/>
       <c r="O32" s="52"/>
       <c r="P32" s="50"/>
     </row>
@@ -4253,8 +4392,8 @@
         <v>16</v>
       </c>
       <c r="L33" s="51"/>
-      <c r="M33" s="87"/>
-      <c r="N33" s="87"/>
+      <c r="M33" s="90"/>
+      <c r="N33" s="90"/>
       <c r="O33" s="52"/>
       <c r="P33" s="50"/>
     </row>
@@ -4263,8 +4402,8 @@
         <v>17</v>
       </c>
       <c r="L34" s="51"/>
-      <c r="M34" s="87"/>
-      <c r="N34" s="87"/>
+      <c r="M34" s="90"/>
+      <c r="N34" s="90"/>
       <c r="O34" s="52"/>
       <c r="P34" s="50"/>
     </row>
@@ -4273,8 +4412,8 @@
         <v>18</v>
       </c>
       <c r="L35" s="51"/>
-      <c r="M35" s="87"/>
-      <c r="N35" s="87"/>
+      <c r="M35" s="90"/>
+      <c r="N35" s="90"/>
       <c r="O35" s="52"/>
       <c r="P35" s="50"/>
     </row>
@@ -4283,8 +4422,8 @@
         <v>19</v>
       </c>
       <c r="L36" s="51"/>
-      <c r="M36" s="87"/>
-      <c r="N36" s="87"/>
+      <c r="M36" s="90"/>
+      <c r="N36" s="90"/>
       <c r="O36" s="52"/>
       <c r="P36" s="50"/>
     </row>
@@ -4293,8 +4432,8 @@
         <v>20</v>
       </c>
       <c r="L37" s="51"/>
-      <c r="M37" s="87"/>
-      <c r="N37" s="87"/>
+      <c r="M37" s="90"/>
+      <c r="N37" s="90"/>
       <c r="O37" s="52"/>
       <c r="P37" s="50"/>
     </row>
@@ -4303,8 +4442,8 @@
         <v>21</v>
       </c>
       <c r="L38" s="51"/>
-      <c r="M38" s="87"/>
-      <c r="N38" s="87"/>
+      <c r="M38" s="90"/>
+      <c r="N38" s="90"/>
       <c r="O38" s="52"/>
       <c r="P38" s="50"/>
     </row>
@@ -4345,4 +4484,894 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A8CBCC-2E8E-DE41-B680-C419BF748250}">
+  <dimension ref="A1:R38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="12" style="35" customWidth="1"/>
+    <col min="3" max="4" width="11.5" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="35" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="35" customWidth="1"/>
+    <col min="7" max="9" width="13.1640625" style="35" customWidth="1"/>
+    <col min="10" max="10" width="27.83203125" style="35" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" style="35" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" style="35" customWidth="1"/>
+    <col min="13" max="13" width="15" style="35" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" style="35" customWidth="1"/>
+    <col min="15" max="15" width="13.1640625" style="35" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" style="35" customWidth="1"/>
+    <col min="17" max="17" width="19.5" style="35" customWidth="1"/>
+    <col min="18" max="16384" width="8.83203125" style="35"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="113" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="37">
+        <v>43115</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="39">
+        <v>0</v>
+      </c>
+      <c r="D3" s="39">
+        <v>0</v>
+      </c>
+      <c r="E3" s="39">
+        <v>0</v>
+      </c>
+      <c r="F3" s="39">
+        <v>0</v>
+      </c>
+      <c r="G3" s="39">
+        <v>0</v>
+      </c>
+      <c r="H3" s="39">
+        <v>0</v>
+      </c>
+      <c r="I3" s="39">
+        <v>0</v>
+      </c>
+      <c r="J3" s="40"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="R3" s="34"/>
+    </row>
+    <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="37">
+        <v>43146</v>
+      </c>
+      <c r="B4" s="38">
+        <v>195.13</v>
+      </c>
+      <c r="C4" s="38">
+        <v>53.31</v>
+      </c>
+      <c r="D4" s="38">
+        <v>35.51</v>
+      </c>
+      <c r="E4" s="39">
+        <v>35.51</v>
+      </c>
+      <c r="F4" s="39">
+        <v>35.51</v>
+      </c>
+      <c r="G4" s="39">
+        <v>35.29</v>
+      </c>
+      <c r="H4" s="39">
+        <v>0</v>
+      </c>
+      <c r="I4" s="39">
+        <v>0</v>
+      </c>
+      <c r="J4" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="34"/>
+      <c r="M4" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="39">
+        <f>SUM(C3:C14)</f>
+        <v>124.82999999999998</v>
+      </c>
+      <c r="O4" s="39">
+        <f>SUM(P16)</f>
+        <v>80</v>
+      </c>
+      <c r="P4" s="46">
+        <f>N4-O4+Q4</f>
+        <v>110.29999999999998</v>
+      </c>
+      <c r="Q4" s="109">
+        <v>65.47</v>
+      </c>
+      <c r="R4" s="34"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="37">
+        <v>43174</v>
+      </c>
+      <c r="B5" s="38">
+        <v>177.33</v>
+      </c>
+      <c r="C5" s="38">
+        <v>35.51</v>
+      </c>
+      <c r="D5" s="38">
+        <v>35.51</v>
+      </c>
+      <c r="E5" s="39">
+        <v>35.51</v>
+      </c>
+      <c r="F5" s="39">
+        <v>35.51</v>
+      </c>
+      <c r="G5" s="39">
+        <v>35.29</v>
+      </c>
+      <c r="H5" s="39">
+        <v>0</v>
+      </c>
+      <c r="I5" s="39">
+        <v>0</v>
+      </c>
+      <c r="J5" s="40"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" s="39">
+        <f>SUM(D3:D14)</f>
+        <v>107.03</v>
+      </c>
+      <c r="O5" s="39">
+        <v>107.03</v>
+      </c>
+      <c r="P5" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="45">
+        <v>0</v>
+      </c>
+      <c r="R5" s="34"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="37">
+        <v>43205</v>
+      </c>
+      <c r="B6" s="38">
+        <v>179.85</v>
+      </c>
+      <c r="C6" s="38">
+        <v>36.01</v>
+      </c>
+      <c r="D6" s="38">
+        <v>36.01</v>
+      </c>
+      <c r="E6" s="39">
+        <v>36.01</v>
+      </c>
+      <c r="F6" s="39">
+        <v>36.01</v>
+      </c>
+      <c r="G6" s="39">
+        <v>35.81</v>
+      </c>
+      <c r="H6" s="39">
+        <v>0</v>
+      </c>
+      <c r="I6" s="39">
+        <v>0</v>
+      </c>
+      <c r="J6" s="40"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="N6" s="39">
+        <f>SUM(E3:E14)</f>
+        <v>107.03</v>
+      </c>
+      <c r="O6" s="103">
+        <f>SUM(P17)</f>
+        <v>150</v>
+      </c>
+      <c r="P6" s="114">
+        <f>N6+N7-O6+Q6</f>
+        <v>-24.120000000000005</v>
+      </c>
+      <c r="Q6" s="61">
+        <v>-88.18</v>
+      </c>
+      <c r="R6" s="34"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="37">
+        <v>43235</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="40"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="39">
+        <f>SUM(F3:F14)</f>
+        <v>107.03</v>
+      </c>
+      <c r="O7" s="104"/>
+      <c r="P7" s="115"/>
+      <c r="Q7" s="62"/>
+      <c r="R7" s="34"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="37">
+        <v>43266</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="40"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="N8" s="39">
+        <f>SUM(G3:G14)</f>
+        <v>106.39</v>
+      </c>
+      <c r="O8" s="39">
+        <v>0</v>
+      </c>
+      <c r="P8" s="46">
+        <f>N8-O8+Q8</f>
+        <v>638.63</v>
+      </c>
+      <c r="Q8" s="47">
+        <v>532.24</v>
+      </c>
+      <c r="R8" s="34"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" s="37">
+        <v>43296</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="40"/>
+      <c r="L9" s="34"/>
+      <c r="R9" s="34"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" s="37">
+        <v>43327</v>
+      </c>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="40"/>
+      <c r="L10" s="34"/>
+      <c r="R10" s="34"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" s="37">
+        <v>43358</v>
+      </c>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="40"/>
+      <c r="L11" s="34"/>
+      <c r="R11" s="34"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="37">
+        <v>43388</v>
+      </c>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="40"/>
+      <c r="L12" s="34"/>
+      <c r="R12" s="34"/>
+    </row>
+    <row r="13" spans="1:18" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="37">
+        <v>43419</v>
+      </c>
+      <c r="B13" s="39"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="40"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="48"/>
+    </row>
+    <row r="14" spans="1:18" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="37">
+        <v>43449</v>
+      </c>
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="40"/>
+      <c r="L14" s="110" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="111"/>
+      <c r="N14" s="111"/>
+      <c r="O14" s="111"/>
+      <c r="P14" s="111"/>
+      <c r="Q14" s="112"/>
+    </row>
+    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="L15" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="N15" s="99" t="s">
+        <v>24</v>
+      </c>
+      <c r="O15" s="99"/>
+      <c r="P15" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q15" s="63" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="107" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="108"/>
+      <c r="E16" s="108"/>
+      <c r="F16" s="108"/>
+      <c r="G16" s="108"/>
+      <c r="H16" s="108"/>
+      <c r="L16" s="50">
+        <v>1</v>
+      </c>
+      <c r="M16" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="N16" s="90">
+        <v>43210</v>
+      </c>
+      <c r="O16" s="90"/>
+      <c r="P16" s="52">
+        <v>80</v>
+      </c>
+      <c r="Q16" s="50" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="L17" s="50">
+        <v>2</v>
+      </c>
+      <c r="M17" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="N17" s="90">
+        <v>43188</v>
+      </c>
+      <c r="O17" s="90"/>
+      <c r="P17" s="52">
+        <v>150</v>
+      </c>
+      <c r="Q17" s="50" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="39">
+        <v>15</v>
+      </c>
+      <c r="E18" s="55">
+        <v>15</v>
+      </c>
+      <c r="F18" s="55">
+        <v>6.01</v>
+      </c>
+      <c r="G18" s="55">
+        <f t="shared" ref="G18:G22" si="0">SUM(D18:F18)</f>
+        <v>36.01</v>
+      </c>
+      <c r="H18" s="55"/>
+      <c r="L18" s="50">
+        <v>3</v>
+      </c>
+      <c r="M18" s="51"/>
+      <c r="N18" s="90"/>
+      <c r="O18" s="90"/>
+      <c r="P18" s="52"/>
+      <c r="Q18" s="50"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="39">
+        <v>15</v>
+      </c>
+      <c r="E19" s="55">
+        <v>15</v>
+      </c>
+      <c r="F19" s="55">
+        <v>6.01</v>
+      </c>
+      <c r="G19" s="55">
+        <f t="shared" si="0"/>
+        <v>36.01</v>
+      </c>
+      <c r="H19" s="55"/>
+      <c r="L19" s="50">
+        <v>4</v>
+      </c>
+      <c r="M19" s="51"/>
+      <c r="N19" s="90"/>
+      <c r="O19" s="90"/>
+      <c r="P19" s="52"/>
+      <c r="Q19" s="50"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B20" s="34"/>
+      <c r="C20" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="39">
+        <v>15</v>
+      </c>
+      <c r="E20" s="55">
+        <v>15</v>
+      </c>
+      <c r="F20" s="55">
+        <v>5.81</v>
+      </c>
+      <c r="G20" s="55">
+        <f t="shared" si="0"/>
+        <v>35.81</v>
+      </c>
+      <c r="H20" s="55"/>
+      <c r="L20" s="50">
+        <v>5</v>
+      </c>
+      <c r="M20" s="51"/>
+      <c r="N20" s="90"/>
+      <c r="O20" s="90"/>
+      <c r="P20" s="52"/>
+      <c r="Q20" s="50"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B21" s="34"/>
+      <c r="C21" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="39">
+        <v>15</v>
+      </c>
+      <c r="E21" s="55">
+        <v>15</v>
+      </c>
+      <c r="F21" s="55">
+        <v>6.01</v>
+      </c>
+      <c r="G21" s="55">
+        <f t="shared" si="0"/>
+        <v>36.01</v>
+      </c>
+      <c r="H21" s="55"/>
+      <c r="L21" s="50">
+        <v>6</v>
+      </c>
+      <c r="M21" s="51"/>
+      <c r="N21" s="90"/>
+      <c r="O21" s="90"/>
+      <c r="P21" s="52"/>
+      <c r="Q21" s="50"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B22" s="34"/>
+      <c r="C22" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="39">
+        <v>15</v>
+      </c>
+      <c r="E22" s="55">
+        <v>15</v>
+      </c>
+      <c r="F22" s="55">
+        <v>6.01</v>
+      </c>
+      <c r="G22" s="55">
+        <f t="shared" si="0"/>
+        <v>36.01</v>
+      </c>
+      <c r="H22" s="55"/>
+      <c r="L22" s="50">
+        <v>7</v>
+      </c>
+      <c r="M22" s="51"/>
+      <c r="N22" s="90"/>
+      <c r="O22" s="90"/>
+      <c r="P22" s="52"/>
+      <c r="Q22" s="50"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="E23" s="34"/>
+      <c r="F23" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="58">
+        <f>SUM(G18:J22)</f>
+        <v>179.85</v>
+      </c>
+      <c r="L23" s="50">
+        <v>8</v>
+      </c>
+      <c r="M23" s="51"/>
+      <c r="N23" s="90"/>
+      <c r="O23" s="90"/>
+      <c r="P23" s="52"/>
+      <c r="Q23" s="50"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L24" s="50">
+        <v>9</v>
+      </c>
+      <c r="M24" s="51"/>
+      <c r="N24" s="90"/>
+      <c r="O24" s="90"/>
+      <c r="P24" s="52"/>
+      <c r="Q24" s="50"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D25" s="34"/>
+      <c r="L25" s="50">
+        <v>10</v>
+      </c>
+      <c r="M25" s="51"/>
+      <c r="N25" s="90"/>
+      <c r="O25" s="90"/>
+      <c r="P25" s="52"/>
+      <c r="Q25" s="50"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D26" s="34"/>
+      <c r="L26" s="50">
+        <v>10</v>
+      </c>
+      <c r="M26" s="51"/>
+      <c r="N26" s="90"/>
+      <c r="O26" s="90"/>
+      <c r="P26" s="52"/>
+      <c r="Q26" s="50"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L27" s="50">
+        <v>11</v>
+      </c>
+      <c r="M27" s="51"/>
+      <c r="N27" s="90"/>
+      <c r="O27" s="90"/>
+      <c r="P27" s="52"/>
+      <c r="Q27" s="50"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L28" s="50">
+        <v>11</v>
+      </c>
+      <c r="M28" s="51"/>
+      <c r="N28" s="90"/>
+      <c r="O28" s="90"/>
+      <c r="P28" s="52"/>
+      <c r="Q28" s="50"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L29" s="50">
+        <v>12</v>
+      </c>
+      <c r="M29" s="51"/>
+      <c r="N29" s="90"/>
+      <c r="O29" s="90"/>
+      <c r="P29" s="52"/>
+      <c r="Q29" s="50"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L30" s="50">
+        <v>13</v>
+      </c>
+      <c r="M30" s="51"/>
+      <c r="N30" s="90"/>
+      <c r="O30" s="90"/>
+      <c r="P30" s="52"/>
+      <c r="Q30" s="50"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L31" s="50">
+        <v>14</v>
+      </c>
+      <c r="M31" s="51"/>
+      <c r="N31" s="90"/>
+      <c r="O31" s="90"/>
+      <c r="P31" s="52"/>
+      <c r="Q31" s="50"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L32" s="50">
+        <v>15</v>
+      </c>
+      <c r="M32" s="51"/>
+      <c r="N32" s="90"/>
+      <c r="O32" s="90"/>
+      <c r="P32" s="52"/>
+      <c r="Q32" s="50"/>
+    </row>
+    <row r="33" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L33" s="50">
+        <v>16</v>
+      </c>
+      <c r="M33" s="51"/>
+      <c r="N33" s="90"/>
+      <c r="O33" s="90"/>
+      <c r="P33" s="52"/>
+      <c r="Q33" s="50"/>
+    </row>
+    <row r="34" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L34" s="50">
+        <v>17</v>
+      </c>
+      <c r="M34" s="51"/>
+      <c r="N34" s="90"/>
+      <c r="O34" s="90"/>
+      <c r="P34" s="52"/>
+      <c r="Q34" s="50"/>
+    </row>
+    <row r="35" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L35" s="50">
+        <v>18</v>
+      </c>
+      <c r="M35" s="51"/>
+      <c r="N35" s="90"/>
+      <c r="O35" s="90"/>
+      <c r="P35" s="52"/>
+      <c r="Q35" s="50"/>
+    </row>
+    <row r="36" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L36" s="50">
+        <v>19</v>
+      </c>
+      <c r="M36" s="51"/>
+      <c r="N36" s="90"/>
+      <c r="O36" s="90"/>
+      <c r="P36" s="52"/>
+      <c r="Q36" s="50"/>
+    </row>
+    <row r="37" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L37" s="50">
+        <v>20</v>
+      </c>
+      <c r="M37" s="51"/>
+      <c r="N37" s="90"/>
+      <c r="O37" s="90"/>
+      <c r="P37" s="52"/>
+      <c r="Q37" s="50"/>
+    </row>
+    <row r="38" spans="12:17" x14ac:dyDescent="0.2">
+      <c r="L38" s="50">
+        <v>21</v>
+      </c>
+      <c r="M38" s="51"/>
+      <c r="N38" s="90"/>
+      <c r="O38" s="90"/>
+      <c r="P38" s="52"/>
+      <c r="Q38" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="L14:Q14"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>